<commit_message>
Day panel clean zooming scrolling
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="87">
   <si>
     <t>Feature</t>
   </si>
@@ -279,6 +279,12 @@
   </si>
   <si>
     <t>Finish properties. Different types? There are tasks that can be completed and pushed, but there are immutables like holidays. Different dimension for holidays. Dimensions signify layers when drawn. Objs of diff dimensions can be simultaneous. Objs can filter by label even if label is in another dimension.</t>
+  </si>
+  <si>
+    <t>What is WCF and why should I care?</t>
+  </si>
+  <si>
+    <t>ADO.NET</t>
   </si>
 </sst>
 </file>
@@ -336,10 +342,10 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -434,18 +440,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:F45" totalsRowShown="0">
-  <autoFilter ref="A1:F45" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:F46" totalsRowShown="0">
+  <autoFilter ref="A1:F46" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
   <sortState ref="A2:F37">
     <sortCondition ref="D1:D37"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{9AABA1CB-4CFB-4C32-BB29-C2A627D5143C}" name="Needs"/>
     <tableColumn id="3" xr3:uid="{44037830-D1A7-4275-9E76-8E8A27CFA5FA}" name="Timeframe"/>
     <tableColumn id="4" xr3:uid="{BF9C91B9-D741-4386-8F98-4D819EB67396}" name="Priority"/>
     <tableColumn id="6" xr3:uid="{1FFE88A6-F499-42FB-A3F4-F5BDCD9D0CF0}" name="Done"/>
-    <tableColumn id="5" xr3:uid="{65384592-5F41-4A06-A57C-FE71C87B4BDD}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{65384592-5F41-4A06-A57C-FE71C87B4BDD}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -748,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -885,6 +891,9 @@
       <c r="A11" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
       <c r="F11" s="2" t="s">
         <v>73</v>
       </c>
@@ -1289,6 +1298,16 @@
       </c>
       <c r="F44" s="2" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DayView selecting, styles, some CalendarVM basics
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="94">
   <si>
     <t>Feature</t>
   </si>
@@ -41,9 +41,6 @@
     <t>VM only change tracking</t>
   </si>
   <si>
-    <t>Assessment</t>
-  </si>
-  <si>
     <t>Calendar views</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>better timespan picker</t>
   </si>
   <si>
-    <t>breakthrough</t>
-  </si>
-  <si>
     <t>task events</t>
   </si>
   <si>
@@ -119,33 +113,9 @@
     <t>Could be achieved by not putting CollectionView in edit mode when VM is in edit mode, but if view is editing when trying to commit, cancel view edit, then commit</t>
   </si>
   <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>6h</t>
-  </si>
-  <si>
-    <t>4h</t>
-  </si>
-  <si>
-    <t>30m</t>
-  </si>
-  <si>
     <t>Remote Desktop Tight VNC</t>
   </si>
   <si>
-    <t>1h</t>
-  </si>
-  <si>
-    <t>1d</t>
-  </si>
-  <si>
-    <t>2d</t>
-  </si>
-  <si>
-    <t>4 hours</t>
-  </si>
-  <si>
     <t>Clock</t>
   </si>
   <si>
@@ -179,9 +149,6 @@
     <t>Day panel max scale</t>
   </si>
   <si>
-    <t>3h</t>
-  </si>
-  <si>
     <t>week zooming</t>
   </si>
   <si>
@@ -248,15 +215,9 @@
     <t>An animated glowy rgb line that continuously updates to follow DateTime.Now. Animates smoothly over 1 second, updated once per second</t>
   </si>
   <si>
-    <t>week panel</t>
-  </si>
-  <si>
     <t>week view</t>
   </si>
   <si>
-    <t>Day horizontal, max scale weekk panel</t>
-  </si>
-  <si>
     <t>day panel</t>
   </si>
   <si>
@@ -284,10 +245,67 @@
     <t>What is WCF and why should I care?</t>
   </si>
   <si>
-    <t>ADO.NET</t>
-  </si>
-  <si>
     <t>Ruler teeth style</t>
+  </si>
+  <si>
+    <t>Day panel UI Virtualization</t>
+  </si>
+  <si>
+    <t>MainWindowVM -&gt; Navigate -&gt; GetDataCmd -&gt;</t>
+  </si>
+  <si>
+    <t>trigger states based on timertick event</t>
+  </si>
+  <si>
+    <t>click a CalendarObject</t>
+  </si>
+  <si>
+    <t>CalObj creates event. VM listens for event. Register even when creating in VM before adding to collection.</t>
+  </si>
+  <si>
+    <t>Selector</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>CalendarViewModel</t>
+  </si>
+  <si>
+    <t>DayViewModel</t>
+  </si>
+  <si>
+    <t>WeekViewModel</t>
+  </si>
+  <si>
+    <t>MonthViewModel</t>
+  </si>
+  <si>
+    <t>weekview</t>
+  </si>
+  <si>
+    <t>SCM issue tracking</t>
+  </si>
+  <si>
+    <t>Agile Scrum</t>
+  </si>
+  <si>
+    <t>CalendarObject thumbs</t>
+  </si>
+  <si>
+    <t>no need?</t>
+  </si>
+  <si>
+    <t>ListBox already does virtualization?</t>
+  </si>
+  <si>
+    <t>using ListBox</t>
+  </si>
+  <si>
+    <t>TextMargin bug after zoom + scroll</t>
+  </si>
+  <si>
+    <t>mistimed?</t>
   </si>
 </sst>
 </file>
@@ -457,10 +475,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:F47" totalsRowShown="0">
-  <autoFilter ref="A1:F47" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
-  <sortState ref="A2:F37">
-    <sortCondition ref="D1:D37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:F56" totalsRowShown="0">
+  <autoFilter ref="A1:F56" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+  <sortState ref="A2:F50">
+    <sortCondition ref="D1:D50"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="1"/>
@@ -771,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -788,7 +806,7 @@
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -802,535 +820,670 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="30">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30">
       <c r="A3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <v>1.1000000000000001</v>
       </c>
       <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6">
+        <f>SUM(C12:C32)</f>
+        <v>65</v>
+      </c>
+      <c r="I6">
+        <f>H6/11</f>
+        <v>5.9090909090909092</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7">
+        <f>SUM(C12:C47)</f>
+        <v>130</v>
+      </c>
+      <c r="I7">
+        <f>H7/11</f>
+        <v>11.818181818181818</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30">
+      <c r="A10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11">
+        <v>0.7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="5" customFormat="1" ht="30">
+      <c r="A14" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="3" t="s">
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="5" customFormat="1">
+      <c r="A15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15"/>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="5" customFormat="1">
+      <c r="A16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="I20" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10">
-        <v>0.7</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30">
-      <c r="A11" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="5" customFormat="1">
-      <c r="A12" s="4" t="s">
+    </row>
+    <row r="21" spans="1:10" ht="45">
+      <c r="A21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>11</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
         <v>16</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="5">
+      <c r="F26" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" ht="30">
-      <c r="A13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13">
-        <v>0.77</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14">
-        <v>0.8</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>18</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D15">
-        <v>0.85</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16">
-        <v>0.9</v>
-      </c>
-      <c r="I16" t="s">
-        <v>41</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="45">
-      <c r="A18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25">
-        <v>8</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" t="s">
-        <v>33</v>
+        <v>13</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
       </c>
       <c r="D29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>20</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31">
+      <c r="B32" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" t="s">
-        <v>33</v>
+      <c r="C32">
+        <v>4</v>
       </c>
       <c r="D32">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" t="s">
-        <v>32</v>
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
       </c>
       <c r="D33">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C34" t="s">
-        <v>31</v>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
       </c>
       <c r="D34">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30">
       <c r="A35" s="3" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="30">
+        <v>13</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>30</v>
+        <v>51</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="30">
+      <c r="A38" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" t="s">
-        <v>14</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>61</v>
+        <v>29</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="3" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30">
+        <v>24</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40">
+        <v>27</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="30">
+        <v>9</v>
+      </c>
+      <c r="C41">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>79</v>
+        <v>18</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>81</v>
+        <v>16</v>
+      </c>
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43">
+        <v>20</v>
+      </c>
+      <c r="D43">
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>31</v>
+      </c>
+      <c r="E44" t="s">
+        <v>89</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="30">
       <c r="A45" s="3" t="s">
-        <v>85</v>
+        <v>65</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>32</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="3" t="s">
-        <v>86</v>
+        <v>67</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>33</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="30">
+      <c r="A49" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="30">
+      <c r="A50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="3" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MonthView, calendar navigation from toolbar, button styles
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="106">
   <si>
     <t>Feature</t>
   </si>
@@ -149,18 +150,12 @@
     <t>Day panel max scale</t>
   </si>
   <si>
-    <t>week zooming</t>
-  </si>
-  <si>
     <t>Make max scale proportional to viewport, if scale less than viewport, scale to viewport, then expand to week view, IsMaxScale</t>
   </si>
   <si>
     <t>Day panel horizontal</t>
   </si>
   <si>
-    <t>With horizontal Days at max scale, scaling should already happen by just shrinking week grid, nothing to code</t>
-  </si>
-  <si>
     <t>Date watermark</t>
   </si>
   <si>
@@ -278,9 +273,6 @@
     <t>MonthViewModel</t>
   </si>
   <si>
-    <t>weekview</t>
-  </si>
-  <si>
     <t>SCM issue tracking</t>
   </si>
   <si>
@@ -299,12 +291,6 @@
     <t>using ListBox</t>
   </si>
   <si>
-    <t>TextMargin bug after zoom + scroll</t>
-  </si>
-  <si>
-    <t>mistimed?</t>
-  </si>
-  <si>
     <t>VerticalLRWeekView</t>
   </si>
   <si>
@@ -330,6 +316,33 @@
   </si>
   <si>
     <t>Vertical week, vertical days. This will just use a vertical ContinuousDay panel</t>
+  </si>
+  <si>
+    <t>Day not in month styles</t>
+  </si>
+  <si>
+    <t>flag, gray background, darker gray watermark, distinguishable from month days</t>
+  </si>
+  <si>
+    <t>Pages</t>
+  </si>
+  <si>
+    <t>in month view click on a week to page to week, click on a day to page to day</t>
+  </si>
+  <si>
+    <t>Double click week to WeekView</t>
+  </si>
+  <si>
+    <t>CalendarPicker</t>
+  </si>
+  <si>
+    <t>Swap Calendar Views</t>
+  </si>
+  <si>
+    <t>Figure out how to easily swap to month/week/day views</t>
+  </si>
+  <si>
+    <t>Use the DatePicker to choose a date</t>
   </si>
 </sst>
 </file>
@@ -521,10 +534,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:F60" totalsRowShown="0">
-  <autoFilter ref="A1:F60" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
-  <sortState ref="A2:F54">
-    <sortCondition ref="D1:D54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:F63" totalsRowShown="0">
+  <autoFilter ref="A1:F63" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+  <sortState ref="A2:F57">
+    <sortCondition ref="D1:D57"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="1"/>
@@ -835,15 +848,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -894,18 +907,18 @@
         <v>37</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
         <v>37</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -924,33 +937,33 @@
         <v>37</v>
       </c>
       <c r="H6">
-        <f>SUM(C12:C34)</f>
-        <v>65</v>
+        <f>SUM(C12:C37)</f>
+        <v>64</v>
       </c>
       <c r="I6">
         <f>H6/11</f>
-        <v>5.9090909090909092</v>
+        <v>5.8181818181818183</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
         <v>37</v>
       </c>
       <c r="H7">
-        <f>SUM(C12:C52)</f>
-        <v>130</v>
+        <f>SUM(C12:C55)</f>
+        <v>129</v>
       </c>
       <c r="I7">
         <f>H7/11</f>
-        <v>11.818181818181818</v>
+        <v>11.727272727272727</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
         <v>37</v>
@@ -958,7 +971,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
         <v>37</v>
@@ -966,18 +979,18 @@
     </row>
     <row r="10" spans="1:9" ht="30">
       <c r="A10" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
         <v>37</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D11">
         <v>0.7</v>
@@ -986,176 +999,174 @@
         <v>37</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30">
+      <c r="A12" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
+      <c r="B12" t="s">
+        <v>62</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="5" customFormat="1">
       <c r="A13" s="3" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" s="5" customFormat="1" ht="30">
+        <v>57</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="5" customFormat="1">
       <c r="A14" s="3" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="C14"/>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14"/>
+      <c r="D14"/>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
       <c r="F14" s="2" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="5" customFormat="1">
       <c r="A15" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
+        <v>38</v>
+      </c>
+      <c r="B15"/>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
       <c r="F15" s="2" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="5" customFormat="1">
       <c r="A16" s="3" t="s">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16" s="2" t="s">
-        <v>97</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:10" s="5" customFormat="1">
       <c r="A17" s="3" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="B17"/>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17">
-        <v>5</v>
-      </c>
-      <c r="E17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
       <c r="F17" s="2" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="5" customFormat="1">
       <c r="A18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" t="s">
-        <v>84</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B18"/>
       <c r="C18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>6</v>
-      </c>
-      <c r="E18"/>
-      <c r="F18" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="5" customFormat="1">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19"/>
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19">
-        <v>7</v>
-      </c>
-      <c r="E19"/>
-      <c r="F19" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21">
-        <v>9</v>
+        <v>103</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="3" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
       <c r="D22">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="3" t="s">
-        <v>36</v>
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>78</v>
       </c>
       <c r="C23">
         <v>3</v>
       </c>
       <c r="D23">
-        <v>11</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="I23" t="s">
         <v>31</v>
@@ -1166,440 +1177,479 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>22</v>
+        <v>80</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
       </c>
       <c r="D24">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
+        <v>81</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
       </c>
       <c r="D25">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="45">
       <c r="A26" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C26">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D26">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27">
         <v>12</v>
       </c>
-      <c r="B27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27">
-        <v>6</v>
-      </c>
-      <c r="D27">
-        <v>15</v>
+      <c r="E27" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
       </c>
       <c r="D28">
-        <v>16</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="3" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D29">
-        <v>17</v>
-      </c>
-      <c r="E29" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
         <v>13</v>
-      </c>
-      <c r="B30" t="s">
-        <v>6</v>
       </c>
       <c r="C30">
         <v>6</v>
       </c>
       <c r="D30">
-        <v>18</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="C31">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D31">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="3" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>37</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D33">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
         <v>13</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D34">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D35">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C36">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D36">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="30">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="3" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
         <v>13</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>50</v>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="3" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>13</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30">
+      <c r="A40" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" t="s">
         <v>13</v>
       </c>
-      <c r="C39">
-        <v>4</v>
-      </c>
-      <c r="D39">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="6"/>
+      <c r="F40" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>26</v>
+        <v>49</v>
+      </c>
+      <c r="B41" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C42">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D42">
-        <v>27</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43">
-        <v>6</v>
-      </c>
-      <c r="D43">
-        <v>28</v>
-      </c>
+      <c r="A43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="6"/>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>27</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46">
+        <v>6</v>
+      </c>
+      <c r="D46">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B48" t="s">
         <v>25</v>
       </c>
-      <c r="C45">
+      <c r="C48">
         <v>20</v>
       </c>
-      <c r="D45">
+      <c r="D48">
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8">
+    <row r="49" spans="1:6">
+      <c r="A49" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8">
         <v>4</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D49" s="8">
         <v>31</v>
       </c>
-      <c r="E46" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="30">
-      <c r="A47" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D47">
-        <v>31.1</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11">
-        <v>31.2</v>
-      </c>
-      <c r="E48" s="11"/>
-      <c r="F48" s="12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11">
-        <v>31.3</v>
-      </c>
-      <c r="E49" s="11"/>
-      <c r="F49" s="12" t="s">
-        <v>101</v>
+      <c r="E49" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="30">
       <c r="A50" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50">
+        <v>31.1</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11">
+        <v>31.2</v>
+      </c>
+      <c r="E51" s="11"/>
+      <c r="F51" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11">
+        <v>31.3</v>
+      </c>
+      <c r="E52" s="11"/>
+      <c r="F52" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="30">
+      <c r="A53" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>32</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B50" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="D50">
-        <v>32</v>
-      </c>
-      <c r="F50" s="2" t="s">
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <v>33</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C51">
-        <v>4</v>
-      </c>
-      <c r="D51">
-        <v>33</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C52">
-        <v>4</v>
-      </c>
-      <c r="D52">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="30">
-      <c r="A54" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55">
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+        <v>30</v>
+      </c>
+      <c r="E56" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="30">
       <c r="A57" s="3" t="s">
-        <v>85</v>
+        <v>4</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="3" t="s">
-        <v>86</v>
+        <v>67</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="3" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Colored TaskTypes and trying to get note boxes
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="121">
   <si>
     <t>Feature</t>
   </si>
@@ -375,6 +375,18 @@
   </si>
   <si>
     <t>Draw notes with a little note graphic on the right side of a day</t>
+  </si>
+  <si>
+    <t>New Note Here</t>
+  </si>
+  <si>
+    <t>Set time to where cursor is on day/week panel</t>
+  </si>
+  <si>
+    <t>CalendarVM works like NotesVM</t>
+  </si>
+  <si>
+    <t>Legend</t>
   </si>
 </sst>
 </file>
@@ -566,8 +578,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:F70" totalsRowShown="0">
-  <autoFilter ref="A1:F70" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:F73" totalsRowShown="0">
+  <autoFilter ref="A1:F73" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
   <sortState ref="A2:F61">
     <sortCondition ref="D1:D61"/>
   </sortState>
@@ -880,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1752,6 +1764,24 @@
         <v>113</v>
       </c>
     </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed validation lists, focus textbox on edit
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="137">
   <si>
     <t>Feature</t>
   </si>
@@ -424,6 +424,18 @@
   </si>
   <si>
     <t>save image and txt</t>
+  </si>
+  <si>
+    <t>edit labels from pattern editor</t>
+  </si>
+  <si>
+    <t>label editor popup from pattern editor popup</t>
+  </si>
+  <si>
+    <t>edit patterns from task editor</t>
+  </si>
+  <si>
+    <t>pattern editor popup from task editor popup</t>
   </si>
 </sst>
 </file>
@@ -493,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -518,6 +530,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -624,10 +642,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:F78" totalsRowShown="0">
-  <autoFilter ref="A1:F78" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
-  <sortState ref="A2:F61">
-    <sortCondition ref="D1:D61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:F80" totalsRowShown="0">
+  <autoFilter ref="A1:F80" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+  <sortState ref="A2:F63">
+    <sortCondition ref="D1:D63"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="1"/>
@@ -938,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1029,7 +1047,7 @@
         <v>37</v>
       </c>
       <c r="H6" s="3">
-        <f>SUM(C12:C41)</f>
+        <f>SUM(C12:C43)</f>
         <v>64</v>
       </c>
       <c r="I6" s="3">
@@ -1045,7 +1063,7 @@
         <v>37</v>
       </c>
       <c r="H7" s="3">
-        <f>SUM(C12:C59)</f>
+        <f>SUM(C12:C61)</f>
         <v>129</v>
       </c>
       <c r="I7" s="3">
@@ -1355,72 +1373,57 @@
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="2" t="s">
-        <v>112</v>
+      <c r="A30" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="3">
-        <v>13</v>
+      <c r="A31" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="3">
-        <v>6</v>
-      </c>
-      <c r="D32" s="3">
-        <v>18</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="3">
         <v>13</v>
-      </c>
-      <c r="C33" s="3">
-        <v>6</v>
-      </c>
-      <c r="D33" s="3">
-        <v>19</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2" t="s">
-        <v>75</v>
+        <v>13</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="C34" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D34" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>13</v>
@@ -1429,439 +1432,470 @@
         <v>6</v>
       </c>
       <c r="D35" s="3">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" s="3">
         <v>3</v>
       </c>
       <c r="D36" s="3">
-        <v>17</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>107</v>
+        <v>12</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="3">
+        <v>6</v>
+      </c>
+      <c r="D37" s="3">
+        <v>15</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>115</v>
+        <v>77</v>
+      </c>
+      <c r="C38" s="3">
+        <v>3</v>
+      </c>
+      <c r="D38" s="3">
+        <v>17</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" s="3">
-        <v>2</v>
-      </c>
-      <c r="D39" s="3">
-        <v>20</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="3">
-        <v>4</v>
-      </c>
-      <c r="D40" s="3">
-        <v>21</v>
+        <v>114</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C41" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D41" s="3">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C42" s="3">
         <v>4</v>
       </c>
       <c r="D42" s="3">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="3">
+        <v>4</v>
+      </c>
+      <c r="D43" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C43" s="3">
-        <v>6</v>
-      </c>
-      <c r="D43" s="3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="30">
-      <c r="A44" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>48</v>
+      <c r="C44" s="3">
+        <v>4</v>
+      </c>
+      <c r="D44" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>14</v>
+      </c>
+      <c r="C45" s="3">
+        <v>6</v>
+      </c>
+      <c r="D45" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="30">
       <c r="A46" s="2" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="3">
-        <v>4</v>
-      </c>
-      <c r="D46" s="3">
-        <v>25</v>
+      <c r="F46" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F47" s="8"/>
+      <c r="A47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C48" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D48" s="3">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C49" s="3">
-        <v>10</v>
-      </c>
-      <c r="D49" s="3">
-        <v>27</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>73</v>
-      </c>
+      <c r="A49" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F49" s="8"/>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C50" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D50" s="3">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C51" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D51" s="3">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="3">
+        <v>6</v>
+      </c>
+      <c r="D52" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" s="3">
+        <v>1</v>
+      </c>
+      <c r="D53" s="3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C54" s="3">
         <v>20</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D54" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="9" t="s">
+    <row r="55" spans="1:6">
+      <c r="A55" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10">
+      <c r="B55" s="10"/>
+      <c r="C55" s="10">
         <v>4</v>
       </c>
-      <c r="D53" s="10">
+      <c r="D55" s="10">
         <v>31</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E55" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F53" s="11" t="s">
+      <c r="F55" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="30">
-      <c r="A54" s="2" t="s">
+    <row r="56" spans="1:6" ht="30">
+      <c r="A56" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D56" s="3">
         <v>31.1</v>
       </c>
-      <c r="F54" s="4" t="s">
+      <c r="F56" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="2" t="s">
+    <row r="57" spans="1:6">
+      <c r="A57" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D55" s="3">
-        <v>31.2</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D56" s="3">
-        <v>31.3</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="30">
-      <c r="A57" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C57" s="3">
-        <v>1</v>
-      </c>
       <c r="D57" s="3">
-        <v>32</v>
+        <v>31.2</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C58" s="3">
-        <v>4</v>
+        <v>95</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="D58" s="3">
-        <v>33</v>
+        <v>31.3</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="30">
       <c r="A59" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="C59" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D59" s="3">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="30">
+        <v>65</v>
+      </c>
+      <c r="C60" s="3">
+        <v>4</v>
+      </c>
+      <c r="D60" s="3">
+        <v>33</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61" s="3">
         <v>4</v>
       </c>
-      <c r="F61" s="4" t="s">
-        <v>28</v>
+      <c r="D61" s="3">
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+        <v>30</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="30">
       <c r="A63" s="2" t="s">
-        <v>70</v>
+        <v>4</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2" t="s">
-        <v>82</v>
+        <v>67</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F71" s="4" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F76" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F78" s="4" t="s">
+      <c r="F80" s="4" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Redesigned TimeKeeperDAL. Filter. Filterable.
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="128">
   <si>
     <t>Feature</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>Note graphic</t>
+  </si>
+  <si>
+    <t>Auto Assign names to new notes</t>
   </si>
 </sst>
 </file>
@@ -515,6 +518,12 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -559,12 +568,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -601,9 +604,9 @@
       <tableStyleElement type="firstRowStripe" size="2"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="3" xr9:uid="{A53ADC7C-9332-4916-9ACB-0EFC07D28AC6}">
-      <tableStyleElement type="wholeTable" dxfId="3"/>
-      <tableStyleElement type="headerRow" dxfId="2"/>
-      <tableStyleElement type="secondRowStripe" dxfId="1"/>
+      <tableStyleElement type="wholeTable" dxfId="5"/>
+      <tableStyleElement type="headerRow" dxfId="4"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -625,16 +628,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D83" totalsRowShown="0">
-  <autoFilter ref="A1:D83" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D84" totalsRowShown="0">
+  <autoFilter ref="A1:D84" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
   <sortState ref="A2:D65">
     <sortCondition ref="B1:B65"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{BF9C91B9-D741-4386-8F98-4D819EB67396}" name="Priority"/>
     <tableColumn id="6" xr3:uid="{1FFE88A6-F499-42FB-A3F4-F5BDCD9D0CF0}" name="Done"/>
-    <tableColumn id="5" xr3:uid="{65384592-5F41-4A06-A57C-FE71C87B4BDD}" name="Notes" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{65384592-5F41-4A06-A57C-FE71C87B4BDD}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -937,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:H10"/>
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -976,7 +979,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -1060,7 +1063,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>48</v>
       </c>
@@ -1741,9 +1744,14 @@
         <v>110</v>
       </c>
     </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
more redesign of DAL
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="131">
   <si>
     <t>Feature</t>
   </si>
@@ -409,6 +409,15 @@
   </si>
   <si>
     <t>Auto Assign names to new notes</t>
+  </si>
+  <si>
+    <t>Should a Resource be a Filterable?</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Because I made Allocation.TimeTask nullable, if I make a Task, give it an Allocation, then delete the Task, will the Allocation remain?</t>
   </si>
 </sst>
 </file>
@@ -628,8 +637,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D84" totalsRowShown="0">
-  <autoFilter ref="A1:D84" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D86" totalsRowShown="0">
+  <autoFilter ref="A1:D86" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
   <sortState ref="A2:D65">
     <sortCondition ref="B1:B65"/>
   </sortState>
@@ -940,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1747,6 +1756,19 @@
     <row r="84" spans="1:4">
       <c r="A84" s="12" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D86" s="13" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filterables, Filters, working DAL
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="137">
   <si>
     <t>Feature</t>
   </si>
@@ -436,21 +436,6 @@
   </si>
   <si>
     <t>like TPClause view</t>
-  </si>
-  <si>
-    <t>maybe I need to separate everything from Filterables table into their own tables? Maybe I didn't setup filter delete correctly?</t>
-  </si>
-  <si>
-    <t>There was a problem updating the database: Database Update Failed</t>
-  </si>
-  <si>
-    <t>An error occurred while saving entities that do not expose foreign key properties for their relationships. The EntityEntries property will return null because a single entity cannot be identified as the source of the exception. Handling of exceptions while saving can be made easier by exposing foreign key properties in your entity types. See the InnerException for details.</t>
-  </si>
-  <si>
-    <t>A relationship from the 'TimeTaskFilter_TimeTask' AssociationSet is in the 'Deleted' state. Given multiplicity constraints, a corresponding 'TimeTaskFilter_TimeTask_Source' must also in the 'Deleted' state.</t>
-  </si>
-  <si>
-    <t>some kind of error when removing filters</t>
   </si>
 </sst>
 </file>
@@ -670,8 +655,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D93" totalsRowShown="0">
-  <autoFilter ref="A1:D93" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D91" totalsRowShown="0">
+  <autoFilter ref="A1:D91" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
   <sortState ref="A2:D71">
     <sortCondition ref="B1:B71"/>
   </sortState>
@@ -982,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1758,7 +1743,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:4">
       <c r="A81" s="12" t="s">
         <v>118</v>
       </c>
@@ -1766,7 +1751,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
         <v>69</v>
       </c>
@@ -1774,7 +1759,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
         <v>70</v>
       </c>
@@ -1782,7 +1767,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:4" ht="30">
       <c r="A84" s="9" t="s">
         <v>43</v>
       </c>
@@ -1792,7 +1777,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="30">
+    <row r="85" spans="1:4" ht="30">
       <c r="A85" s="9" t="s">
         <v>52</v>
       </c>
@@ -1802,7 +1787,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="10" customFormat="1">
+    <row r="86" spans="1:4" s="10" customFormat="1">
       <c r="A86" s="9" t="s">
         <v>18</v>
       </c>
@@ -1810,7 +1795,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:4">
       <c r="A87" s="9" t="s">
         <v>21</v>
       </c>
@@ -1818,7 +1803,7 @@
       <c r="C87" s="10"/>
       <c r="D87" s="11"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:4">
       <c r="A88" s="9" t="s">
         <v>108</v>
       </c>
@@ -1828,7 +1813,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:4">
       <c r="A89" s="9" t="s">
         <v>109</v>
       </c>
@@ -1838,7 +1823,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:4">
       <c r="A90" s="12" t="s">
         <v>127</v>
       </c>
@@ -1846,37 +1831,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:4">
       <c r="A91" s="12" t="s">
         <v>133</v>
       </c>
       <c r="D91" s="13" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
-      <c r="A92" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="D92" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
-      <c r="A93" s="12"/>
-      <c r="D93" s="13"/>
-    </row>
-    <row r="94" spans="1:5">
-      <c r="E94" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
-      <c r="E96" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TimeTasksView finally completed up and running with no errors as far as I can tell. *single clap* OKAY now lets get to the good
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="139">
   <si>
     <t>Feature</t>
   </si>
@@ -303,9 +303,6 @@
     <t>Implmnt TimeTasks on Calendar</t>
   </si>
   <si>
-    <t>Color by type/state</t>
-  </si>
-  <si>
     <t>Draw notes with a little note graphic on the right side of a day</t>
   </si>
   <si>
@@ -384,12 +381,6 @@
     <t>WCF</t>
   </si>
   <si>
-    <t>Include/Exclude Labels</t>
-  </si>
-  <si>
-    <t>Should Tasks have labels?</t>
-  </si>
-  <si>
     <t>More theme colors</t>
   </si>
   <si>
@@ -436,6 +427,21 @@
   </si>
   <si>
     <t>like TPClause view</t>
+  </si>
+  <si>
+    <t>Create CalObjs from TimeTask data</t>
+  </si>
+  <si>
+    <t>detect range, build cal objs inside areas specified by filters</t>
+  </si>
+  <si>
+    <t>bug</t>
+  </si>
+  <si>
+    <t>reproduce: select a task. Hit refresh. After refresh, can still press edit. If press edit, it opens weird old task? Should clear selected task and not allow press of edit when refresh is pressed until new task selected</t>
+  </si>
+  <si>
+    <t>toggle Color by type/state</t>
   </si>
 </sst>
 </file>
@@ -655,10 +661,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D91" totalsRowShown="0">
-  <autoFilter ref="A1:D91" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
-  <sortState ref="A2:D71">
-    <sortCondition ref="B1:B71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D90" totalsRowShown="0">
+  <autoFilter ref="A1:D90" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+  <sortState ref="A2:D70">
+    <sortCondition ref="B1:B70"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="2"/>
@@ -967,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:H91"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1322,7 +1328,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>29</v>
@@ -1330,7 +1336,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>29</v>
@@ -1338,470 +1344,483 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="14" customFormat="1">
+      <c r="A38" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B38" s="10">
+      <c r="B38" s="14">
         <v>0.1</v>
       </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="11"/>
+      <c r="C38" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="13"/>
     </row>
     <row r="39" spans="1:4" s="14" customFormat="1">
       <c r="A39" s="12" t="s">
-        <v>135</v>
+        <v>132</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="12"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="11"/>
+      <c r="A40" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B41" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="C41" s="14"/>
+        <v>0.3</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B42" s="3">
-        <v>0.3</v>
+        <v>134</v>
       </c>
       <c r="C42" s="14"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B43" s="3">
-        <v>1</v>
+      <c r="D42" s="13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30">
+      <c r="A43" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="13" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B45" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="10" customFormat="1">
-      <c r="A45" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B45" s="10">
-        <v>3</v>
-      </c>
-      <c r="D45" s="11"/>
-    </row>
-    <row r="46" spans="1:4" s="10" customFormat="1">
-      <c r="A46" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B46" s="10">
-        <v>4</v>
-      </c>
-      <c r="D46" s="11"/>
+    <row r="46" spans="1:4">
+      <c r="A46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="3">
+        <v>5</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="2" t="s">
-        <v>10</v>
+      <c r="A47" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="B47" s="3">
-        <v>5</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="B48" s="3">
-        <v>6</v>
+        <v>6.5</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>9</v>
+        <v>94</v>
       </c>
       <c r="B49" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="B50" s="3">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="B51" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="B52" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="2" t="s">
-        <v>102</v>
+      <c r="A53" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="B53" s="3">
-        <v>10</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>103</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="12" t="s">
-        <v>123</v>
+      <c r="A54" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="B54" s="3">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="B55" s="3">
-        <v>13</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B56" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B57" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>13</v>
+        <v>95</v>
       </c>
       <c r="B58" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="B59" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B60" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="B61" s="3">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="2" t="s">
-        <v>56</v>
+      <c r="A62" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="B62" s="3">
-        <v>20</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>57</v>
+        <v>21</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="12" t="s">
-        <v>116</v>
+      <c r="A63" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B63" s="3">
-        <v>21</v>
-      </c>
-      <c r="D63" s="13" t="s">
-        <v>117</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="2" t="s">
-        <v>16</v>
+      <c r="A64" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="B64" s="3">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="12" t="s">
-        <v>126</v>
+      <c r="A65" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B65" s="3">
-        <v>23</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B66" s="3">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="B67" s="3">
-        <v>25</v>
-      </c>
-      <c r="D67" s="13" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="2" t="s">
-        <v>6</v>
+      <c r="A68" s="12" t="s">
+        <v>118</v>
       </c>
       <c r="B68" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B69" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="12" t="s">
-        <v>122</v>
+      <c r="A70" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="B70" s="3">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B71" s="3">
-        <v>29</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B72" s="3">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="B73" s="3">
-        <v>31</v>
-      </c>
-      <c r="D73" s="13" t="s">
-        <v>125</v>
+        <v>32</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B74" s="3">
-        <v>32</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>86</v>
+        <v>33</v>
+      </c>
+      <c r="D74" s="13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B75" s="3">
-        <v>33</v>
-      </c>
-      <c r="D75" s="13" t="s">
-        <v>124</v>
+        <v>34</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B76" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="2" t="s">
-        <v>104</v>
+      <c r="A77" s="12" t="s">
+        <v>113</v>
       </c>
       <c r="B77" s="3">
-        <v>35</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>105</v>
+        <v>36</v>
+      </c>
+      <c r="D77" s="13" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="12" t="s">
-        <v>114</v>
+      <c r="A78" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="B78" s="3">
-        <v>36</v>
-      </c>
-      <c r="D78" s="13" t="s">
-        <v>115</v>
+        <v>37</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B79" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="2" t="s">
-        <v>79</v>
+      <c r="A80" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="B80" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="12" t="s">
-        <v>118</v>
+      <c r="A81" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="B81" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B82" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B83" s="3">
         <v>41</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="30">
+      <c r="A83" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="30">
       <c r="A84" s="9" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
       <c r="D84" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="30">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" s="10" customFormat="1">
       <c r="A85" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B85" s="10"/>
-      <c r="C85" s="10"/>
+        <v>18</v>
+      </c>
       <c r="D85" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" s="10" customFormat="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D86" s="11" t="s">
-        <v>42</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B86" s="10"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="11"/>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="9" t="s">
-        <v>21</v>
+        <v>107</v>
       </c>
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
-      <c r="D87" s="11"/>
+      <c r="D87" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="9" t="s">
@@ -1810,33 +1829,23 @@
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
       <c r="D88" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B89" s="10"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="11" t="s">
-        <v>110</v>
+      <c r="A89" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D89" s="13" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="12" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D90" s="13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D91" s="13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1868,17 +1877,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
. working on CreateEventObjectsFromTimeTasks
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="150">
   <si>
     <t>Feature</t>
   </si>
@@ -438,9 +438,6 @@
     <t>bug</t>
   </si>
   <si>
-    <t>reproduce: select a task. Hit refresh. After refresh, can still press edit. If press edit, it opens weird old task? Should clear selected task and not allow press of edit when refresh is pressed until new task selected</t>
-  </si>
-  <si>
     <t>toggle Color by type/state</t>
   </si>
   <si>
@@ -451,6 +448,33 @@
   </si>
   <si>
     <t>create an API that exposes functions that allow an external program to interact with resource consumption/acquisition</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>TimeTasks need to be created entirely, not just by the current calendar view because the resources it allocates may be consumed differently outside of the view because of collisions or filters</t>
+  </si>
+  <si>
+    <t>SPOOKY LANGOLIERS. reproduce: select a task. Hit refresh. After refresh, can still press edit. If press edit, it opens weird old task? Should clear selected task and not allow press of edit when refresh is pressed until new task selected</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>In EF is there a way to prevent the modification of certain entities?</t>
+  </si>
+  <si>
+    <t>Enforce only one time allocation</t>
+  </si>
+  <si>
+    <t>Validation? Disable add command</t>
+  </si>
+  <si>
+    <t>requires at least one allocation to be enabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TimeTask Eager/Even/Apathetic </t>
   </si>
 </sst>
 </file>
@@ -670,10 +694,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D92" totalsRowShown="0">
-  <autoFilter ref="A1:D92" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
-  <sortState ref="A2:D70">
-    <sortCondition ref="B1:B70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D96" totalsRowShown="0">
+  <autoFilter ref="A1:D96" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+  <sortState ref="A2:D73">
+    <sortCondition ref="B1:B73"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="2"/>
@@ -982,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:H92"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1404,470 +1428,505 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" ht="30">
       <c r="A42" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="13" t="s">
+      <c r="C45" s="14"/>
+      <c r="D45" s="13" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30">
-      <c r="A43" s="12" t="s">
+    <row r="46" spans="1:4" ht="30">
+      <c r="A46" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="2" t="s">
+      <c r="C46" s="14"/>
+      <c r="D46" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B47" s="3">
         <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B46" s="3">
-        <v>5</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="B47" s="3">
-        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B48" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>90</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>94</v>
+        <v>10</v>
       </c>
       <c r="B49" s="3">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="2" t="s">
-        <v>17</v>
+      <c r="A50" s="12" t="s">
+        <v>137</v>
       </c>
       <c r="B50" s="3">
-        <v>8</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="B51" s="3">
-        <v>9</v>
+        <v>6.5</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B52" s="3">
-        <v>10</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>102</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="12" t="s">
-        <v>120</v>
+      <c r="A53" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B53" s="3">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
-        <v>105</v>
+        <v>62</v>
       </c>
       <c r="B54" s="3">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="B55" s="3">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="2" t="s">
-        <v>8</v>
+      <c r="A56" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="B56" s="3">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B57" s="3">
         <v>13</v>
       </c>
-      <c r="B57" s="3">
-        <v>16</v>
+      <c r="D57" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="B58" s="3">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B59" s="3">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B60" s="3">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="B61" s="3">
-        <v>20</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="12" t="s">
-        <v>115</v>
+      <c r="A62" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B62" s="3">
-        <v>21</v>
-      </c>
-      <c r="D62" s="13" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B63" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="12" t="s">
-        <v>123</v>
+      <c r="A64" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B64" s="3">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="2" t="s">
-        <v>41</v>
+      <c r="A65" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="B65" s="3">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B67" s="3">
+        <v>23</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B69" s="3">
         <v>25</v>
       </c>
-      <c r="D66" s="13" t="s">
+      <c r="D69" s="13" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" s="3">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B68" s="3">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B69" s="3">
-        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="B70" s="3">
-        <v>29</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="2" t="s">
-        <v>59</v>
+      <c r="A71" s="12" t="s">
+        <v>118</v>
       </c>
       <c r="B71" s="3">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="2" t="s">
-        <v>71</v>
+      <c r="A72" s="12" t="s">
+        <v>119</v>
       </c>
       <c r="B72" s="3">
-        <v>31</v>
-      </c>
-      <c r="D72" s="13" t="s">
-        <v>122</v>
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="B73" s="3">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="B74" s="3">
-        <v>33</v>
-      </c>
-      <c r="D74" s="13" t="s">
-        <v>121</v>
+        <v>30</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="B75" s="3">
-        <v>34</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>100</v>
+        <v>31</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B76" s="3">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="12" t="s">
-        <v>113</v>
+      <c r="A77" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="B77" s="3">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B78" s="3">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="B79" s="3">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B80" s="3">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="D80" s="13" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="B81" s="3">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B83" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B84" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B82" s="3">
+      <c r="B85" s="3">
         <v>41</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="30">
-      <c r="A83" s="9" t="s">
+    <row r="86" spans="1:4" s="10" customFormat="1" ht="30">
+      <c r="A86" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B83" s="10"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="11" t="s">
+      <c r="D86" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="30">
-      <c r="A84" s="9" t="s">
+    <row r="87" spans="1:4" ht="30">
+      <c r="A87" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" s="10" customFormat="1">
-      <c r="A85" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="11"/>
-    </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
       <c r="D87" s="11" t="s">
-        <v>110</v>
+        <v>53</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="9" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
       <c r="D88" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="11"/>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B91" s="10"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="11" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D89" s="13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="D90" s="13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="12" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D92" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D93" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D95" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="D92" s="13" t="s">
-        <v>141</v>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D96" s="13" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
default resource, tasktypes, locked
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="169">
   <si>
     <t>Feature</t>
   </si>
@@ -462,9 +462,6 @@
     <t>Question</t>
   </si>
   <si>
-    <t>In EF is there a way to prevent the modification of certain entities?</t>
-  </si>
-  <si>
     <t>Enforce only one time allocation</t>
   </si>
   <si>
@@ -496,6 +493,45 @@
   </si>
   <si>
     <t>time pattern where clauses are not saving/retrieving the correct equivalency</t>
+  </si>
+  <si>
+    <t>Time Resources UI stuff</t>
+  </si>
+  <si>
+    <t>color Time resources differently (V). Don't allow time resources to be modified (VM).</t>
+  </si>
+  <si>
+    <t>Add lots of stuff to seed method</t>
+  </si>
+  <si>
+    <t>Holiday patterns, more labels, task types, time resources, other resources</t>
+  </si>
+  <si>
+    <t>If I can make it so time resources are distinctly different than other resources, couldn't I do the same for TaskTypes? Is there any reason that TaskTypes must be a separate entity from Labels? It's not bad that they are. I don't want other labels in the tasktype list and I don't want tasktypes in the labels list, so theres no point in making them labels.</t>
+  </si>
+  <si>
+    <t>Data Analysis of Resource allocations/ consumption</t>
+  </si>
+  <si>
+    <t>Let me select a set of labeledentities and let me add a certain label to all of them with one click. At the same time, show me a list of all common labels amoung them and let me delete each.</t>
+  </si>
+  <si>
+    <t>better editors regarding labels</t>
+  </si>
+  <si>
+    <t>Show me all of the entities that are labeled with a certain label</t>
+  </si>
+  <si>
+    <t>LabeledEntitiesView</t>
+  </si>
+  <si>
+    <t>Loading scalability</t>
+  </si>
+  <si>
+    <t>Instead of loading everything and blocking, load only enough to fit the screen, load in the background, allow me to use the program even while it is loading rows.</t>
+  </si>
+  <si>
+    <t>In EF is there a way to prevent the modification of certain entities? No just do it from VM</t>
   </si>
 </sst>
 </file>
@@ -724,10 +760,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D101" totalsRowShown="0">
-  <autoFilter ref="A1:D101" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
-  <sortState ref="A2:D78">
-    <sortCondition ref="B1:B78"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D107" totalsRowShown="0">
+  <autoFilter ref="A1:D107" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+  <sortState ref="A2:D83">
+    <sortCondition ref="B1:B83"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="2"/>
@@ -1036,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1495,508 +1531,602 @@
     </row>
     <row r="46" spans="1:4" s="14" customFormat="1">
       <c r="A46" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="D46" s="13"/>
-    </row>
-    <row r="47" spans="1:4" s="14" customFormat="1">
+    </row>
+    <row r="47" spans="1:4" s="14" customFormat="1" ht="30">
       <c r="A47" s="12" t="s">
         <v>136</v>
       </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="D47" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="10" customFormat="1">
+      <c r="A48" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="10" customFormat="1">
+      <c r="A49" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="15" customFormat="1">
+      <c r="A51" s="12" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" s="10" customFormat="1" ht="30">
-      <c r="A48" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="12" t="s">
+      <c r="B51" s="14"/>
+      <c r="C51" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="15" customFormat="1">
+      <c r="A52" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="D49" s="13" t="s">
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="13"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D54" s="13" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="15" customFormat="1">
-      <c r="A50" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="D51" s="13"/>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="30">
-      <c r="A53" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" s="3">
-        <v>5</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B55" s="3">
-        <v>6</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="D55" s="13"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B56" s="3">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="2" t="s">
-        <v>94</v>
+      <c r="A57" s="12" t="s">
+        <v>137</v>
       </c>
       <c r="B57" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B58" s="3">
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="B59" s="3">
-        <v>9</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="B60" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="12" t="s">
-        <v>120</v>
+      <c r="A61" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="B61" s="3">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B62" s="3">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="2" t="s">
-        <v>7</v>
+      <c r="A63" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="B63" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="B64" s="3">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B65" s="3">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="B66" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B67" s="3">
-        <v>18</v>
+      <c r="A67" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B68" s="3">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="B69" s="3">
-        <v>20</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="12" t="s">
-        <v>115</v>
+      <c r="A70" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B70" s="3">
-        <v>21</v>
-      </c>
-      <c r="D70" s="13" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B71" s="3">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="12" t="s">
-        <v>123</v>
+      <c r="A72" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B72" s="3">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="2" t="s">
-        <v>41</v>
+      <c r="A73" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="B73" s="3">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="D73" s="13" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B75" s="3">
+        <v>23</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B76" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B77" s="3">
         <v>25</v>
       </c>
-      <c r="D74" s="13" t="s">
+      <c r="D77" s="13" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B75" s="3">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B76" s="3">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B77" s="3">
-        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="B78" s="3">
-        <v>29</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B79" s="3">
-        <v>30</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="30">
+      <c r="A79" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B80" s="3">
-        <v>31</v>
+      <c r="A80" s="12" t="s">
+        <v>165</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="2" t="s">
-        <v>85</v>
+      <c r="A81" s="12" t="s">
+        <v>118</v>
       </c>
       <c r="B81" s="3">
-        <v>32</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="2" t="s">
-        <v>93</v>
+      <c r="A82" s="12" t="s">
+        <v>119</v>
       </c>
       <c r="B82" s="3">
-        <v>33</v>
-      </c>
-      <c r="D82" s="13" t="s">
-        <v>121</v>
+        <v>28</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="B83" s="3">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="B84" s="3">
-        <v>35</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="12" t="s">
-        <v>113</v>
+      <c r="A85" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="B85" s="3">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B86" s="3">
-        <v>37</v>
+        <v>32</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B87" s="3">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="D87" s="13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="12" t="s">
-        <v>117</v>
+      <c r="A88" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="B88" s="3">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B89" s="3">
+        <v>35</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B90" s="3">
+        <v>36</v>
+      </c>
+      <c r="D90" s="13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B91" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B92" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B93" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B89" s="3">
+      <c r="B94" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="2" t="s">
+    <row r="95" spans="1:4" s="10" customFormat="1">
+      <c r="A95" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B90" s="3">
+      <c r="B95" s="3">
         <v>41</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" s="10" customFormat="1" ht="30">
-      <c r="A91" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D91" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="30">
-      <c r="A92" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B92" s="10"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B93" s="10"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="11" t="s">
+      <c r="C95" s="3"/>
+      <c r="D95" s="4"/>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B96" s="3">
         <v>42</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B94" s="10"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="11"/>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B95" s="10"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="11" t="s">
-        <v>109</v>
+      <c r="D96" s="13" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="12" t="s">
-        <v>124</v>
+        <v>139</v>
+      </c>
+      <c r="B97" s="3">
+        <v>43</v>
       </c>
       <c r="D97" s="13" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="12" t="s">
-        <v>130</v>
+        <v>158</v>
+      </c>
+      <c r="B98" s="3">
+        <v>44</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="45">
       <c r="A99" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
+        <v>144</v>
+      </c>
+      <c r="B99" s="3">
+        <v>45</v>
+      </c>
+      <c r="C99" s="14"/>
+      <c r="D99" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="30">
       <c r="A100" s="12" t="s">
-        <v>139</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="C100" s="14"/>
       <c r="D100" s="13" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="D101" s="13" t="s">
-        <v>145</v>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="30">
+      <c r="A101" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B101" s="10"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="30">
+      <c r="A102" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B102" s="10"/>
+      <c r="C102" s="10"/>
+      <c r="D102" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="30">
+      <c r="A103" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B103" s="10"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B104" s="10"/>
+      <c r="C104" s="10"/>
+      <c r="D104" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B105" s="10"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="11"/>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B106" s="10"/>
+      <c r="C106" s="10"/>
+      <c r="D106" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="11" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TimeTasks now appear on WeekView
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="173">
   <si>
     <t>Feature</t>
   </si>
@@ -156,9 +156,6 @@
     <t>separate spinners for year month day time</t>
   </si>
   <si>
-    <t>Continuous Day Panel</t>
-  </si>
-  <si>
     <t>Identical to a Day panel, but not restricted to a single day, update Date and watermark to date with most area, when midnight passes viewport middle. Update extent range to 3 days before, current, after</t>
   </si>
   <si>
@@ -532,6 +529,21 @@
   </si>
   <si>
     <t>In EF is there a way to prevent the modification of certain entities? No just do it from VM</t>
+  </si>
+  <si>
+    <t>MonthPanel</t>
+  </si>
+  <si>
+    <t>YearPanel</t>
+  </si>
+  <si>
+    <t>Continuous Panel</t>
+  </si>
+  <si>
+    <t>LoadingView as separate window</t>
+  </si>
+  <si>
+    <t>Run in a separate borderless window fixed on the parent window in a different thread. See: project "LoadingOverlay"</t>
   </si>
 </sst>
 </file>
@@ -760,8 +772,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D107" totalsRowShown="0">
-  <autoFilter ref="A1:D107" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D110" totalsRowShown="0">
+  <autoFilter ref="A1:D110" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
   <sortState ref="A2:D83">
     <sortCondition ref="B1:B83"/>
   </sortState>
@@ -1072,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:H107"/>
+  <dimension ref="A1:H110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1175,59 +1187,59 @@
     </row>
     <row r="10" spans="1:4" ht="30">
       <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1">
       <c r="A13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1">
       <c r="A14" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="5" customFormat="1">
@@ -1239,7 +1251,7 @@
         <v>29</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="5" customFormat="1">
@@ -1254,14 +1266,14 @@
     </row>
     <row r="17" spans="1:8" s="5" customFormat="1">
       <c r="A17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="5" customFormat="1">
@@ -1276,7 +1288,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>29</v>
@@ -1284,29 +1296,29 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>29</v>
@@ -1314,7 +1326,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>29</v>
@@ -1328,7 +1340,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>29</v>
@@ -1336,7 +1348,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>29</v>
@@ -1350,18 +1362,18 @@
         <v>29</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1374,7 +1386,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>29</v>
@@ -1406,7 +1418,7 @@
         <v>29</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1427,7 +1439,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>29</v>
@@ -1435,7 +1447,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>29</v>
@@ -1443,7 +1455,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>29</v>
@@ -1451,7 +1463,7 @@
     </row>
     <row r="38" spans="1:4" s="14" customFormat="1">
       <c r="A38" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>29</v>
@@ -1460,18 +1472,18 @@
     </row>
     <row r="39" spans="1:4" s="14" customFormat="1">
       <c r="A39" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="13" t="s">
         <v>132</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>29</v>
@@ -1479,7 +1491,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>29</v>
@@ -1487,29 +1499,29 @@
     </row>
     <row r="42" spans="1:4" ht="30">
       <c r="A42" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="13" t="s">
         <v>141</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" s="13" t="s">
         <v>134</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="3">
         <v>1</v>
@@ -1531,42 +1543,42 @@
     </row>
     <row r="46" spans="1:4" s="14" customFormat="1">
       <c r="A46" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="14" customFormat="1" ht="30">
       <c r="A47" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="10" customFormat="1">
       <c r="A48" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="10" customFormat="1">
       <c r="A49" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="14" t="s">
@@ -1576,42 +1588,42 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C50" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="15" customFormat="1">
       <c r="A51" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B51" s="14"/>
       <c r="C51" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:4" s="15" customFormat="1">
       <c r="A52" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
@@ -1619,15 +1631,15 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D55" s="13"/>
     </row>
@@ -1639,12 +1651,12 @@
         <v>5</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B57" s="3">
         <v>6</v>
@@ -1658,12 +1670,12 @@
         <v>6.5</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B59" s="3">
         <v>7</v>
@@ -1677,34 +1689,34 @@
         <v>8</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B61" s="3">
         <v>9</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B62" s="3">
         <v>10</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B63" s="3">
         <v>12</v>
@@ -1712,13 +1724,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B64" s="3">
         <v>13</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1739,10 +1751,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D67" s="13" t="s">
         <v>152</v>
-      </c>
-      <c r="D67" s="13" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1755,7 +1767,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B69" s="3">
         <v>17</v>
@@ -1777,29 +1789,29 @@
         <v>19</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B72" s="3">
         <v>20</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B73" s="3">
         <v>21</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1812,13 +1824,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B75" s="3">
         <v>23</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1850,23 +1862,23 @@
     </row>
     <row r="79" spans="1:4" ht="30">
       <c r="A79" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B81" s="3">
         <v>27</v>
@@ -1874,7 +1886,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B82" s="3">
         <v>28</v>
@@ -1882,18 +1894,18 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B83" s="3">
+        <v>29</v>
+      </c>
+      <c r="D83" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="B83" s="3">
-        <v>29</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B84" s="3">
         <v>30</v>
@@ -1901,232 +1913,253 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B85" s="3">
         <v>31</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B86" s="3">
-        <v>32</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="A86" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="D86" s="13"/>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B87" s="3">
-        <v>33</v>
-      </c>
-      <c r="D87" s="13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B88" s="3">
-        <v>34</v>
-      </c>
-      <c r="D88" s="4" t="s">
-        <v>100</v>
+      <c r="A87" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="D87" s="13"/>
+    </row>
+    <row r="88" spans="1:4" ht="30">
+      <c r="A88" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="B89" s="3">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="12" t="s">
-        <v>113</v>
+      <c r="A90" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="B90" s="3">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D90" s="13" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B91" s="3">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="B92" s="3">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="12" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B93" s="3">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="D93" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="B94" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" s="10" customFormat="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B95" s="3">
-        <v>41</v>
-      </c>
-      <c r="C95" s="3"/>
-      <c r="D95" s="4"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="12" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B96" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" s="10" customFormat="1">
+      <c r="A97" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B97" s="3">
+        <v>40</v>
+      </c>
+      <c r="C97" s="3"/>
+      <c r="D97" s="4"/>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B98" s="3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B99" s="3">
         <v>42</v>
       </c>
-      <c r="D96" s="13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="12" t="s">
+      <c r="D99" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B100" s="3">
+        <v>43</v>
+      </c>
+      <c r="D100" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="B97" s="3">
-        <v>43</v>
-      </c>
-      <c r="D97" s="13" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="12" t="s">
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B101" s="3">
+        <v>44</v>
+      </c>
+      <c r="D101" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="B98" s="3">
-        <v>44</v>
-      </c>
-      <c r="D98" s="13" t="s">
+    </row>
+    <row r="102" spans="1:4" ht="45">
+      <c r="A102" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B102" s="3">
+        <v>45</v>
+      </c>
+      <c r="C102" s="14"/>
+      <c r="D102" s="13" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="45">
-      <c r="A99" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="B99" s="3">
-        <v>45</v>
-      </c>
-      <c r="C99" s="14"/>
-      <c r="D99" s="13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="30">
-      <c r="A100" s="12" t="s">
+    <row r="103" spans="1:4" ht="30">
+      <c r="A103" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C103" s="14"/>
+      <c r="D103" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="C100" s="14"/>
-      <c r="D100" s="13" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="30">
-      <c r="A101" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="B101" s="10"/>
-      <c r="C101" s="10"/>
-      <c r="D101" s="11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="30">
-      <c r="A102" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B102" s="10"/>
-      <c r="C102" s="10"/>
-      <c r="D102" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="30">
-      <c r="A103" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B103" s="10"/>
-      <c r="C103" s="10"/>
-      <c r="D103" s="11" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B104" s="10"/>
-      <c r="C104" s="10"/>
-      <c r="D104" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
+      <c r="A104" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="C104" s="14"/>
+      <c r="D104" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" s="14" customFormat="1" ht="30">
       <c r="A105" s="9" t="s">
-        <v>21</v>
+        <v>148</v>
       </c>
       <c r="B105" s="10"/>
       <c r="C105" s="10"/>
-      <c r="D105" s="11"/>
-    </row>
-    <row r="106" spans="1:4">
+      <c r="D105" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="30">
       <c r="A106" s="9" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="B106" s="10"/>
       <c r="C106" s="10"/>
       <c r="D106" s="11" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="9" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="B107" s="10"/>
       <c r="C107" s="10"/>
       <c r="D107" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B108" s="10"/>
+      <c r="C108" s="10"/>
+      <c r="D108" s="11"/>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B109" s="10"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="11" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B110" s="10"/>
+      <c r="C110" s="10"/>
+      <c r="D110" s="11" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2158,17 +2191,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CheckIn Views, CalendarViewModel redone, CheckIn CRUDS
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="448">
   <si>
     <t>Feature</t>
   </si>
@@ -640,9 +640,6 @@
   </si>
   <si>
     <t>CalculateCollisions()</t>
-  </si>
-  <si>
-    <t>Square with rounded corners and the right bottom corner is flipped up. Color by task type, but with a darker shade and a black border.</t>
   </si>
   <si>
     <t>Filters on the EntityViews</t>
@@ -1443,13 +1440,40 @@
     <t>Recalculate remaining allocations. Identify empty spaces. For each empty space, check if there is any relevant task that can be allocated by priority of: Highest priority intersecting insufficient InclusionZone, highest priority intersecting InclusionZone with CanFill.</t>
   </si>
   <si>
-    <t>async CreateTaskObjs</t>
-  </si>
-  <si>
-    <t>Is it possible to make the Interpret Data/Organize Data async?</t>
-  </si>
-  <si>
-    <t>What funcs do I need to call? I don’t need to BuildCheckIns() but everything afterwards?</t>
+    <t>Sequential Prioritization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e.g. Task A can't be done until Task B is done. </t>
+  </si>
+  <si>
+    <t>CheckIns on Calendar</t>
+  </si>
+  <si>
+    <t>like Notes</t>
+  </si>
+  <si>
+    <t>CheckIn graphic</t>
+  </si>
+  <si>
+    <t>Triangle centered on time, on the side, line spanning day</t>
+  </si>
+  <si>
+    <t>Square with rounded corners and the right bottom corner is flipped up.</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Zooming in is glitchy, more glitchy the farther scrolled down</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>Need to reload Notes/CheckIns/Tasks when adding new respectively in Calendar</t>
+  </si>
+  <si>
+    <t>What funcs do I need to call? I don’t need to BuildCheckIns() but everything afterwards? Add CheckIns to TaskMaps on new. Find CheckIn from TaskMaps on edit.</t>
   </si>
 </sst>
 </file>
@@ -1855,7 +1879,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2031,6 +2055,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2239,34 +2266,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -2464,13 +2463,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -2483,6 +2475,41 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3559,8 +3586,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:C150" totalsRowShown="0">
-  <autoFilter ref="A1:C150" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:C154" totalsRowShown="0">
+  <autoFilter ref="A1:C154" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="86"/>
     <tableColumn id="6" xr3:uid="{1FFE88A6-F499-42FB-A3F4-F5BDCD9D0CF0}" name="Done"/>
@@ -3648,17 +3675,17 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A637EB4D-B0BD-451A-AEF8-4F572CDAEA03}" name="Table7" displayName="Table7" ref="A1:H5" totalsRowShown="0" headerRowDxfId="26" dataDxfId="27" headerRowBorderDxfId="36" tableBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A637EB4D-B0BD-451A-AEF8-4F572CDAEA03}" name="Table7" displayName="Table7" ref="A1:H5" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34">
   <autoFilter ref="A1:H5" xr:uid="{1C355147-87D4-4562-8BCA-2AC6E8731BE0}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{2D2C5C32-B8C1-434D-9678-8FA28AA9E25E}" name="C1 ∩ C2" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{83D2755C-6BC6-444B-B47B-E805256587D2}" name="C2HasRoom = T_x000a_C1 &gt;= C2" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{1CE782A0-B082-4A0B-9C40-AF715F441CC4}" name="C2HasRoom = T_x000a_C1 &lt; C2" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{BD5AA1DC-AE84-47FC-9B2A-54FD9FA153CE}" name="C2HasRoom = F_x000a_C2CanReDist = T_x000a_C1 &gt;= C2" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{BB1432BE-D946-4CB6-B3F6-04E8F22BC33F}" name="C2HasRoom = F_x000a_C2CanReDist = T_x000a_C1 &lt; C2" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{69EA148B-29D0-4FD1-8924-7228DCD5168D}" name="C2HasRoom = F_x000a_C2CanReDist = F_x000a_C1 &gt;= C2" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{5304745C-6EDF-461B-A5C3-75B5645DF5C0}" name="C2HasRoom = F_x000a_C2CanReDist = F_x000a_C1 &lt; C2" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{94277B06-039D-4427-8C01-ABF777E3ED15}" name="C2S🔒" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{2D2C5C32-B8C1-434D-9678-8FA28AA9E25E}" name="C1 ∩ C2" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{83D2755C-6BC6-444B-B47B-E805256587D2}" name="C2HasRoom = T_x000a_C1 &gt;= C2" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{1CE782A0-B082-4A0B-9C40-AF715F441CC4}" name="C2HasRoom = T_x000a_C1 &lt; C2" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{BD5AA1DC-AE84-47FC-9B2A-54FD9FA153CE}" name="C2HasRoom = F_x000a_C2CanReDist = T_x000a_C1 &gt;= C2" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{BB1432BE-D946-4CB6-B3F6-04E8F22BC33F}" name="C2HasRoom = F_x000a_C2CanReDist = T_x000a_C1 &lt; C2" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{69EA148B-29D0-4FD1-8924-7228DCD5168D}" name="C2HasRoom = F_x000a_C2CanReDist = F_x000a_C1 &gt;= C2" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{5304745C-6EDF-461B-A5C3-75B5645DF5C0}" name="C2HasRoom = F_x000a_C2CanReDist = F_x000a_C1 &lt; C2" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{94277B06-039D-4427-8C01-ABF777E3ED15}" name="C2S🔒" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3961,9 +3988,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:G150"/>
+  <dimension ref="A1:G154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
       <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
@@ -4536,13 +4563,13 @@
     </row>
     <row r="59" spans="1:3" ht="30">
       <c r="A59" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="12" t="s">
         <v>211</v>
-      </c>
-      <c r="B59" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -4553,56 +4580,56 @@
         <v>23</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B61" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C64" s="24" t="s">
         <v>311</v>
-      </c>
-      <c r="B64" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C64" s="24" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>23</v>
@@ -4611,7 +4638,7 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>23</v>
@@ -4620,7 +4647,7 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>23</v>
@@ -4629,7 +4656,7 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>23</v>
@@ -4638,7 +4665,7 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>23</v>
@@ -4647,7 +4674,7 @@
     </row>
     <row r="70" spans="1:3" s="9" customFormat="1">
       <c r="A70" s="11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>23</v>
@@ -4656,38 +4683,38 @@
     </row>
     <row r="71" spans="1:3" s="9" customFormat="1" ht="30">
       <c r="A71" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="9" customFormat="1">
       <c r="A72" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="73" spans="1:3" s="9" customFormat="1">
       <c r="A73" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B73" s="13"/>
       <c r="C73" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="74" spans="1:3" s="9" customFormat="1">
       <c r="A74" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>23</v>
@@ -4696,16 +4723,16 @@
     </row>
     <row r="75" spans="1:3" s="9" customFormat="1">
       <c r="A75" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B75" s="13"/>
       <c r="C75" s="12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="9" customFormat="1">
       <c r="A76" s="11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>23</v>
@@ -4723,7 +4750,7 @@
     </row>
     <row r="78" spans="1:3" s="9" customFormat="1">
       <c r="A78" s="11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>23</v>
@@ -4732,7 +4759,7 @@
     </row>
     <row r="79" spans="1:3" s="9" customFormat="1">
       <c r="A79" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>23</v>
@@ -4741,7 +4768,7 @@
     </row>
     <row r="80" spans="1:3" s="13" customFormat="1">
       <c r="A80" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>23</v>
@@ -4750,60 +4777,68 @@
     </row>
     <row r="81" spans="1:3" s="13" customFormat="1">
       <c r="A81" s="11" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
     </row>
     <row r="82" spans="1:3" s="13" customFormat="1">
       <c r="A82" s="11" t="s">
-        <v>431</v>
+        <v>445</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="13" customFormat="1">
       <c r="A83" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="C83" s="12" t="s">
         <v>432</v>
       </c>
-      <c r="C83" s="12" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" s="13" customFormat="1" ht="30">
+    </row>
+    <row r="84" spans="1:3" s="13" customFormat="1">
       <c r="A84" s="11" t="s">
-        <v>255</v>
+        <v>438</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>254</v>
+        <v>439</v>
       </c>
     </row>
     <row r="85" spans="1:3" s="13" customFormat="1">
       <c r="A85" s="11" t="s">
-        <v>125</v>
+        <v>440</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>210</v>
+        <v>441</v>
       </c>
     </row>
     <row r="86" spans="1:3" s="13" customFormat="1">
-      <c r="A86" s="11" t="s">
+      <c r="A86" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="B86" s="3"/>
-      <c r="C86" s="12" t="s">
-        <v>203</v>
+      <c r="B86" s="9"/>
+      <c r="C86" s="10" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="87" spans="1:3" s="13" customFormat="1">
       <c r="A87" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B87" s="3"/>
+      <c r="B87" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="C87" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="88" spans="1:3" s="13" customFormat="1">
@@ -4818,443 +4853,479 @@
       <c r="A89" s="11" t="s">
         <v>196</v>
       </c>
+      <c r="B89" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="C89" s="12"/>
     </row>
     <row r="90" spans="1:3" s="13" customFormat="1">
       <c r="A90" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="C90" s="12" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" s="13" customFormat="1" ht="30">
+      <c r="A91" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" s="13" customFormat="1">
+      <c r="A92" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" s="13" customFormat="1">
+      <c r="A93" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C90" s="12"/>
-    </row>
-    <row r="91" spans="1:3" s="13" customFormat="1">
-      <c r="A91" s="11" t="s">
+      <c r="C93" s="12"/>
+    </row>
+    <row r="94" spans="1:3" s="13" customFormat="1">
+      <c r="A94" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C91" s="12" t="s">
+      <c r="C94" s="12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="2" t="s">
+    <row r="95" spans="1:3" s="13" customFormat="1">
+      <c r="A95" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="B95" s="3"/>
+      <c r="C95" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="B93" s="13"/>
-      <c r="C93" s="12"/>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" s="11" t="s">
+    <row r="96" spans="1:3">
+      <c r="A96" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B96" s="13"/>
+      <c r="C96" s="12"/>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
-      <c r="A95" s="11" t="s">
+    <row r="98" spans="1:3">
+      <c r="A98" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="C95" s="12" t="s">
+      <c r="C98" s="12" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
-      <c r="A96" s="2" t="s">
+    <row r="99" spans="1:3">
+      <c r="A99" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C99" s="4" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="C99" s="12" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C102" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="30">
-      <c r="A101" s="11" t="s">
+    <row r="104" spans="1:3" ht="30">
+      <c r="A104" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="C104" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="C101" s="12" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" s="2" t="s">
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
-      <c r="A103" s="11" t="s">
+    <row r="106" spans="1:3">
+      <c r="A106" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C103" s="12" t="s">
+      <c r="C106" s="12" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
-      <c r="A104" s="11" t="s">
+    <row r="107" spans="1:3">
+      <c r="A107" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="C104" s="12" t="s">
+      <c r="C107" s="12" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
-      <c r="A105" s="11" t="s">
+    <row r="108" spans="1:3">
+      <c r="A108" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C105" s="12" t="s">
+      <c r="C108" s="12" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
-      <c r="A106" s="2" t="s">
+    <row r="109" spans="1:3">
+      <c r="A109" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C107" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C109" s="12" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="C111" s="12" t="s">
-        <v>225</v>
+      <c r="A111" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="112" spans="1:3">
-      <c r="A112" s="2" t="s">
-        <v>79</v>
+      <c r="A112" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="2" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="2" t="s">
-        <v>33</v>
+      <c r="A114" s="11" t="s">
+        <v>223</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>34</v>
+        <v>224</v>
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="11" t="s">
-        <v>125</v>
+      <c r="A115" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>205</v>
+        <v>103</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C116" s="12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="30">
-      <c r="A117" s="11" t="s">
-        <v>142</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>141</v>
+        <v>34</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="11" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="C118" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="30">
-      <c r="A119" s="11" t="s">
-        <v>372</v>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="30">
       <c r="A120" s="11" t="s">
-        <v>373</v>
+        <v>142</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>374</v>
+        <v>141</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="11" t="s">
-        <v>100</v>
+        <v>144</v>
+      </c>
+      <c r="C121" s="12" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C123" s="4" t="s">
-        <v>45</v>
+        <v>436</v>
+      </c>
+      <c r="C122" s="12" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="30">
+      <c r="A123" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="C123" s="12" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="2" t="s">
-        <v>49</v>
+      <c r="A124" s="11" t="s">
+        <v>372</v>
+      </c>
+      <c r="C124" s="12" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C125" s="12" t="s">
-        <v>104</v>
+      <c r="A125" s="11" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="C126" s="12"/>
+        <v>101</v>
+      </c>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="C127" s="12"/>
+      <c r="A127" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="11" t="s">
+      <c r="A128" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C129" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C130" s="12"/>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C131" s="12"/>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="C128" s="12"/>
-    </row>
-    <row r="129" spans="1:3">
-      <c r="A129" s="11" t="s">
+      <c r="C132" s="12"/>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C129" s="12"/>
-    </row>
-    <row r="130" spans="1:3" ht="30">
-      <c r="A130" s="11" t="s">
+      <c r="C133" s="12"/>
+    </row>
+    <row r="134" spans="1:3" ht="30">
+      <c r="A134" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B130" s="13"/>
-      <c r="C130" s="12" t="s">
+      <c r="B134" s="13"/>
+      <c r="C134" s="12" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
-      <c r="A131" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3">
-      <c r="A132" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C132" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3">
-      <c r="A133" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3">
-      <c r="A134" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C134" s="12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="136" spans="1:3">
-      <c r="A136" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C136" s="12" t="s">
-        <v>209</v>
+      <c r="A136" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" s="9" customFormat="1">
+        <v>89</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
       <c r="A138" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B138" s="3"/>
-      <c r="C138" s="4"/>
+        <v>95</v>
+      </c>
+      <c r="C138" s="12" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="2" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
     </row>
     <row r="140" spans="1:3">
-      <c r="A140" s="2" t="s">
-        <v>59</v>
+      <c r="A140" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C140" s="12" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="141" spans="1:3">
-      <c r="A141" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C141" s="12" t="s">
-        <v>113</v>
+      <c r="A141" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C142" s="12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3">
-      <c r="A143" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C143" s="12" t="s">
-        <v>138</v>
-      </c>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" s="9" customFormat="1">
+      <c r="A143" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B143" s="3"/>
+      <c r="C143" s="4"/>
     </row>
     <row r="144" spans="1:3">
-      <c r="A144" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B144" s="13"/>
-      <c r="C144" s="12" t="s">
-        <v>146</v>
+      <c r="A144" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="B145" s="13"/>
+        <v>106</v>
+      </c>
       <c r="C145" s="12" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="B146" s="13"/>
+        <v>120</v>
+      </c>
       <c r="C146" s="12" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="B147" s="13"/>
+        <v>137</v>
+      </c>
       <c r="C147" s="12" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="30">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
       <c r="A148" s="11" t="s">
-        <v>240</v>
+        <v>145</v>
       </c>
       <c r="B148" s="13"/>
       <c r="C148" s="12" t="s">
-        <v>241</v>
+        <v>146</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="11" t="s">
-        <v>242</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="B149" s="13"/>
       <c r="C149" s="12" t="s">
-        <v>243</v>
+        <v>152</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B150" s="13"/>
+      <c r="C150" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B151" s="13"/>
+      <c r="C151" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="30">
+      <c r="A152" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="B152" s="13"/>
+      <c r="C152" s="12" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="C153" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C154" s="12" t="s">
         <v>271</v>
-      </c>
-      <c r="C150" s="12" t="s">
-        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -5318,18 +5389,18 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="23" customFormat="1">
@@ -5337,47 +5408,47 @@
         <v>201</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="23" customFormat="1">
       <c r="A7" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>247</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="23" customFormat="1">
       <c r="A9" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="B9" s="27" t="s">
         <v>305</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="18" customFormat="1">
       <c r="A10" s="16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="45">
@@ -5385,63 +5456,63 @@
         <v>202</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A13" s="23" t="s">
+        <v>434</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>435</v>
-      </c>
-      <c r="B13" s="27" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="45">
       <c r="B21" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="30">
       <c r="B22" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="30">
       <c r="B23" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="45">
       <c r="B24" s="15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -5479,7 +5550,7 @@
         <v>163</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>164</v>
@@ -5488,7 +5559,7 @@
         <v>197</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5502,10 +5573,10 @@
         <v>184</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5519,7 +5590,7 @@
         <v>185</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5533,7 +5604,7 @@
         <v>186</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>166</v>
@@ -5541,13 +5612,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B6" s="33" t="s">
         <v>176</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5558,10 +5629,10 @@
         <v>177</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5575,7 +5646,7 @@
         <v>187</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5589,10 +5660,10 @@
         <v>188</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5603,10 +5674,10 @@
         <v>180</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>171</v>
@@ -5623,15 +5694,15 @@
         <v>190</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B12" s="39" t="s">
         <v>182</v>
@@ -5640,10 +5711,10 @@
         <v>192</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -5657,50 +5728,50 @@
         <v>191</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="29" customFormat="1">
       <c r="A21" s="29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="29" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -5740,222 +5811,222 @@
   <sheetData>
     <row r="1" spans="1:10" ht="30.75" thickBot="1">
       <c r="A1" s="50" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="51" t="s">
+        <v>290</v>
+      </c>
+      <c r="C1" s="52" t="s">
         <v>291</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="D1" s="52" t="s">
         <v>292</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="E1" s="52" t="s">
         <v>293</v>
       </c>
-      <c r="E1" s="52" t="s">
-        <v>294</v>
-      </c>
       <c r="F1" s="52" t="s">
+        <v>283</v>
+      </c>
+      <c r="G1" s="52" t="s">
         <v>284</v>
       </c>
-      <c r="G1" s="52" t="s">
-        <v>285</v>
-      </c>
       <c r="H1" s="53" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="75">
       <c r="A2" s="46" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H2" s="48" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="60">
       <c r="A3" s="47" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H3" s="49" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="75">
       <c r="A4" s="47" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H4" s="49" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:10" ht="60">
       <c r="A5" s="47" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H5" s="49" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:10" ht="60">
       <c r="A6" s="47" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H6" s="49" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
     </row>
     <row r="7" spans="1:10" ht="60">
       <c r="A7" s="47" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H7" s="49" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
     </row>
     <row r="8" spans="1:10" ht="60">
       <c r="A8" s="54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C8" s="56" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D8" s="56" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E8" s="56" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G8" s="56" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H8" s="57" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
@@ -6225,7 +6296,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="12" customFormat="1">
       <c r="A1" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -6235,7 +6306,7 @@
     </row>
     <row r="2" spans="1:6" s="12" customFormat="1">
       <c r="A2" s="27" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
@@ -6245,7 +6316,7 @@
     </row>
     <row r="3" spans="1:6" s="12" customFormat="1">
       <c r="A3" s="27" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
@@ -6255,7 +6326,7 @@
     </row>
     <row r="4" spans="1:6" s="12" customFormat="1">
       <c r="A4" s="27" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B4" s="44"/>
       <c r="C4" s="44"/>
@@ -6265,7 +6336,7 @@
     </row>
     <row r="5" spans="1:6" s="12" customFormat="1">
       <c r="A5" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
@@ -6275,177 +6346,177 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="27" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="27" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="27" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="12" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="30">
       <c r="A19" s="27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="27" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="27" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="30">
       <c r="A26" s="27" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="27" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="90">
       <c r="A28" s="61" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="61" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="61" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="61" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="135">
       <c r="A35" s="61" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="24" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30">
       <c r="A39" s="27" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="30">
       <c r="A40" s="27" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="27" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30">
       <c r="A42" s="27" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="27" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="27" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="8" customFormat="1">
       <c r="A48" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B48" s="80"/>
       <c r="C48" s="80"/>
@@ -6455,7 +6526,7 @@
     </row>
     <row r="49" spans="1:6" s="8" customFormat="1" ht="30">
       <c r="A49" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B49" s="80"/>
       <c r="C49" s="80"/>
@@ -6465,7 +6536,7 @@
     </row>
     <row r="50" spans="1:6" s="8" customFormat="1" ht="30">
       <c r="A50" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B50" s="80"/>
       <c r="C50" s="80"/>
@@ -6475,7 +6546,7 @@
     </row>
     <row r="51" spans="1:6" s="8" customFormat="1">
       <c r="A51" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B51" s="80"/>
       <c r="C51" s="80"/>
@@ -6492,7 +6563,7 @@
     </row>
     <row r="53" spans="1:6" s="8" customFormat="1">
       <c r="A53" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B53" s="80"/>
       <c r="C53" s="80"/>
@@ -6502,7 +6573,7 @@
     </row>
     <row r="54" spans="1:6" s="8" customFormat="1">
       <c r="A54" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B54" s="80"/>
       <c r="C54" s="80"/>
@@ -6512,7 +6583,7 @@
     </row>
     <row r="55" spans="1:6" s="8" customFormat="1" ht="30">
       <c r="A55" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B55" s="80"/>
       <c r="C55" s="80"/>
@@ -6522,7 +6593,7 @@
     </row>
     <row r="56" spans="1:6" s="8" customFormat="1">
       <c r="A56" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B56" s="80"/>
       <c r="C56" s="80"/>
@@ -6532,7 +6603,7 @@
     </row>
     <row r="57" spans="1:6" s="8" customFormat="1" ht="45">
       <c r="A57" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B57" s="80"/>
       <c r="C57" s="80"/>
@@ -6542,27 +6613,27 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="30">
       <c r="A61" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -6595,132 +6666,132 @@
   <sheetData>
     <row r="1" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A1" s="59" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B1" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>393</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>394</v>
-      </c>
       <c r="D1" s="27" t="s">
+        <v>413</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>412</v>
+      </c>
+      <c r="F1" s="27" t="s">
         <v>414</v>
       </c>
-      <c r="E1" s="27" t="s">
-        <v>413</v>
-      </c>
-      <c r="F1" s="27" t="s">
+      <c r="G1" s="27" t="s">
         <v>415</v>
       </c>
-      <c r="G1" s="27" t="s">
-        <v>416</v>
-      </c>
       <c r="H1" s="27" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="23" customFormat="1">
       <c r="A2" s="62" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B2" s="41" t="s">
+        <v>380</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>381</v>
       </c>
-      <c r="C2" s="28" t="s">
-        <v>382</v>
-      </c>
       <c r="D2" s="28" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G2" s="48" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H2" s="48" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A3" s="62" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B3" s="42" t="s">
+        <v>380</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>380</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>380</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="F3" s="19" t="s">
         <v>381</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="G3" s="49" t="s">
         <v>381</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="H3" s="49" t="s">
         <v>381</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>383</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>382</v>
-      </c>
-      <c r="G3" s="49" t="s">
-        <v>382</v>
-      </c>
-      <c r="H3" s="49" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A4" s="62" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E4" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="F4" s="19" t="s">
         <v>383</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>384</v>
-      </c>
       <c r="G4" s="49" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H4" s="49" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="23" customFormat="1" ht="15.75" thickBot="1">
       <c r="A5" s="58" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D5" s="56" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G5" s="57" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H5" s="57" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="23" customFormat="1">
@@ -6735,119 +6806,119 @@
     </row>
     <row r="7" spans="1:12" ht="30.75" thickBot="1">
       <c r="A7" s="50" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B7" s="51" t="s">
+        <v>395</v>
+      </c>
+      <c r="C7" s="52" t="s">
         <v>396</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="D7" s="52" t="s">
         <v>397</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="E7" s="52" t="s">
         <v>398</v>
       </c>
-      <c r="E7" s="52" t="s">
-        <v>399</v>
-      </c>
       <c r="F7" s="53" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H7" s="43"/>
       <c r="I7" s="43"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="46" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B8" s="41" t="s">
+        <v>380</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>381</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>382</v>
-      </c>
       <c r="D8" s="28" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F8" s="48" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H8" s="43"/>
       <c r="I8" s="43"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="47" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D9" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>383</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>384</v>
-      </c>
       <c r="F9" s="49" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H9" s="43"/>
       <c r="I9" s="43"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="54" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B10" s="55" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D10" s="56" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H10" s="43"/>
       <c r="I10" s="43"/>
     </row>
     <row r="12" spans="1:12" ht="45.75" thickBot="1">
       <c r="A12" s="63" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B12" s="64" t="s">
+        <v>401</v>
+      </c>
+      <c r="C12" s="65" t="s">
         <v>402</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="D12" s="65" t="s">
         <v>403</v>
       </c>
-      <c r="D12" s="65" t="s">
+      <c r="E12" s="65" t="s">
         <v>404</v>
       </c>
-      <c r="E12" s="65" t="s">
+      <c r="F12" s="65" t="s">
         <v>405</v>
       </c>
-      <c r="F12" s="65" t="s">
+      <c r="G12" s="66" t="s">
         <v>406</v>
       </c>
-      <c r="G12" s="66" t="s">
+      <c r="H12" s="66" t="s">
         <v>407</v>
       </c>
-      <c r="H12" s="66" t="s">
-        <v>408</v>
-      </c>
       <c r="I12" s="66" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J12" s="45"/>
       <c r="K12" s="43"/>
@@ -6855,176 +6926,176 @@
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" s="67" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B13" s="68" t="s">
+        <v>380</v>
+      </c>
+      <c r="C13" s="69" t="s">
+        <v>380</v>
+      </c>
+      <c r="D13" s="70" t="s">
         <v>381</v>
       </c>
-      <c r="C13" s="69" t="s">
+      <c r="E13" s="69" t="s">
         <v>381</v>
       </c>
-      <c r="D13" s="70" t="s">
-        <v>382</v>
-      </c>
-      <c r="E13" s="69" t="s">
-        <v>382</v>
-      </c>
       <c r="F13" s="70" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G13" s="70" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H13" s="70" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I13" s="70" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="45">
       <c r="A14" s="71" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B14" s="72" t="s">
+        <v>380</v>
+      </c>
+      <c r="C14" s="73" t="s">
+        <v>227</v>
+      </c>
+      <c r="D14" s="74" t="s">
+        <v>380</v>
+      </c>
+      <c r="E14" s="73" t="s">
+        <v>382</v>
+      </c>
+      <c r="F14" s="75" t="s">
         <v>381</v>
       </c>
-      <c r="C14" s="73" t="s">
-        <v>228</v>
-      </c>
-      <c r="D14" s="74" t="s">
+      <c r="G14" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="H14" s="75" t="s">
         <v>381</v>
       </c>
-      <c r="E14" s="73" t="s">
-        <v>383</v>
-      </c>
-      <c r="F14" s="75" t="s">
-        <v>382</v>
-      </c>
-      <c r="G14" s="74" t="s">
-        <v>228</v>
-      </c>
-      <c r="H14" s="75" t="s">
-        <v>382</v>
-      </c>
       <c r="I14" s="75" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A15" s="71" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B15" s="72" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C15" s="73" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D15" s="74" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E15" s="73" t="s">
+        <v>382</v>
+      </c>
+      <c r="F15" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="G15" s="74" t="s">
         <v>383</v>
       </c>
-      <c r="F15" s="74" t="s">
-        <v>228</v>
-      </c>
-      <c r="G15" s="74" t="s">
-        <v>384</v>
-      </c>
       <c r="H15" s="74" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I15" s="74" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="23" customFormat="1">
       <c r="A16" s="67" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B16" s="76" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C16" s="77" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D16" s="78" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E16" s="77" t="s">
+        <v>382</v>
+      </c>
+      <c r="F16" s="78" t="s">
+        <v>382</v>
+      </c>
+      <c r="G16" s="78" t="s">
         <v>383</v>
       </c>
-      <c r="F16" s="78" t="s">
+      <c r="H16" s="78" t="s">
         <v>383</v>
       </c>
-      <c r="G16" s="78" t="s">
-        <v>384</v>
-      </c>
-      <c r="H16" s="78" t="s">
-        <v>384</v>
-      </c>
       <c r="I16" s="78" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="23" customFormat="1">
       <c r="A17" s="79" t="s">
+        <v>379</v>
+      </c>
+      <c r="B17" s="76" t="s">
         <v>380</v>
       </c>
-      <c r="B17" s="76" t="s">
-        <v>381</v>
-      </c>
       <c r="C17" s="77" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D17" s="78" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E17" s="77" t="s">
+        <v>382</v>
+      </c>
+      <c r="F17" s="78" t="s">
+        <v>382</v>
+      </c>
+      <c r="G17" s="78" t="s">
         <v>383</v>
       </c>
-      <c r="F17" s="78" t="s">
+      <c r="H17" s="78" t="s">
         <v>383</v>
       </c>
-      <c r="G17" s="78" t="s">
-        <v>384</v>
-      </c>
-      <c r="H17" s="78" t="s">
-        <v>384</v>
-      </c>
       <c r="I17" s="78" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="79" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B18" s="76" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C18" s="77" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D18" s="78" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E18" s="77" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F18" s="78" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G18" s="78" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H18" s="78" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I18" s="78" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -7087,132 +7158,132 @@
   <sheetData>
     <row r="1" spans="1:8" ht="45.75" thickBot="1">
       <c r="A1" s="50" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B1" s="51" t="s">
+        <v>341</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>337</v>
+      </c>
+      <c r="D1" s="52" t="s">
         <v>342</v>
       </c>
-      <c r="C1" s="52" t="s">
-        <v>338</v>
-      </c>
-      <c r="D1" s="52" t="s">
-        <v>343</v>
-      </c>
       <c r="E1" s="52" t="s">
+        <v>328</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>340</v>
+      </c>
+      <c r="G1" s="52" t="s">
         <v>329</v>
       </c>
-      <c r="F1" s="52" t="s">
-        <v>341</v>
-      </c>
-      <c r="G1" s="52" t="s">
-        <v>330</v>
-      </c>
       <c r="H1" s="53" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="46" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H2" s="48" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30">
       <c r="A3" s="47" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H3" s="49" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30">
       <c r="A4" s="47" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B4" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="F4" s="19" t="s">
         <v>335</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>337</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>337</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>336</v>
-      </c>
       <c r="G4" s="19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H4" s="49" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="54" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B5" s="55" t="s">
+        <v>334</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>334</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>336</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>336</v>
+      </c>
+      <c r="F5" s="56" t="s">
         <v>335</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="G5" s="56" t="s">
         <v>335</v>
       </c>
-      <c r="D5" s="56" t="s">
-        <v>337</v>
-      </c>
-      <c r="E5" s="56" t="s">
-        <v>337</v>
-      </c>
-      <c r="F5" s="56" t="s">
-        <v>336</v>
-      </c>
-      <c r="G5" s="56" t="s">
-        <v>336</v>
-      </c>
       <c r="H5" s="57" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:8">

</xml_diff>

<commit_message>
"It's time to go to bed" -Cat
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24930" windowHeight="12330" tabRatio="753" activeTab="4" xr2:uid="{B08B66F6-8B10-48BD-8CBC-92B4F4D60D54}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24930" windowHeight="12330" tabRatio="753" xr2:uid="{B08B66F6-8B10-48BD-8CBC-92B4F4D60D54}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="519">
   <si>
     <t>Feature</t>
   </si>
@@ -976,15 +976,6 @@
     <t>See: Collisions</t>
   </si>
   <si>
-    <t>A collision between two COs can be covered by a simple one pass approach, however as soon as we introduce chain collisions it becomes non-trivial and we run into problems like Ping-Ponging.</t>
-  </si>
-  <si>
-    <t>In theory, there should not be any remaining collisions after the second pass except for unresolvable collisions that are marked as conflict.</t>
-  </si>
-  <si>
-    <t>In the first pass, Measure, we look at every existing collision, calculate and propagate the forces produced by each collision based on the COs properties. A CO can have two forces acting on it, one on start, one on end. These forces are stored on the CO as properties. Any two forces acting on start or end are combined. Forces are propagated recursively in order to confirm that everything in a collision chain agrees.</t>
-  </si>
-  <si>
     <t>Redistribution</t>
   </si>
   <si>
@@ -1000,16 +991,10 @@
     <t>Redistribution problem: What if two CalObjs experience a collision where a lower priority task can only be done on a Monday, but the higher priority task can be done any day of the week?</t>
   </si>
   <si>
-    <t>To solve this, we need to introduce amultiple passes of Measure then Arrange approach to collisions.</t>
-  </si>
-  <si>
     <t>The consequence of not calculating this is that in the case where a non-redistributable lower priority C1 collides with a redistributable higher priority C2, the lower priority C1 will be incorrectly overwritten by the higher priority C2 that could have been redistributed.</t>
   </si>
   <si>
     <t>What if we, instead of detecting if C2 can truly redistribute, we detect if it might be able to based on if there is room for its sibling CO's. Then we put C2 in a "redistributing" state, finish the Measure/Arrange pass, then do a second Measure/Arrange pass. In the second pass, any CO in a "redistributing" state that failed to redistrubute in the first pass (wherein the time lost from the collision was not redistributed fully), will gain back the leftover time and go through another collision but this time assume that it can't be redistributed. Therein only after giving redistribution a try will C2 overwrite C1.</t>
-  </si>
-  <si>
-    <t>The aformentioned forces are not mathematical vectors, but instead are data structures that carry certain data. A force carries direction, size, and priority.</t>
   </si>
   <si>
     <t>C1 ∩ C2</t>
@@ -1154,9 +1139,6 @@
   </si>
   <si>
     <t>Inside Collision</t>
-  </si>
-  <si>
-    <t>If a Per has remaining &gt; 0, mark all of its CalObjs as Insufficient. If there are still collisions, mark them as Conflict. If there are any CalObjs that cross a zone boundary by more than MinDur, split it. Make sure states are correct: If a CalObj marked Unscheduled is within a proper InclusionZone, mark it correctly. If any CalObj not marked Unscheduled is outside of a proper InclusionZone, mark it Unscheduled.</t>
   </si>
   <si>
     <t>Does C2 have room to be split and pushed left or right?</t>
@@ -1194,9 +1176,6 @@
     <t>Not actually a CheckIn, but creates an End CheckIn at the start of the selected CalObj so that the CalObj takes up no time</t>
   </si>
   <si>
-    <t>Redistributions. If I want to do this, consider that collisions currently do not modify allocation.remaining, but instead handled in AllocateInsufficient().</t>
-  </si>
-  <si>
     <t>AllocateEmptySpace()</t>
   </si>
   <si>
@@ -1540,9 +1519,6 @@
     <t>Even Eager/Centered/Apathetic</t>
   </si>
   <si>
-    <t>When we have C1E and C2S both locked, that causes a conflict. But would it instead make sense to shrink one of them to cause a split? That way, conflicts won’t happen.</t>
-  </si>
-  <si>
     <t>CI Start
 in Z</t>
   </si>
@@ -1663,11 +1639,6 @@
     <t>Multi-Pass Collision Tests: to solve redistribution problem</t>
   </si>
   <si>
-    <t>Second, for each remaining collision, find empty spaces. 
-Using the loser C, for each empty space, if the empty space S intersects an inZone Z of the C.Per, shrink C up to Min(size of empty space, size of collision overlap), then FillEmptyWithInsuffZ(S, Z).
-Using the winner C, do the same.</t>
-  </si>
-  <si>
     <t>Ignore</t>
   </si>
   <si>
@@ -1680,10 +1651,27 @@
 … T C1 ∩ C2 T …</t>
   </si>
   <si>
-    <t>Third, check if any collisions still exist. Assume that these collisions cannot be redistributed and will be handled with shrinks.</t>
-  </si>
-  <si>
-    <t>First, for each collision, only push or split. Otherwise, ignore the collision.</t>
+    <t>First, for each collision, only push during an intersection collision and only split an inside collision when insider wins. Otherwise, ignore the collision.</t>
+  </si>
+  <si>
+    <t>Third, for each remaining collision, find empty spaces. 
+Using the loser C, for each empty space, if the empty space S intersects an inZone Z of the C.Per, shrink C up to Min(size of empty space, size of collision overlap), then FillEmptyWithInsuffZ(S, Z).
+Using the winner C, do the same.</t>
+  </si>
+  <si>
+    <t>Fourth, check if any collisions still exist. Assume that these collisions cannot be redistributed and will be handled with shrinks.</t>
+  </si>
+  <si>
+    <t>Second, for each remaining inside collision, split.</t>
+  </si>
+  <si>
+    <t>Redistribution Collisions</t>
+  </si>
+  <si>
+    <t>Redistributions.</t>
+  </si>
+  <si>
+    <t>If a Per has remaining &gt; 0, mark all of its CalObjs as Insufficient. If there are still collisions, mark them as Conflict. If there are any CalObjs that cross a zone boundary by more than MinDur, split it. Make sure states are correct: If a CalObj marked Unscheduled is within a proper InclusionZone, mark it correctly. If any CalObj not marked Unscheduled is outside of a proper InclusionZone, mark it Unscheduled. Delete cancels. Merge unnecessary splits.</t>
   </si>
 </sst>
 </file>
@@ -2259,7 +2247,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="121">
+  <dxfs count="105">
     <dxf>
       <fill>
         <patternFill>
@@ -2591,314 +2579,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC0CB"/>
-          <bgColor rgb="FFFFC0CB"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC0CB"/>
-          <bgColor rgb="FFFFC0CB"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -3144,6 +2824,192 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -3888,15 +3754,15 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="4" xr9:uid="{5F0E2908-E7EC-43FB-9BBB-CB014E9A6F67}">
-      <tableStyleElement type="wholeTable" dxfId="120"/>
-      <tableStyleElement type="headerRow" dxfId="119"/>
-      <tableStyleElement type="firstColumn" dxfId="118"/>
+      <tableStyleElement type="wholeTable" dxfId="104"/>
+      <tableStyleElement type="headerRow" dxfId="103"/>
+      <tableStyleElement type="firstColumn" dxfId="102"/>
       <tableStyleElement type="firstRowStripe" size="2"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="3" xr9:uid="{A53ADC7C-9332-4916-9ACB-0EFC07D28AC6}">
-      <tableStyleElement type="wholeTable" dxfId="117"/>
-      <tableStyleElement type="headerRow" dxfId="116"/>
-      <tableStyleElement type="secondRowStripe" dxfId="115"/>
+      <tableStyleElement type="wholeTable" dxfId="101"/>
+      <tableStyleElement type="headerRow" dxfId="100"/>
+      <tableStyleElement type="secondRowStripe" dxfId="99"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3928,70 +3794,70 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:C194" totalsRowShown="0">
   <autoFilter ref="A1:C194" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="98"/>
     <tableColumn id="6" xr3:uid="{1FFE88A6-F499-42FB-A3F4-F5BDCD9D0CF0}" name="Done"/>
-    <tableColumn id="5" xr3:uid="{65384592-5F41-4A06-A57C-FE71C87B4BDD}" name="Notes" dataDxfId="113"/>
+    <tableColumn id="5" xr3:uid="{65384592-5F41-4A06-A57C-FE71C87B4BDD}" name="Notes" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E4DD08F2-9CC2-46CC-93EE-E01A4DBC8EEE}" name="Table5" displayName="Table5" ref="A1:H8" totalsRowShown="0" headerRowDxfId="112" dataDxfId="110" headerRowBorderDxfId="111" tableBorderDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E4DD08F2-9CC2-46CC-93EE-E01A4DBC8EEE}" name="Table5" displayName="Table5" ref="A1:H8" totalsRowShown="0" headerRowDxfId="96" dataDxfId="94" headerRowBorderDxfId="95" tableBorderDxfId="93">
   <autoFilter ref="A1:H8" xr:uid="{9EF71295-67E3-4AA7-981B-99814F9C00D6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5F56F396-ECBF-4022-A747-BB6579150BC5}" name="Previous" dataDxfId="108"/>
-    <tableColumn id="2" xr3:uid="{52DF5424-7715-4094-9055-254252166B84}" name="CI Start_x000a_in Z" dataDxfId="107"/>
-    <tableColumn id="3" xr3:uid="{4BF25F2B-3788-4EC0-877F-738CFB7416BD}" name="CI End_x000a_in Z" dataDxfId="106"/>
-    <tableColumn id="4" xr3:uid="{3D1264CD-7DED-47FE-9A26-02FAA9BC34AE}" name="CI Start_x000a_out Z" dataDxfId="105"/>
-    <tableColumn id="5" xr3:uid="{91478E3E-F2EC-42B9-9CAC-61EA2AD657CB}" name="CI End_x000a_out Z" dataDxfId="104"/>
-    <tableColumn id="6" xr3:uid="{BD45968E-F796-4835-9D67-3627C99D24EC}" name="Z Start" dataDxfId="103"/>
-    <tableColumn id="7" xr3:uid="{3B4EE896-0831-43E7-8AE0-49A3476BEA97}" name="Z End" dataDxfId="102"/>
-    <tableColumn id="8" xr3:uid="{D4DAA8AA-8B7A-4978-8C26-61D2C9036856}" name="P End" dataDxfId="101"/>
+    <tableColumn id="1" xr3:uid="{5F56F396-ECBF-4022-A747-BB6579150BC5}" name="Previous" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{52DF5424-7715-4094-9055-254252166B84}" name="CI Start_x000a_in Z" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{4BF25F2B-3788-4EC0-877F-738CFB7416BD}" name="CI End_x000a_in Z" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{3D1264CD-7DED-47FE-9A26-02FAA9BC34AE}" name="CI Start_x000a_out Z" dataDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{91478E3E-F2EC-42B9-9CAC-61EA2AD657CB}" name="CI End_x000a_out Z" dataDxfId="88"/>
+    <tableColumn id="6" xr3:uid="{BD45968E-F796-4835-9D67-3627C99D24EC}" name="Z Start" dataDxfId="87"/>
+    <tableColumn id="7" xr3:uid="{3B4EE896-0831-43E7-8AE0-49A3476BEA97}" name="Z End" dataDxfId="86"/>
+    <tableColumn id="8" xr3:uid="{D4DAA8AA-8B7A-4978-8C26-61D2C9036856}" name="P End" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC6FE9AE-35E3-4705-A142-315DB9D43B3A}" name="Table3" displayName="Table3" ref="A1:A119" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
-  <autoFilter ref="A1:A119" xr:uid="{A2F7B623-DE53-4896-BDD6-CCC38D4467C3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC6FE9AE-35E3-4705-A142-315DB9D43B3A}" name="Table3" displayName="Table3" ref="A1:A120" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83">
+  <autoFilter ref="A1:A120" xr:uid="{A2F7B623-DE53-4896-BDD6-CCC38D4467C3}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0C8999A5-1CD8-483C-A3BB-7AD00E0E2478}" name="Collision Theory" dataDxfId="98"/>
+    <tableColumn id="1" xr3:uid="{0C8999A5-1CD8-483C-A3BB-7AD00E0E2478}" name="Collision Theory" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BEABA309-E652-49AF-B0CA-0DBB8732C3D3}" name="Table6" displayName="Table6" ref="A7:H11" totalsRowShown="0" headerRowDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BEABA309-E652-49AF-B0CA-0DBB8732C3D3}" name="Table6" displayName="Table6" ref="A7:H11" totalsRowShown="0" headerRowDxfId="81">
   <autoFilter ref="A7:H11" xr:uid="{3AB9159B-B403-4CC8-8649-2A74831EFA39}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{72C9A77E-AFBC-404B-A7F6-E681135EDAE9}" name="Redistribute_x000a_Collision_x000a_… T C1 ∩ C2 T …" dataDxfId="96"/>
-    <tableColumn id="2" xr3:uid="{7B5E19F2-C874-4B16-82C8-FA89018E0F3A}" name="C2HasRoom=T_x000a_LP &gt;= RP_x000a_" dataDxfId="95"/>
-    <tableColumn id="3" xr3:uid="{E21AAA4F-92B4-436C-B55B-4DFD07C4BE29}" name="C2HasRoom=T_x000a_LP &lt; RP_x000a_" dataDxfId="94"/>
-    <tableColumn id="4" xr3:uid="{833A1012-7AE2-431D-82C0-B7CB5960C752}" name="C2HasRoom=F_x000a_LP &gt;= RP_x000a_C2 &gt; RP" dataDxfId="93"/>
-    <tableColumn id="9" xr3:uid="{43D8BEE4-A2A2-4CFF-9608-9E5B08D746D9}" name="C2HasRoom=F_x000a_LP &gt;= RP_x000a_C2 == RP" dataDxfId="92"/>
-    <tableColumn id="5" xr3:uid="{0599BB19-BD4F-4332-92DE-B1E045C56EEF}" name="C2HasRoom=F_x000a_LP &lt; RP_x000a_C2 &gt; RP" dataDxfId="91"/>
-    <tableColumn id="10" xr3:uid="{3C3A9FF5-1451-4E38-87EA-C000A51EC5B5}" name="C2HasRoom=F_x000a_LP &lt; RP_x000a_C2 == RP" dataDxfId="90"/>
-    <tableColumn id="6" xr3:uid="{D413EC93-83CF-4773-9080-8AB9148DFA4E}" name="C2S🔒" dataDxfId="89"/>
+    <tableColumn id="1" xr3:uid="{72C9A77E-AFBC-404B-A7F6-E681135EDAE9}" name="Redistribute_x000a_Collision_x000a_… T C1 ∩ C2 T …" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{7B5E19F2-C874-4B16-82C8-FA89018E0F3A}" name="C2HasRoom=T_x000a_LP &gt;= RP_x000a_" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{E21AAA4F-92B4-436C-B55B-4DFD07C4BE29}" name="C2HasRoom=T_x000a_LP &lt; RP_x000a_" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{833A1012-7AE2-431D-82C0-B7CB5960C752}" name="C2HasRoom=F_x000a_LP &gt;= RP_x000a_C2 &gt; RP" dataDxfId="77"/>
+    <tableColumn id="9" xr3:uid="{43D8BEE4-A2A2-4CFF-9608-9E5B08D746D9}" name="C2HasRoom=F_x000a_LP &gt;= RP_x000a_C2 == RP" dataDxfId="76"/>
+    <tableColumn id="5" xr3:uid="{0599BB19-BD4F-4332-92DE-B1E045C56EEF}" name="C2HasRoom=F_x000a_LP &lt; RP_x000a_C2 &gt; RP" dataDxfId="75"/>
+    <tableColumn id="10" xr3:uid="{3C3A9FF5-1451-4E38-87EA-C000A51EC5B5}" name="C2HasRoom=F_x000a_LP &lt; RP_x000a_C2 == RP" dataDxfId="74"/>
+    <tableColumn id="6" xr3:uid="{D413EC93-83CF-4773-9080-8AB9148DFA4E}" name="C2S🔒" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{93CBC134-27AD-41AE-8603-BC9BCEAA8F11}" name="Table610" displayName="Table610" ref="A1:H5" totalsRowShown="0" headerRowDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{93CBC134-27AD-41AE-8603-BC9BCEAA8F11}" name="Table610" displayName="Table610" ref="A1:H5" totalsRowShown="0" headerRowDxfId="72">
   <autoFilter ref="A1:H5" xr:uid="{DBDA7C3F-B912-41A0-8E32-1B45D5F55BB3}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{73FF1CDD-C19A-439F-8319-FB0B0F2A6AC4}" name="Collision_x000a_… T C1 ∩ C2 T …" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{96F560A4-2F02-47CF-935D-415FDA638BA8}" name="C2HasRoom=T_x000a_LP &gt;= RP_x000a_" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{68C7390F-DF17-4355-86A4-16178BDC1B7B}" name="C2HasRoom=T_x000a_LP &lt; RP_x000a_" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{3BF403DF-AE49-422C-9F91-3F1A4275E2C9}" name="C2HasRoom=F_x000a_LP &gt;= RP_x000a_C2 &gt; RP" dataDxfId="63"/>
-    <tableColumn id="9" xr3:uid="{654E46D7-CC87-4CF2-84C4-42D91264DFCD}" name="C2HasRoom=F_x000a_LP &gt;= RP_x000a_C2 == RP" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{3DFA7DD4-A524-4469-BADE-AA83A3E28227}" name="C2HasRoom=F_x000a_LP &lt; RP_x000a_C2 &gt; RP" dataDxfId="61"/>
-    <tableColumn id="10" xr3:uid="{548A8B9B-722F-40BF-AB00-09CF12109AE0}" name="C2HasRoom=F_x000a_LP &lt; RP_x000a_C2 == RP" dataDxfId="60"/>
-    <tableColumn id="6" xr3:uid="{C8A545C6-8C4A-48A6-BD97-5899CBD70A11}" name="C2S🔒" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{73FF1CDD-C19A-439F-8319-FB0B0F2A6AC4}" name="Collision_x000a_… T C1 ∩ C2 T …" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{96F560A4-2F02-47CF-935D-415FDA638BA8}" name="C2HasRoom=T_x000a_LP &gt;= RP_x000a_" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{68C7390F-DF17-4355-86A4-16178BDC1B7B}" name="C2HasRoom=T_x000a_LP &lt; RP_x000a_" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{3BF403DF-AE49-422C-9F91-3F1A4275E2C9}" name="C2HasRoom=F_x000a_LP &gt;= RP_x000a_C2 &gt; RP" dataDxfId="68"/>
+    <tableColumn id="9" xr3:uid="{654E46D7-CC87-4CF2-84C4-42D91264DFCD}" name="C2HasRoom=F_x000a_LP &gt;= RP_x000a_C2 == RP" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{3DFA7DD4-A524-4469-BADE-AA83A3E28227}" name="C2HasRoom=F_x000a_LP &lt; RP_x000a_C2 &gt; RP" dataDxfId="66"/>
+    <tableColumn id="10" xr3:uid="{548A8B9B-722F-40BF-AB00-09CF12109AE0}" name="C2HasRoom=F_x000a_LP &lt; RP_x000a_C2 == RP" dataDxfId="65"/>
+    <tableColumn id="6" xr3:uid="{C8A545C6-8C4A-48A6-BD97-5899CBD70A11}" name="C2S🔒" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4013,34 +3879,34 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5CD4512-FB3C-4A60-9915-D17031B620E4}" name="Table63" displayName="Table63" ref="A1:H5" totalsRowShown="0" headerRowDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5CD4512-FB3C-4A60-9915-D17031B620E4}" name="Table63" displayName="Table63" ref="A1:H5" totalsRowShown="0" headerRowDxfId="63">
   <autoFilter ref="A1:H5" xr:uid="{19B6DDA4-9078-416B-AE59-743686D136CE}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8519F6B4-4AD2-4A90-910C-D5232E6BE34E}" name="Collision_x000a_C3 T C1 ∩ C2 T C4" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{7C59C76A-7FA5-41EC-AEEE-18F0E9292626}" name="C2HasRoom=T_x000a_LP &gt;= RP_x000a_" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{760F1A2B-39F4-4ED6-9AE0-5191303AFB37}" name="C2HasRoom=T_x000a_LP &lt; RP_x000a_" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{C038BC97-3885-4614-9CDB-DAEA1A258BEC}" name="C2HasRoom=F_x000a_LP &gt;= RP_x000a_C2 &gt; RP" dataDxfId="84"/>
-    <tableColumn id="9" xr3:uid="{18E1D4B5-6B11-4BB8-BEB6-D59F6614CC81}" name="C2HasRoom=F_x000a_LP &gt;= RP_x000a_C2 == RP" dataDxfId="83"/>
-    <tableColumn id="5" xr3:uid="{7096584B-D49B-4FE2-8597-B519F84AEAD2}" name="C2HasRoom=F_x000a_LP &lt; RP_x000a_C2 &gt; RP" dataDxfId="82"/>
-    <tableColumn id="10" xr3:uid="{67BCF0D7-6B24-4EFA-8008-A5D48711999E}" name="C2HasRoom=F_x000a_LP &lt; RP_x000a_C2 == RP" dataDxfId="81"/>
-    <tableColumn id="6" xr3:uid="{34320458-CD37-4DF6-8FE5-68E4F84BBEA8}" name="C2S🔒" dataDxfId="80"/>
+    <tableColumn id="1" xr3:uid="{8519F6B4-4AD2-4A90-910C-D5232E6BE34E}" name="Collision_x000a_C3 T C1 ∩ C2 T C4" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{7C59C76A-7FA5-41EC-AEEE-18F0E9292626}" name="C2HasRoom=T_x000a_LP &gt;= RP_x000a_" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{760F1A2B-39F4-4ED6-9AE0-5191303AFB37}" name="C2HasRoom=T_x000a_LP &lt; RP_x000a_" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{C038BC97-3885-4614-9CDB-DAEA1A258BEC}" name="C2HasRoom=F_x000a_LP &gt;= RP_x000a_C2 &gt; RP" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{18E1D4B5-6B11-4BB8-BEB6-D59F6614CC81}" name="C2HasRoom=F_x000a_LP &gt;= RP_x000a_C2 == RP" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{7096584B-D49B-4FE2-8597-B519F84AEAD2}" name="C2HasRoom=F_x000a_LP &lt; RP_x000a_C2 &gt; RP" dataDxfId="57"/>
+    <tableColumn id="10" xr3:uid="{67BCF0D7-6B24-4EFA-8008-A5D48711999E}" name="C2HasRoom=F_x000a_LP &lt; RP_x000a_C2 == RP" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{34320458-CD37-4DF6-8FE5-68E4F84BBEA8}" name="C2S🔒" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A637EB4D-B0BD-451A-AEF8-4F572CDAEA03}" name="Table7" displayName="Table7" ref="A1:H5" totalsRowShown="0" headerRowDxfId="79" dataDxfId="77" headerRowBorderDxfId="78" tableBorderDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A637EB4D-B0BD-451A-AEF8-4F572CDAEA03}" name="Table7" displayName="Table7" ref="A1:H5" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51">
   <autoFilter ref="A1:H5" xr:uid="{1C355147-87D4-4562-8BCA-2AC6E8731BE0}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{2D2C5C32-B8C1-434D-9678-8FA28AA9E25E}" name="C1 ∩ C2" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{83D2755C-6BC6-444B-B47B-E805256587D2}" name="C2HasRoom = T_x000a_C1 &gt;= C2" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{1CE782A0-B082-4A0B-9C40-AF715F441CC4}" name="C2HasRoom = T_x000a_C1 &lt; C2" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{BD5AA1DC-AE84-47FC-9B2A-54FD9FA153CE}" name="C2HasRoom = F_x000a_C2CanReDist = T_x000a_C1 &gt;= C2" dataDxfId="72"/>
-    <tableColumn id="5" xr3:uid="{BB1432BE-D946-4CB6-B3F6-04E8F22BC33F}" name="C2HasRoom = F_x000a_C2CanReDist = T_x000a_C1 &lt; C2" dataDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{69EA148B-29D0-4FD1-8924-7228DCD5168D}" name="C2HasRoom = F_x000a_C2CanReDist = F_x000a_C1 &gt;= C2" dataDxfId="70"/>
-    <tableColumn id="7" xr3:uid="{5304745C-6EDF-461B-A5C3-75B5645DF5C0}" name="C2HasRoom = F_x000a_C2CanReDist = F_x000a_C1 &lt; C2" dataDxfId="69"/>
-    <tableColumn id="8" xr3:uid="{94277B06-039D-4427-8C01-ABF777E3ED15}" name="C2S🔒" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{2D2C5C32-B8C1-434D-9678-8FA28AA9E25E}" name="C1 ∩ C2" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{83D2755C-6BC6-444B-B47B-E805256587D2}" name="C2HasRoom = T_x000a_C1 &gt;= C2" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{1CE782A0-B082-4A0B-9C40-AF715F441CC4}" name="C2HasRoom = T_x000a_C1 &lt; C2" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{BD5AA1DC-AE84-47FC-9B2A-54FD9FA153CE}" name="C2HasRoom = F_x000a_C2CanReDist = T_x000a_C1 &gt;= C2" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{BB1432BE-D946-4CB6-B3F6-04E8F22BC33F}" name="C2HasRoom = F_x000a_C2CanReDist = T_x000a_C1 &lt; C2" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{69EA148B-29D0-4FD1-8924-7228DCD5168D}" name="C2HasRoom = F_x000a_C2CanReDist = F_x000a_C1 &gt;= C2" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{5304745C-6EDF-461B-A5C3-75B5645DF5C0}" name="C2HasRoom = F_x000a_C2CanReDist = F_x000a_C1 &lt; C2" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{94277B06-039D-4427-8C01-ABF777E3ED15}" name="C2S🔒" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4345,8 +4211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
   <dimension ref="A1:G194"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130:C130"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104:XFD104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4657,7 +4523,7 @@
         <v>23</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -5062,7 +4928,7 @@
     </row>
     <row r="73" spans="1:3" s="9" customFormat="1">
       <c r="A73" s="11" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>23</v>
@@ -5071,7 +4937,7 @@
     </row>
     <row r="74" spans="1:3" s="9" customFormat="1">
       <c r="A74" s="11" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>23</v>
@@ -5089,7 +4955,7 @@
     </row>
     <row r="76" spans="1:3" s="9" customFormat="1">
       <c r="A76" s="11" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>23</v>
@@ -5116,46 +4982,46 @@
     </row>
     <row r="79" spans="1:3" s="9" customFormat="1" ht="30">
       <c r="A79" s="11" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="13" customFormat="1">
       <c r="A80" s="11" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="81" spans="1:3" s="13" customFormat="1">
       <c r="A81" s="11" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="82" spans="1:3" s="13" customFormat="1">
       <c r="A82" s="11" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B82" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="13" customFormat="1">
@@ -5180,68 +5046,68 @@
     </row>
     <row r="85" spans="1:3" s="13" customFormat="1" ht="30">
       <c r="A85" s="11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="86" spans="1:3" s="13" customFormat="1" ht="45">
       <c r="A86" s="11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
     </row>
     <row r="87" spans="1:3" s="13" customFormat="1">
       <c r="A87" s="11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="88" spans="1:3" s="13" customFormat="1" ht="30">
       <c r="A88" s="11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
     </row>
     <row r="89" spans="1:3" s="13" customFormat="1" ht="30">
       <c r="A89" s="11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
     </row>
     <row r="90" spans="1:3" s="13" customFormat="1">
       <c r="A90" s="11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="91" spans="1:3" s="13" customFormat="1">
@@ -5252,84 +5118,84 @@
         <v>23</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
     </row>
     <row r="92" spans="1:3" s="13" customFormat="1">
       <c r="A92" s="11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
     </row>
     <row r="93" spans="1:3" s="13" customFormat="1" ht="60">
       <c r="A93" s="11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
     </row>
     <row r="94" spans="1:3" s="13" customFormat="1">
       <c r="A94" s="11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
     </row>
     <row r="95" spans="1:3" s="13" customFormat="1">
       <c r="A95" s="11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B95" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
     </row>
     <row r="96" spans="1:3" s="13" customFormat="1" ht="45">
       <c r="A96" s="11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B96" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
     </row>
     <row r="97" spans="1:3" s="13" customFormat="1">
       <c r="A97" s="11" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="B97" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
     </row>
     <row r="98" spans="1:3" s="13" customFormat="1" ht="150">
       <c r="A98" s="11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B98" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
     </row>
     <row r="99" spans="1:3" s="13" customFormat="1">
@@ -5340,12 +5206,12 @@
         <v>23</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
     </row>
     <row r="100" spans="1:3" s="13" customFormat="1">
       <c r="A100" s="11" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="B100" s="13" t="s">
         <v>23</v>
@@ -5360,328 +5226,330 @@
         <v>23</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" s="13" customFormat="1" ht="60">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" s="13" customFormat="1">
       <c r="A102" s="11" t="s">
-        <v>384</v>
+        <v>278</v>
+      </c>
+      <c r="B102" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>471</v>
+        <v>517</v>
       </c>
     </row>
     <row r="103" spans="1:3" s="13" customFormat="1">
       <c r="A103" s="11" t="s">
-        <v>386</v>
-      </c>
-      <c r="C103" s="12" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" s="13" customFormat="1">
+        <v>516</v>
+      </c>
+      <c r="B103" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C103" s="12"/>
+    </row>
+    <row r="104" spans="1:3" s="13" customFormat="1" ht="60">
       <c r="A104" s="11" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
     </row>
     <row r="105" spans="1:3" s="13" customFormat="1">
       <c r="A105" s="11" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
     </row>
     <row r="106" spans="1:3" s="13" customFormat="1">
       <c r="A106" s="11" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" s="13" customFormat="1" ht="30">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" s="13" customFormat="1">
       <c r="A107" s="11" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" s="13" customFormat="1" ht="30">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" s="13" customFormat="1">
       <c r="A108" s="11" t="s">
-        <v>121</v>
+        <v>377</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" s="13" customFormat="1" ht="60">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" s="13" customFormat="1" ht="30">
       <c r="A109" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="C109" s="12" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" s="13" customFormat="1" ht="60">
+      <c r="A110" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C109" s="12" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" s="13" customFormat="1">
-      <c r="A110" s="11" t="s">
-        <v>384</v>
-      </c>
       <c r="C110" s="12" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" s="13" customFormat="1" ht="30">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" s="13" customFormat="1">
       <c r="A111" s="11" t="s">
-        <v>472</v>
-      </c>
-      <c r="B111" s="13" t="s">
-        <v>23</v>
+        <v>377</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" s="13" customFormat="1">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" s="13" customFormat="1" ht="30">
       <c r="A112" s="11" t="s">
-        <v>410</v>
+        <v>465</v>
       </c>
       <c r="B112" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>437</v>
+        <v>469</v>
       </c>
     </row>
     <row r="113" spans="1:3" s="13" customFormat="1">
       <c r="A113" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="B113" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C113" s="12" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" s="13" customFormat="1">
+      <c r="A114" s="11" t="s">
         <v>211</v>
-      </c>
-      <c r="B113" s="3"/>
-      <c r="C113" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" s="13" customFormat="1" ht="30">
-      <c r="A114" s="11" t="s">
-        <v>439</v>
       </c>
       <c r="B114" s="3"/>
       <c r="C114" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" s="13" customFormat="1" ht="30">
+      <c r="A115" s="11" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" s="13" customFormat="1">
-      <c r="A115" s="11" t="s">
-        <v>438</v>
-      </c>
+      <c r="B115" s="3"/>
       <c r="C115" s="12" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" s="13" customFormat="1" ht="30">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" s="13" customFormat="1">
       <c r="A116" s="11" t="s">
-        <v>373</v>
+        <v>431</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" s="13" customFormat="1">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" s="13" customFormat="1" ht="30">
       <c r="A117" s="11" t="s">
-        <v>431</v>
-      </c>
-      <c r="B117" s="3"/>
+        <v>367</v>
+      </c>
       <c r="C117" s="12" t="s">
-        <v>102</v>
+        <v>368</v>
       </c>
     </row>
     <row r="118" spans="1:3" s="13" customFormat="1">
       <c r="A118" s="11" t="s">
-        <v>409</v>
-      </c>
-      <c r="C118" s="12"/>
-    </row>
-    <row r="119" spans="1:3" s="13" customFormat="1" ht="75">
+        <v>424</v>
+      </c>
+      <c r="B118" s="3"/>
+      <c r="C118" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" s="13" customFormat="1">
       <c r="A119" s="11" t="s">
-        <v>478</v>
-      </c>
-      <c r="C119" s="12" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" s="13" customFormat="1" ht="30">
+        <v>402</v>
+      </c>
+      <c r="C119" s="12"/>
+    </row>
+    <row r="120" spans="1:3" s="13" customFormat="1" ht="75">
       <c r="A120" s="11" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" s="13" customFormat="1" ht="60">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" s="13" customFormat="1" ht="30">
       <c r="A121" s="11" t="s">
-        <v>434</v>
+        <v>472</v>
       </c>
       <c r="C121" s="12" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" s="13" customFormat="1" ht="60">
+      <c r="A122" s="11" t="s">
+        <v>427</v>
+      </c>
+      <c r="C122" s="12" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="122" spans="1:3" s="13" customFormat="1">
-      <c r="A122" s="11" t="s">
+    <row r="123" spans="1:3" s="13" customFormat="1">
+      <c r="A123" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C122" s="12" t="s">
+      <c r="C123" s="12" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="123" spans="1:3" s="13" customFormat="1">
-      <c r="A123" s="66" t="s">
+    <row r="124" spans="1:3" s="13" customFormat="1">
+      <c r="A124" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="B123" s="9"/>
-      <c r="C123" s="10"/>
-    </row>
-    <row r="124" spans="1:3" s="13" customFormat="1" ht="30">
-      <c r="A124" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C124" s="12" t="s">
-        <v>52</v>
-      </c>
+      <c r="B124" s="9"/>
+      <c r="C124" s="10"/>
     </row>
     <row r="125" spans="1:3" s="13" customFormat="1" ht="30">
       <c r="A125" s="11" t="s">
-        <v>393</v>
-      </c>
-      <c r="B125" s="3"/>
+        <v>51</v>
+      </c>
       <c r="C125" s="12" t="s">
-        <v>392</v>
+        <v>52</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="30">
-      <c r="A126" s="2" t="s">
+      <c r="A126" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="C126" s="12" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="30">
+      <c r="A127" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C126" s="4" t="s">
+      <c r="C127" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="A127" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="B127" s="13"/>
-      <c r="C127" s="12"/>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B128" s="13"/>
+      <c r="C128" s="12"/>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="30">
-      <c r="A129" s="11" t="s">
-        <v>421</v>
-      </c>
-      <c r="C129" s="12" t="s">
-        <v>422</v>
-      </c>
-    </row>
     <row r="130" spans="1:3" ht="30">
-      <c r="A130" s="66" t="s">
+      <c r="A130" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="C130" s="12" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="30">
+      <c r="A131" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="B130" s="9"/>
-      <c r="C130" s="10" t="s">
+      <c r="B131" s="9"/>
+      <c r="C131" s="10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
-      <c r="A131" s="2" t="s">
+    <row r="132" spans="1:3">
+      <c r="A132" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C131" s="4" t="s">
+      <c r="C132" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="45">
-      <c r="A132" s="11" t="s">
+    <row r="133" spans="1:3" ht="45">
+      <c r="A133" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B132" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C132" s="12" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3">
-      <c r="A133" s="11" t="s">
-        <v>425</v>
-      </c>
       <c r="B133" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C133" s="12" t="s">
-        <v>196</v>
+        <v>405</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="11" t="s">
-        <v>407</v>
-      </c>
-      <c r="C134" s="12"/>
+        <v>418</v>
+      </c>
+      <c r="B134" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C134" s="12" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C135" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="A135" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="C135" s="12"/>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="2" t="s">
-        <v>6</v>
+        <v>90</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="30">
-      <c r="A138" s="11" t="s">
+    <row r="139" spans="1:3" ht="30">
+      <c r="A139" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C138" s="12" t="s">
+      <c r="C139" s="12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
-      <c r="A139" s="2" t="s">
+    <row r="140" spans="1:3">
+      <c r="A140" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
-      <c r="A140" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="B140" s="13"/>
-      <c r="C140" s="12" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="30">
+    <row r="141" spans="1:3">
       <c r="A141" s="11" t="s">
-        <v>278</v>
+        <v>358</v>
       </c>
       <c r="B141" s="13"/>
       <c r="C141" s="12" t="s">
-        <v>375</v>
+        <v>421</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="60">
@@ -5710,7 +5578,7 @@
         <v>151</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -5765,7 +5633,7 @@
         <v>121</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -5778,10 +5646,10 @@
     </row>
     <row r="155" spans="1:3" ht="45">
       <c r="A155" s="11" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="45">
@@ -5802,42 +5670,42 @@
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="11" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C158" s="12" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="90">
       <c r="A159" s="11" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C159" s="12" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="90">
       <c r="A160" s="11" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="C160" s="12" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="60">
       <c r="A161" s="11" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C161" s="12" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C162" s="12" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -5865,7 +5733,7 @@
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="11" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="C167" s="12"/>
     </row>
@@ -5942,7 +5810,7 @@
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="11" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -5972,7 +5840,7 @@
         <v>117</v>
       </c>
       <c r="C183" s="12" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -6007,7 +5875,7 @@
       </c>
       <c r="B187" s="13"/>
       <c r="C187" s="12" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -6046,24 +5914,24 @@
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="11" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="C192" s="12"/>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="11" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="11" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="C194" s="12" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -6091,13 +5959,13 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="192.85546875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="98.42578125" style="15" customWidth="1"/>
     <col min="12" max="12" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6125,7 +5993,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
         <v>222</v>
       </c>
@@ -6133,7 +6001,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
         <v>231</v>
       </c>
@@ -6141,7 +6009,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="23" customFormat="1">
+    <row r="6" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A6" t="s">
         <v>191</v>
       </c>
@@ -6149,7 +6017,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="23" customFormat="1">
+    <row r="7" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A7" s="23" t="s">
         <v>234</v>
       </c>
@@ -6181,7 +6049,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="11" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A11" t="s">
         <v>269</v>
       </c>
@@ -6189,7 +6057,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="45">
+    <row r="12" spans="1:12" ht="75">
       <c r="A12" t="s">
         <v>192</v>
       </c>
@@ -6197,20 +6065,20 @@
         <v>251</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="13" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A13" s="23" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="75">
       <c r="A14" t="s">
         <v>214</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>365</v>
+        <v>518</v>
       </c>
     </row>
     <row r="17" spans="2:2">
@@ -6233,22 +6101,22 @@
         <v>258</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="45">
+    <row r="21" spans="2:2" ht="90">
       <c r="B21" s="10" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="30">
+    <row r="22" spans="2:2" ht="60">
       <c r="B22" s="10" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="30">
+    <row r="23" spans="2:2" ht="45">
       <c r="B23" s="10" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="45">
+    <row r="24" spans="2:2" ht="75">
       <c r="B24" s="15" t="s">
         <v>263</v>
       </c>
@@ -6322,7 +6190,7 @@
         <v>159</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>177</v>
@@ -6474,47 +6342,47 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="29" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="29" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="B16" s="61" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="29" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="B17" s="64" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="29" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="B18" s="62" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="29" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="29" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="B20" s="67" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="29" customFormat="1"/>
@@ -6525,7 +6393,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="20" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -6535,33 +6403,33 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="20" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="20" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="20" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="20" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="20" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="20" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -6604,16 +6472,16 @@
         <v>268</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="D1" s="50" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="F1" s="50" t="s">
         <v>266</v>
@@ -6627,13 +6495,13 @@
     </row>
     <row r="2" spans="1:10" ht="75">
       <c r="A2" s="44" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>215</v>
@@ -6645,7 +6513,7 @@
         <v>215</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="H2" s="46" t="s">
         <v>215</v>
@@ -6655,13 +6523,13 @@
     </row>
     <row r="3" spans="1:10" ht="60">
       <c r="A3" s="45" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>215</v>
@@ -6683,7 +6551,7 @@
     </row>
     <row r="4" spans="1:10" ht="75">
       <c r="A4" s="45" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="B4" s="41" t="s">
         <v>215</v>
@@ -6692,26 +6560,26 @@
         <v>215</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>215</v>
       </c>
       <c r="H4" s="47" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:10" ht="60">
       <c r="A5" s="45" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="B5" s="41" t="s">
         <v>215</v>
@@ -6720,10 +6588,10 @@
         <v>215</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>215</v>
@@ -6742,10 +6610,10 @@
         <v>266</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>215</v>
@@ -6776,10 +6644,10 @@
         <v>215</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>215</v>
@@ -6804,10 +6672,10 @@
         <v>215</v>
       </c>
       <c r="D8" s="54" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="E8" s="54" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="F8" s="54" t="s">
         <v>215</v>
@@ -7070,10 +6938,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F77D648-B449-4B03-97EB-4834E79DA6CD}">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:A69"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7114,7 +6982,7 @@
       <c r="E3" s="43"/>
       <c r="F3" s="43"/>
     </row>
-    <row r="4" spans="1:6" s="12" customFormat="1">
+    <row r="4" spans="1:6" s="12" customFormat="1" ht="30">
       <c r="A4" s="27" t="s">
         <v>285</v>
       </c>
@@ -7134,7 +7002,7 @@
       <c r="E5" s="43"/>
       <c r="F5" s="43"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="27" t="s">
         <v>287</v>
       </c>
@@ -7144,7 +7012,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="30">
       <c r="A8" s="27" t="s">
         <v>289</v>
       </c>
@@ -7156,167 +7024,167 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="27" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="27" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30">
       <c r="A14" s="27" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="27" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="12" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="30">
       <c r="A17" s="27" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="30">
       <c r="A18" s="27" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="30">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="45">
       <c r="A19" s="27" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="30">
       <c r="A20" s="27" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="27" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="27" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="10" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="8" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="30">
       <c r="A26" s="27" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="27" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="90">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="105">
       <c r="A28" s="58" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="30">
       <c r="A29" s="12" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="27" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="27" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="12" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="58" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="58" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="58" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="165">
       <c r="A37" s="58" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="24" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="27" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="30">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="45">
       <c r="A41" s="27" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="30">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="45">
       <c r="A42" s="27" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="27" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="30">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="45">
       <c r="A44" s="27" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="27" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="27" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="8" customFormat="1">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="8" customFormat="1" ht="30">
       <c r="A50" s="8" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B50" s="60"/>
       <c r="C50" s="60"/>
@@ -7324,9 +7192,9 @@
       <c r="E50" s="60"/>
       <c r="F50" s="60"/>
     </row>
-    <row r="51" spans="1:6" s="8" customFormat="1" ht="30">
+    <row r="51" spans="1:6" s="8" customFormat="1" ht="45">
       <c r="A51" s="8" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B51" s="60"/>
       <c r="C51" s="60"/>
@@ -7334,7 +7202,7 @@
       <c r="E51" s="60"/>
       <c r="F51" s="60"/>
     </row>
-    <row r="52" spans="1:6" s="8" customFormat="1" ht="30">
+    <row r="52" spans="1:6" s="8" customFormat="1" ht="45">
       <c r="A52" s="8" t="s">
         <v>308</v>
       </c>
@@ -7346,7 +7214,7 @@
     </row>
     <row r="53" spans="1:6" s="8" customFormat="1">
       <c r="A53" s="8" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B53" s="60"/>
       <c r="C53" s="60"/>
@@ -7363,7 +7231,7 @@
     </row>
     <row r="55" spans="1:6" s="8" customFormat="1">
       <c r="A55" s="8" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B55" s="60"/>
       <c r="C55" s="60"/>
@@ -7373,7 +7241,7 @@
     </row>
     <row r="56" spans="1:6" s="8" customFormat="1">
       <c r="A56" s="8" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B56" s="60"/>
       <c r="C56" s="60"/>
@@ -7383,7 +7251,7 @@
     </row>
     <row r="57" spans="1:6" s="8" customFormat="1" ht="30">
       <c r="A57" s="8" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B57" s="60"/>
       <c r="C57" s="60"/>
@@ -7391,9 +7259,9 @@
       <c r="E57" s="60"/>
       <c r="F57" s="60"/>
     </row>
-    <row r="58" spans="1:6" s="8" customFormat="1">
+    <row r="58" spans="1:6" s="8" customFormat="1" ht="30">
       <c r="A58" s="8" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B58" s="60"/>
       <c r="C58" s="60"/>
@@ -7401,9 +7269,9 @@
       <c r="E58" s="60"/>
       <c r="F58" s="60"/>
     </row>
-    <row r="59" spans="1:6" s="8" customFormat="1" ht="45">
+    <row r="59" spans="1:6" s="8" customFormat="1" ht="75">
       <c r="A59" s="8" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B59" s="60"/>
       <c r="C59" s="60"/>
@@ -7413,68 +7281,63 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="27" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="90">
       <c r="A62" s="27" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="27" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="27" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="58" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="30">
+      <c r="A67" s="58" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="27" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="27" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="60">
-      <c r="A68" s="27" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" s="27" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" ht="30">
-      <c r="A73" s="10" t="s">
-        <v>310</v>
+    <row r="68" spans="1:1">
+      <c r="A68" s="58" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="60">
+      <c r="A69" s="58" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="58" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="10" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" ht="60">
-      <c r="A75" s="10" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" ht="30">
-      <c r="A76" s="10" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" ht="30">
-      <c r="A77" s="10" t="s">
-        <v>311</v>
-      </c>
+      <c r="A74" s="10"/>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="10"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="10"/>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="10"/>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7509,25 +7372,25 @@
   <sheetData>
     <row r="1" spans="1:8" s="23" customFormat="1" ht="45">
       <c r="A1" s="57" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
       <c r="B1" s="27" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="E1" s="27" t="s">
         <v>351</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>352</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>357</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>356</v>
-      </c>
       <c r="F1" s="27" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="H1" s="27" t="s">
         <v>291</v>
@@ -7535,80 +7398,80 @@
     </row>
     <row r="2" spans="1:8" s="23" customFormat="1">
       <c r="A2" s="59" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G2" s="46" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="H2" s="46" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="23" customFormat="1" ht="30">
       <c r="A3" s="59" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G3" s="47" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="H3" s="47" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="23" customFormat="1" ht="30">
       <c r="A4" s="59" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="H4" s="47" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="23" customFormat="1" ht="15.75" thickBot="1">
@@ -7616,22 +7479,22 @@
         <v>292</v>
       </c>
       <c r="B5" s="53" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F5" s="54" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G5" s="55" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="H5" s="55" t="s">
         <v>290</v>
@@ -7646,25 +7509,25 @@
     </row>
     <row r="7" spans="1:8" ht="45">
       <c r="A7" s="57" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
       <c r="B7" s="27" t="s">
+        <v>346</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="E7" s="27" t="s">
         <v>351</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>352</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>357</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>356</v>
-      </c>
       <c r="F7" s="27" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="H7" s="27" t="s">
         <v>291</v>
@@ -7672,80 +7535,80 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="59" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G8" s="46" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="H8" s="46" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
       <c r="A9" s="59" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G9" s="47" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="H9" s="47" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30">
       <c r="A10" s="59" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="G10" s="47" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="H10" s="47" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1">
@@ -7753,22 +7616,22 @@
         <v>292</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D11" s="54" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G11" s="55" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="H11" s="55" t="s">
         <v>290</v>
@@ -7859,36 +7722,36 @@
   <sheetData>
     <row r="1" spans="1:12" ht="45">
       <c r="A1" s="57" t="s">
+        <v>342</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="D1" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="E1" s="27" t="s">
         <v>351</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>352</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>357</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>356</v>
-      </c>
       <c r="F1" s="27" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="H1" s="27" t="s">
         <v>291</v>
       </c>
       <c r="L1" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="59" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="B2" s="40" t="s">
         <v>23</v>
@@ -7910,12 +7773,12 @@
       </c>
       <c r="H2" s="46"/>
       <c r="L2" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" s="59" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B3" s="41" t="s">
         <v>23</v>
@@ -7927,18 +7790,18 @@
         <v>23</v>
       </c>
       <c r="E3" s="68" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="47"/>
       <c r="H3" s="47"/>
       <c r="L3" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" s="59" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B4" s="41" t="s">
         <v>23</v>
@@ -7950,13 +7813,13 @@
         <v>23</v>
       </c>
       <c r="E4" s="68" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="47"/>
       <c r="H4" s="47"/>
       <c r="L4" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1">
@@ -7981,17 +7844,17 @@
       </c>
       <c r="H5" s="55"/>
       <c r="L5" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="L6" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="B13" s="27" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
@@ -7999,40 +7862,40 @@
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="B14" s="27" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="C14" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
     </row>
     <row r="19" spans="6:11">
       <c r="F19" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="G19" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="H19" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="I19" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="J19" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="K19" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
     </row>
     <row r="20" spans="6:11">
       <c r="F20" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="21" spans="6:11">
       <c r="F21" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="22" spans="6:11">
@@ -8096,7 +7959,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="45.75" thickBot="1">
       <c r="A1" s="48" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B1" s="49" t="s">
         <v>306</v>

</xml_diff>

<commit_message>
Most major bugs squashed
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24930" windowHeight="12330" tabRatio="753" firstSheet="1" activeTab="1" xr2:uid="{B08B66F6-8B10-48BD-8CBC-92B4F4D60D54}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24930" windowHeight="12330" tabRatio="753" firstSheet="1" activeTab="4" xr2:uid="{B08B66F6-8B10-48BD-8CBC-92B4F4D60D54}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="527">
   <si>
     <t>Feature</t>
   </si>
@@ -4034,8 +4034,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{23251552-5E98-4102-9DE7-0FF2B60CEB4B}" name="Table8" displayName="Table8" ref="F19:K22" totalsRowShown="0">
-  <autoFilter ref="F19:K22" xr:uid="{876B12BE-7000-4382-A947-7B6C125C4C06}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{23251552-5E98-4102-9DE7-0FF2B60CEB4B}" name="Table8" displayName="Table8" ref="C8:H11" totalsRowShown="0">
+  <autoFilter ref="C8:H11" xr:uid="{876B12BE-7000-4382-A947-7B6C125C4C06}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1E78DD40-652F-4A6D-975C-DCA817CDDF28}" name="Type"/>
     <tableColumn id="2" xr3:uid="{0F33217D-11DD-4A3C-8C27-ED6B87268CDF}" name="New"/>
@@ -5964,8 +5964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F160C7F-FB27-4F84-8171-6D9C64590D99}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6074,7 +6074,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45">
+    <row r="10" spans="1:3" ht="60">
       <c r="A10" s="69" t="s">
         <v>370</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="120">
+    <row r="14" spans="1:3" ht="135">
       <c r="A14" s="69" t="s">
         <v>370</v>
       </c>
@@ -6155,7 +6155,9 @@
       <c r="A17" s="69" t="s">
         <v>370</v>
       </c>
-      <c r="B17" s="71"/>
+      <c r="B17" s="71" t="s">
+        <v>23</v>
+      </c>
       <c r="C17" s="70" t="s">
         <v>454</v>
       </c>
@@ -6764,7 +6766,7 @@
   </sheetPr>
   <dimension ref="A1:J196"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -8022,10 +8024,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA241A8-6F93-400B-8E8B-D16ADE5AD9AC}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C7" sqref="C7:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8130,6 +8132,41 @@
         <v>390</v>
       </c>
     </row>
+    <row r="8" spans="1:12">
+      <c r="C8" t="s">
+        <v>382</v>
+      </c>
+      <c r="D8" t="s">
+        <v>386</v>
+      </c>
+      <c r="E8" t="s">
+        <v>387</v>
+      </c>
+      <c r="F8" t="s">
+        <v>383</v>
+      </c>
+      <c r="G8" t="s">
+        <v>384</v>
+      </c>
+      <c r="H8" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="C9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="C10" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="C11" t="s">
+        <v>161</v>
+      </c>
+    </row>
     <row r="13" spans="1:12" ht="30">
       <c r="B13" s="27" t="s">
         <v>452</v>
@@ -8138,41 +8175,6 @@
     <row r="14" spans="1:12" ht="30">
       <c r="B14" s="27" t="s">
         <v>453</v>
-      </c>
-    </row>
-    <row r="19" spans="6:11">
-      <c r="F19" t="s">
-        <v>382</v>
-      </c>
-      <c r="G19" t="s">
-        <v>386</v>
-      </c>
-      <c r="H19" t="s">
-        <v>387</v>
-      </c>
-      <c r="I19" t="s">
-        <v>383</v>
-      </c>
-      <c r="J19" t="s">
-        <v>384</v>
-      </c>
-      <c r="K19" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="20" spans="6:11">
-      <c r="F20" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="21" spans="6:11">
-      <c r="F21" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="22" spans="6:11">
-      <c r="F22" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Probably no more collision bugs
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -9,20 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24930" windowHeight="12330" tabRatio="775" activeTab="2" xr2:uid="{B08B66F6-8B10-48BD-8CBC-92B4F4D60D54}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24930" windowHeight="12330" tabRatio="775" xr2:uid="{B08B66F6-8B10-48BD-8CBC-92B4F4D60D54}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="1" r:id="rId1"/>
     <sheet name="Bugs" sheetId="13" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="17" r:id="rId3"/>
-    <sheet name="Redistributions" sheetId="9" r:id="rId4"/>
-    <sheet name="Calendar Passes" sheetId="5" r:id="rId5"/>
-    <sheet name="Collisions" sheetId="7" r:id="rId6"/>
-    <sheet name="Collisions2" sheetId="11" r:id="rId7"/>
-    <sheet name="CheckIns" sheetId="6" r:id="rId8"/>
-    <sheet name="States" sheetId="4" r:id="rId9"/>
-    <sheet name="Colors" sheetId="15" r:id="rId10"/>
-    <sheet name="Thoughts" sheetId="3" r:id="rId11"/>
+    <sheet name="Redistributions" sheetId="9" r:id="rId3"/>
+    <sheet name="Calendar Passes" sheetId="5" r:id="rId4"/>
+    <sheet name="Collisions" sheetId="7" r:id="rId5"/>
+    <sheet name="Collisions2" sheetId="11" r:id="rId6"/>
+    <sheet name="CheckIns" sheetId="6" r:id="rId7"/>
+    <sheet name="States" sheetId="4" r:id="rId8"/>
+    <sheet name="Colors" sheetId="15" r:id="rId9"/>
+    <sheet name="Thoughts" sheetId="3" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="556">
   <si>
     <t>Feature</t>
   </si>
@@ -1750,127 +1749,7 @@
     <t>Debug mode</t>
   </si>
   <si>
-    <t>LData</t>
-  </si>
-  <si>
-    <t>{Left 🔒 WC[Sleep] CanReDist}</t>
-  </si>
-  <si>
-    <t>Left</t>
-  </si>
-  <si>
-    <t>{TimekeeperWPF P200 18-1-9 S4:00 PM E7:00 PM ZS7:00 AM ZE12:00 AM}</t>
-  </si>
-  <si>
-    <t>Loser</t>
-  </si>
-  <si>
-    <t>{TimekeeperWPF P200 18-1-9 S5:15 PM E8:00 PM ZS7:00 AM ZE12:00 AM}</t>
-  </si>
-  <si>
-    <t>Overlap</t>
-  </si>
-  <si>
-    <t>{01:45:00}</t>
-  </si>
-  <si>
-    <t>RData</t>
-  </si>
-  <si>
-    <t>{Right 🔒 WC[Freetime] CanReDist}</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Right</t>
-  </si>
-  <si>
-    <t>Winner</t>
-  </si>
-  <si>
-    <t>cell</t>
-  </si>
-  <si>
-    <t>D34567</t>
-  </si>
-  <si>
-    <t>{Left  WC[Dinner] CanReDist}</t>
-  </si>
-  <si>
-    <t>{Dinner P250 18-1-9 S7:00 PM E8:00 PM ZS6:00 PM ZE8:00 PM}</t>
-  </si>
-  <si>
-    <t>{TimekeeperWPF P200 18-1-9 S7:00 PM E9:45 PM ZS7:00 AM ZE12:00 AM}</t>
-  </si>
-  <si>
-    <t>{01:00:00}</t>
-  </si>
-  <si>
-    <t>{Right  WC[TimekeeperWPF] CanReDist}</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>{TimekeeperWPF P200 18-1-9 S8:00 PM E10:45 PM ZS7:00 AM ZE12:00 AM}</t>
-  </si>
-  <si>
-    <t>{02:45:00}</t>
-  </si>
-  <si>
-    <t>{Freetime P100 18-1-9 S8:00 PM E12:00 AM ZS7:00 AM ZE12:00 AM}</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
     <t>infinite loop Step1Push. This is a ping pong effect where three objects that are tangent are playing hot potato with a 4th.</t>
-  </si>
-  <si>
-    <t>collision.Left.LeftTangent.LeftTangent.LeftTangent</t>
-  </si>
-  <si>
-    <t>{TimekeeperWPF P200 18-1-9 S2:00 PM E2:30 PM ZS7:00 AM ZE12:00 AM}</t>
-  </si>
-  <si>
-    <t>collision.Left.LeftTangent.LeftTangent</t>
-  </si>
-  <si>
-    <t>{Lunch P250 18-1-9 S2:30 PM E3:00 PM ZS1:00 PM ZE3:00 PM}</t>
-  </si>
-  <si>
-    <t>collision.Left.LeftTangent</t>
-  </si>
-  <si>
-    <t>{ASP.NET P199 18-1-9 S3:00 PM E4:00 PM ZS7:00 AM ZE12:00 AM}</t>
-  </si>
-  <si>
-    <t>collision.Left</t>
-  </si>
-  <si>
-    <t>collision.Right.LeftTangent</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>collision.Left.RightTangent</t>
-  </si>
-  <si>
-    <t>collision.Right</t>
-  </si>
-  <si>
-    <t>collision.Right.RightTangent</t>
-  </si>
-  <si>
-    <t>collision.Right.RightTangent.RightTangent</t>
-  </si>
-  <si>
-    <t>loser</t>
-  </si>
-  <si>
-    <t>winner</t>
   </si>
   <si>
     <t>C2.LT
@@ -1915,6 +1794,35 @@
   <si>
     <t>C1.LT null
 C1.RT null</t>
+  </si>
+  <si>
+    <t>Deadlines</t>
+  </si>
+  <si>
+    <t>New allocation: x before deadline</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">infinite loop Step1Push. Ping ponging between many objects. It seems to be because ReDist isn't handled in Step1 and we're assuming a ReDist-push leads to a ReDist, but at the same time the ReDist-push causes yet another push which cancels out the ReDist-push… 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ignore flag is needed</t>
+    </r>
+  </si>
+  <si>
+    <t>Redistributions should try to overwrite lower priority objects if possible. Include in the "empty spaces" any areas that are occupied by lower priority objects.</t>
+  </si>
+  <si>
+    <t>TimeTask.CanReDist</t>
   </si>
 </sst>
 </file>
@@ -2500,7 +2408,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2714,12 +2622,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2736,6 +2638,67 @@
   </cellStyles>
   <dxfs count="100">
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
@@ -2917,20 +2880,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -2958,31 +2907,267 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3030,283 +3215,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -4259,9 +4167,114 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>933724</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19337</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Screen Clipping">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DED45B8A-12F9-4188-B292-A09F6824925A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="85725" y="3876675"/>
+          <a:ext cx="1962424" cy="2057687"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>981075</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1038528</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>57446</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="Screen Clipping">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91768064-82A1-466F-B3F4-29E88C88A3E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2095500" y="3848100"/>
+          <a:ext cx="2172003" cy="2124371"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:C174" totalsRowShown="0">
-  <autoFilter ref="A1:C174" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:C177" totalsRowShown="0">
+  <autoFilter ref="A1:C177" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="93"/>
     <tableColumn id="6" xr3:uid="{1FFE88A6-F499-42FB-A3F4-F5BDCD9D0CF0}" name="Done"/>
@@ -4272,8 +4285,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F572A93C-B296-47BB-A2B7-E8D930E92020}" name="Table4" displayName="Table4" ref="A1:C50" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90" tableBorderDxfId="89">
-  <autoFilter ref="A1:C50" xr:uid="{5B5CE518-BB75-408C-8F1B-EE90C29E48F3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F572A93C-B296-47BB-A2B7-E8D930E92020}" name="Table4" displayName="Table4" ref="A1:C51" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90" tableBorderDxfId="89">
+  <autoFilter ref="A1:C51" xr:uid="{5B5CE518-BB75-408C-8F1B-EE90C29E48F3}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{2EF2C0F2-7D81-49C3-B8A7-E25CCB336A17}" name="Column1" dataDxfId="88"/>
     <tableColumn id="2" xr3:uid="{FCC47FF7-6739-4E5E-9E09-E5EAD7161467}" name="Column2" dataDxfId="87"/>
@@ -4332,45 +4345,45 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67135CB1-5074-4EBE-BD9A-48C30A4CB81B}" name="Table2" displayName="Table2" ref="A7:E11" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67135CB1-5074-4EBE-BD9A-48C30A4CB81B}" name="Table2" displayName="Table2" ref="A7:E11" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
   <autoFilter ref="A7:E11" xr:uid="{B388395A-7532-4521-958E-47A4C8955AF2}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{70C2C4E6-CAF6-425B-8E04-929D489EC9D7}" name="Determine L, R_x000a_if C1.S == C2.S" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{2FE5E346-C794-4C60-92C1-0865C7DF44B2}" name="C2.LT_x000a_C2.RT" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{D05D7189-86A2-4E66-978C-200C858C620C}" name="C2.LT null_x000a_C2.RT" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{9D36A042-6482-4DEE-A827-BCFC97E3E6B9}" name="C2.LT_x000a_C2.RT null" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{DCA50F46-3DCF-4728-AFF9-64F17E91077A}" name="C2.LT null_x000a_C2.RT null" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{70C2C4E6-CAF6-425B-8E04-929D489EC9D7}" name="Determine L, R_x000a_if C1.S == C2.S" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{2FE5E346-C794-4C60-92C1-0865C7DF44B2}" name="C2.LT_x000a_C2.RT" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{D05D7189-86A2-4E66-978C-200C858C620C}" name="C2.LT null_x000a_C2.RT" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{9D36A042-6482-4DEE-A827-BCFC97E3E6B9}" name="C2.LT_x000a_C2.RT null" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{DCA50F46-3DCF-4728-AFF9-64F17E91077A}" name="C2.LT null_x000a_C2.RT null" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E4DD08F2-9CC2-46CC-93EE-E01A4DBC8EEE}" name="Table5" displayName="Table5" ref="A1:H8" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E4DD08F2-9CC2-46CC-93EE-E01A4DBC8EEE}" name="Table5" displayName="Table5" ref="A1:H8" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48">
   <autoFilter ref="A1:H8" xr:uid="{9EF71295-67E3-4AA7-981B-99814F9C00D6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5F56F396-ECBF-4022-A747-BB6579150BC5}" name="Previous" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{52DF5424-7715-4094-9055-254252166B84}" name="CI Start_x000a_in Z" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{4BF25F2B-3788-4EC0-877F-738CFB7416BD}" name="CI End_x000a_in Z" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{3D1264CD-7DED-47FE-9A26-02FAA9BC34AE}" name="CI Start_x000a_out Z" dataDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{91478E3E-F2EC-42B9-9CAC-61EA2AD657CB}" name="CI End_x000a_out Z" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{BD45968E-F796-4835-9D67-3627C99D24EC}" name="Z Start" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{3B4EE896-0831-43E7-8AE0-49A3476BEA97}" name="Z End" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{D4DAA8AA-8B7A-4978-8C26-61D2C9036856}" name="P End" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{5F56F396-ECBF-4022-A747-BB6579150BC5}" name="Previous" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{52DF5424-7715-4094-9055-254252166B84}" name="CI Start_x000a_in Z" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{4BF25F2B-3788-4EC0-877F-738CFB7416BD}" name="CI End_x000a_in Z" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{3D1264CD-7DED-47FE-9A26-02FAA9BC34AE}" name="CI Start_x000a_out Z" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{91478E3E-F2EC-42B9-9CAC-61EA2AD657CB}" name="CI End_x000a_out Z" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{BD45968E-F796-4835-9D67-3627C99D24EC}" name="Z Start" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{3B4EE896-0831-43E7-8AE0-49A3476BEA97}" name="Z End" dataDxfId="41"/>
+    <tableColumn id="8" xr3:uid="{D4DAA8AA-8B7A-4978-8C26-61D2C9036856}" name="P End" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2B1B7CE4-90F7-42CA-B974-855205A0C605}" name="Table11" displayName="Table11" ref="A2:E12" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2B1B7CE4-90F7-42CA-B974-855205A0C605}" name="Table11" displayName="Table11" ref="A2:E12" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A2:E12" xr:uid="{78FF5B0B-0912-499F-8F6A-339F3CEEC95F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F251C872-2A1D-42A0-994A-2DFC09D7C047}" name="State" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{F251C872-2A1D-42A0-994A-2DFC09D7C047}" name="State" dataDxfId="37"/>
     <tableColumn id="2" xr3:uid="{AB62CF60-B9F3-442C-A4D1-2FC89B02B851}" name="Border Color"/>
-    <tableColumn id="3" xr3:uid="{E3035B58-4720-4F96-BC43-0FE1566CB1AC}" name="Happens When" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{64A950F1-3FCD-413C-8376-9DAD13362BEC}" name="Details" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{6FB2B197-5E34-46A9-BA2C-CE95765F93BA}" name="Leads to" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{E3035B58-4720-4F96-BC43-0FE1566CB1AC}" name="Happens When" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{64A950F1-3FCD-413C-8376-9DAD13362BEC}" name="Details" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{6FB2B197-5E34-46A9-BA2C-CE95765F93BA}" name="Leads to" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4673,10 +4686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:G180"/>
+  <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5565,7 +5578,10 @@
     </row>
     <row r="90" spans="1:3" s="13" customFormat="1">
       <c r="A90" s="11" t="s">
-        <v>538</v>
+        <v>555</v>
+      </c>
+      <c r="B90" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="C90" s="12"/>
     </row>
@@ -5853,10 +5869,11 @@
       <c r="B125" s="3"/>
       <c r="C125" s="4"/>
     </row>
-    <row r="126" spans="1:3" ht="30">
+    <row r="126" spans="1:3" s="13" customFormat="1" ht="30">
       <c r="A126" s="11" t="s">
         <v>148</v>
       </c>
+      <c r="B126" s="3"/>
       <c r="C126" s="12" t="s">
         <v>150</v>
       </c>
@@ -5978,246 +5995,263 @@
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="11" t="s">
-        <v>97</v>
+        <v>551</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="11" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
-      <c r="A144" s="2" t="s">
+    <row r="146" spans="1:3">
+      <c r="A146" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
-      <c r="A145" s="2" t="s">
+    <row r="147" spans="1:3">
+      <c r="A147" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C145" s="12" t="s">
+      <c r="C147" s="12" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="146" spans="1:3">
-      <c r="A146" s="11" t="s">
-        <v>372</v>
-      </c>
-      <c r="C146" s="12"/>
-    </row>
-    <row r="147" spans="1:3">
-      <c r="A147" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="C147" s="12"/>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="11" t="s">
-        <v>142</v>
+        <v>372</v>
       </c>
       <c r="C148" s="12"/>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C149" s="12"/>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C150" s="12"/>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C149" s="12"/>
-    </row>
-    <row r="150" spans="1:3" ht="45">
-      <c r="A150" s="11" t="s">
+      <c r="C151" s="12"/>
+    </row>
+    <row r="152" spans="1:3" ht="45">
+      <c r="A152" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B150" s="13"/>
-      <c r="C150" s="12" t="s">
+      <c r="B152" s="13"/>
+      <c r="C152" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="30">
-      <c r="A151" s="2" t="s">
+    <row r="153" spans="1:3" ht="30">
+      <c r="A153" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C151" s="4" t="s">
+      <c r="C153" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
-      <c r="A152" s="2" t="s">
+    <row r="154" spans="1:3">
+      <c r="A154" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C152" s="4" t="s">
+      <c r="C154" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
-      <c r="A153" s="63" t="s">
+    <row r="155" spans="1:3">
+      <c r="A155" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="B153" s="9"/>
-      <c r="C153" s="10" t="s">
+      <c r="B155" s="9"/>
+      <c r="C155" s="10" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3">
-      <c r="A154" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C154" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3">
-      <c r="A155" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="11" t="s">
-        <v>403</v>
+        <v>125</v>
+      </c>
+      <c r="C156" s="12" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="11" t="s">
-        <v>96</v>
+        <v>403</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
-      <c r="A160" s="2" t="s">
+    <row r="162" spans="1:3">
+      <c r="A162" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="45">
-      <c r="A161" s="11" t="s">
+    <row r="163" spans="1:3" ht="45">
+      <c r="A163" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C161" s="12" t="s">
+      <c r="C163" s="12" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
-      <c r="A162" s="11" t="s">
+    <row r="164" spans="1:3">
+      <c r="A164" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C162" s="12" t="s">
+      <c r="C164" s="12" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="30">
-      <c r="A163" s="11" t="s">
+    <row r="165" spans="1:3" ht="30">
+      <c r="A165" s="11" t="s">
         <v>139</v>
-      </c>
-      <c r="B163" s="13"/>
-      <c r="C163" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" ht="30">
-      <c r="A164" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B164" s="13"/>
-      <c r="C164" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="45">
-      <c r="A165" s="11" t="s">
-        <v>147</v>
       </c>
       <c r="B165" s="13"/>
       <c r="C165" s="12" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="30">
       <c r="A166" s="11" t="s">
-        <v>212</v>
+        <v>145</v>
       </c>
       <c r="B166" s="13"/>
       <c r="C166" s="12" t="s">
-        <v>213</v>
+        <v>146</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="45">
       <c r="A167" s="11" t="s">
-        <v>219</v>
+        <v>147</v>
       </c>
       <c r="B167" s="13"/>
       <c r="C167" s="12" t="s">
-        <v>220</v>
+        <v>375</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="11" t="s">
-        <v>221</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="B168" s="13"/>
       <c r="C168" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="45">
       <c r="A169" s="11" t="s">
-        <v>243</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="B169" s="13"/>
       <c r="C169" s="12" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="C170" s="12"/>
+        <v>221</v>
+      </c>
+      <c r="C170" s="12" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="11" t="s">
-        <v>404</v>
+        <v>243</v>
       </c>
       <c r="C171" s="12" t="s">
-        <v>405</v>
+        <v>244</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="11" t="s">
-        <v>406</v>
-      </c>
-      <c r="C172" s="12" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" ht="30">
+        <v>399</v>
+      </c>
+      <c r="C172" s="12"/>
+    </row>
+    <row r="173" spans="1:3">
       <c r="A173" s="11" t="s">
-        <v>481</v>
+        <v>404</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>482</v>
+        <v>405</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="C174" s="12" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="30">
+      <c r="A175" s="11" t="s">
+        <v>481</v>
+      </c>
+      <c r="C175" s="12" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" s="11" t="s">
         <v>533</v>
       </c>
-      <c r="C174" s="12" t="s">
+      <c r="C176" s="12" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="180" spans="1:3" s="9" customFormat="1">
-      <c r="A180" s="2"/>
-      <c r="B180" s="3"/>
-      <c r="C180" s="4"/>
+    <row r="177" spans="1:3">
+      <c r="A177" s="11" t="s">
+        <v>538</v>
+      </c>
+      <c r="B177" s="13"/>
+      <c r="C177" s="12"/>
+    </row>
+    <row r="181" spans="1:3" s="9" customFormat="1">
+      <c r="A181" s="2"/>
+      <c r="B181" s="3"/>
+      <c r="C181" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6236,231 +6270,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C7A8C5-284A-4109-8C79-92161ADBACD9}">
-  <dimension ref="A1:H29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="B10" s="69" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="B11" s="71" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="G12" t="s">
-        <v>488</v>
-      </c>
-      <c r="H12" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="70" t="s">
-        <v>387</v>
-      </c>
-      <c r="B13" s="58" t="s">
-        <v>392</v>
-      </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="92"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="70" t="s">
-        <v>388</v>
-      </c>
-      <c r="B14" s="61" t="s">
-        <v>391</v>
-      </c>
-      <c r="C14" s="73"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="83"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="88"/>
-      <c r="H14" s="93"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="70" t="s">
-        <v>390</v>
-      </c>
-      <c r="B15" s="59" t="s">
-        <v>393</v>
-      </c>
-      <c r="C15" s="74"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="94"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="70" t="s">
-        <v>389</v>
-      </c>
-      <c r="B16" s="60" t="s">
-        <v>394</v>
-      </c>
-      <c r="C16" s="75"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="85"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="90"/>
-      <c r="H16" s="95"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="70" t="s">
-        <v>386</v>
-      </c>
-      <c r="B17" s="64" t="s">
-        <v>420</v>
-      </c>
-      <c r="C17" s="76"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="85"/>
-      <c r="G17" s="91"/>
-      <c r="H17" s="96"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="29"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="29"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="29"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="29"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="29"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="29"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="29"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="29"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="29"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="29"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2396B387-46D7-4AB3-8C4F-DEA1CC7ED8C8}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -6495,10 +6304,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F160C7F-FB27-4F84-8171-6D9C64590D99}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6816,53 +6625,59 @@
         <v>484</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="65" t="s">
+    <row r="29" spans="1:3" ht="30">
+      <c r="A29" s="68" t="s">
         <v>348</v>
       </c>
-      <c r="B29" s="67"/>
-      <c r="C29" s="66" t="s">
-        <v>349</v>
+      <c r="B29" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="67" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30">
-      <c r="A30" s="65" t="s">
+      <c r="A30" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="67" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="68" t="s">
         <v>348</v>
       </c>
-      <c r="B30" s="66"/>
-      <c r="C30" s="66" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="65" t="s">
+      <c r="B31" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="67" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="68" t="s">
+        <v>350</v>
+      </c>
+      <c r="B32" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="67" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="68" t="s">
         <v>348</v>
       </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="66" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="30">
-      <c r="A32" s="68" t="s">
-        <v>348</v>
-      </c>
-      <c r="B32" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="67" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="30">
-      <c r="A33" s="68" t="s">
-        <v>116</v>
-      </c>
       <c r="B33" s="67" t="s">
         <v>23</v>
       </c>
       <c r="C33" s="67" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -6873,18 +6688,18 @@
         <v>23</v>
       </c>
       <c r="C34" s="67" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="68" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B35" s="67" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="67" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -6895,10 +6710,10 @@
         <v>23</v>
       </c>
       <c r="C36" s="67" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30">
       <c r="A37" s="68" t="s">
         <v>348</v>
       </c>
@@ -6906,7 +6721,7 @@
         <v>23</v>
       </c>
       <c r="C37" s="67" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -6917,7 +6732,7 @@
         <v>23</v>
       </c>
       <c r="C38" s="67" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -6928,10 +6743,10 @@
         <v>23</v>
       </c>
       <c r="C39" s="67" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="30">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="68" t="s">
         <v>348</v>
       </c>
@@ -6939,29 +6754,27 @@
         <v>23</v>
       </c>
       <c r="C40" s="67" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30">
       <c r="A41" s="68" t="s">
         <v>348</v>
       </c>
       <c r="B41" s="67" t="s">
-        <v>23</v>
+        <v>491</v>
       </c>
       <c r="C41" s="67" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="68" t="s">
-        <v>348</v>
-      </c>
-      <c r="B42" s="67" t="s">
-        <v>23</v>
-      </c>
+        <v>350</v>
+      </c>
+      <c r="B42" s="67"/>
       <c r="C42" s="67" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -6972,39 +6785,43 @@
         <v>23</v>
       </c>
       <c r="C43" s="67" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="30">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="68" t="s">
         <v>348</v>
       </c>
       <c r="B44" s="67" t="s">
-        <v>491</v>
+        <v>23</v>
       </c>
       <c r="C44" s="67" t="s">
-        <v>531</v>
+        <v>536</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="68" t="s">
-        <v>350</v>
-      </c>
-      <c r="B45" s="67"/>
+        <v>348</v>
+      </c>
+      <c r="B45" s="67" t="s">
+        <v>23</v>
+      </c>
       <c r="C45" s="67" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30">
       <c r="A46" s="68" t="s">
         <v>348</v>
       </c>
-      <c r="B46" s="67"/>
+      <c r="B46" s="67" t="s">
+        <v>23</v>
+      </c>
       <c r="C46" s="67" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="60">
       <c r="A47" s="68" t="s">
         <v>348</v>
       </c>
@@ -7012,51 +6829,59 @@
         <v>23</v>
       </c>
       <c r="C47" s="67" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="30">
       <c r="A48" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" s="67"/>
+      <c r="C48" s="67" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="65" t="s">
         <v>348</v>
       </c>
-      <c r="B48" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48" s="67" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="30">
-      <c r="A49" s="68" t="s">
+      <c r="B49" s="67"/>
+      <c r="C49" s="66" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30">
+      <c r="A50" s="65" t="s">
         <v>348</v>
       </c>
-      <c r="B49" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" s="67" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="30">
-      <c r="A50" s="68" t="s">
+      <c r="B50" s="66"/>
+      <c r="C50" s="66" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="65" t="s">
         <v>348</v>
       </c>
-      <c r="B50" s="67"/>
-      <c r="C50" s="67" t="s">
-        <v>564</v>
+      <c r="B51" s="66"/>
+      <c r="C51" s="66" t="s">
+        <v>448</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B50">
-    <cfRule type="containsText" dxfId="28" priority="1" operator="containsText" text="Won't Fix">
+  <conditionalFormatting sqref="B2:B51">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Won't Fix">
       <formula>NOT(ISERROR(SEARCH("Won't Fix",B2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Triaged">
+      <formula>NOT(ISERROR(SEARCH("Triaged",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7069,405 +6894,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64DCF449-93DC-43A2-805C-78061F57ADC8}">
-  <dimension ref="A1:M31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="67" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="23" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" t="s">
-        <v>539</v>
-      </c>
-      <c r="B1" t="s">
-        <v>540</v>
-      </c>
-      <c r="D1" t="s">
-        <v>565</v>
-      </c>
-      <c r="E1" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>541</v>
-      </c>
-      <c r="B2" t="s">
-        <v>542</v>
-      </c>
-      <c r="D2" t="s">
-        <v>567</v>
-      </c>
-      <c r="E2" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>543</v>
-      </c>
-      <c r="B3" t="s">
-        <v>544</v>
-      </c>
-      <c r="D3" t="s">
-        <v>569</v>
-      </c>
-      <c r="E3" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>545</v>
-      </c>
-      <c r="B4" t="s">
-        <v>546</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>579</v>
-      </c>
-      <c r="D4" t="s">
-        <v>571</v>
-      </c>
-      <c r="E4" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>547</v>
-      </c>
-      <c r="B5" t="s">
-        <v>548</v>
-      </c>
-      <c r="D5" t="s">
-        <v>572</v>
-      </c>
-      <c r="E5" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" t="s">
-        <v>549</v>
-      </c>
-      <c r="B6" t="s">
-        <v>514</v>
-      </c>
-      <c r="D6" t="s">
-        <v>574</v>
-      </c>
-      <c r="E6" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
-        <v>550</v>
-      </c>
-      <c r="B7" t="s">
-        <v>544</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>578</v>
-      </c>
-      <c r="D7" t="s">
-        <v>575</v>
-      </c>
-      <c r="E7" t="s">
-        <v>544</v>
-      </c>
-      <c r="M7" s="27"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" t="s">
-        <v>551</v>
-      </c>
-      <c r="B8" t="s">
-        <v>542</v>
-      </c>
-      <c r="D8" t="s">
-        <v>576</v>
-      </c>
-      <c r="E8" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" t="s">
-        <v>552</v>
-      </c>
-      <c r="B9" t="s">
-        <v>553</v>
-      </c>
-      <c r="D9" t="s">
-        <v>577</v>
-      </c>
-      <c r="E9" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="23" customFormat="1">
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" t="s">
-        <v>539</v>
-      </c>
-      <c r="B12" t="s">
-        <v>554</v>
-      </c>
-      <c r="D12" t="s">
-        <v>569</v>
-      </c>
-      <c r="E12" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>541</v>
-      </c>
-      <c r="B13" t="s">
-        <v>555</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>579</v>
-      </c>
-      <c r="D13" t="s">
-        <v>571</v>
-      </c>
-      <c r="E13" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" t="s">
-        <v>543</v>
-      </c>
-      <c r="B14" t="s">
-        <v>556</v>
-      </c>
-      <c r="D14" t="s">
-        <v>572</v>
-      </c>
-      <c r="E14" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" t="s">
-        <v>545</v>
-      </c>
-      <c r="B15" t="s">
-        <v>557</v>
-      </c>
-      <c r="D15" t="s">
-        <v>574</v>
-      </c>
-      <c r="E15" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" t="s">
-        <v>547</v>
-      </c>
-      <c r="B16" t="s">
-        <v>558</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>578</v>
-      </c>
-      <c r="D16" t="s">
-        <v>575</v>
-      </c>
-      <c r="E16" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>549</v>
-      </c>
-      <c r="B17" t="s">
-        <v>514</v>
-      </c>
-      <c r="D17" t="s">
-        <v>576</v>
-      </c>
-      <c r="E17" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>550</v>
-      </c>
-      <c r="B18" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>551</v>
-      </c>
-      <c r="B19" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>552</v>
-      </c>
-      <c r="B20" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="23" customFormat="1">
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>539</v>
-      </c>
-      <c r="B23" t="s">
-        <v>554</v>
-      </c>
-      <c r="D23" t="s">
-        <v>567</v>
-      </c>
-      <c r="E23" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>541</v>
-      </c>
-      <c r="B24" t="s">
-        <v>560</v>
-      </c>
-      <c r="D24" t="s">
-        <v>569</v>
-      </c>
-      <c r="E24" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>543</v>
-      </c>
-      <c r="B25" t="s">
-        <v>560</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>578</v>
-      </c>
-      <c r="D25" t="s">
-        <v>571</v>
-      </c>
-      <c r="E25" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>545</v>
-      </c>
-      <c r="B26" t="s">
-        <v>561</v>
-      </c>
-      <c r="D26" t="s">
-        <v>572</v>
-      </c>
-      <c r="E26" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>547</v>
-      </c>
-      <c r="B27" t="s">
-        <v>548</v>
-      </c>
-      <c r="D27" t="s">
-        <v>574</v>
-      </c>
-      <c r="E27" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>549</v>
-      </c>
-      <c r="B28" t="s">
-        <v>515</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>579</v>
-      </c>
-      <c r="D28" t="s">
-        <v>575</v>
-      </c>
-      <c r="E28" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>550</v>
-      </c>
-      <c r="B29" t="s">
-        <v>562</v>
-      </c>
-      <c r="D29" t="s">
-        <v>576</v>
-      </c>
-      <c r="E29" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>551</v>
-      </c>
-      <c r="B30" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>552</v>
-      </c>
-      <c r="B31" t="s">
-        <v>563</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D1CD3F-B09A-47BC-BCAB-315B61D092F4}">
   <dimension ref="A1:L10"/>
   <sheetViews>
@@ -7475,7 +6901,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.5703125" defaultRowHeight="15"/>
@@ -7591,7 +7017,7 @@
       <c r="I3" s="102" t="s">
         <v>515</v>
       </c>
-      <c r="J3" s="111" t="s">
+      <c r="J3" s="102" t="s">
         <v>515</v>
       </c>
       <c r="K3" s="103" t="s">
@@ -7629,10 +7055,10 @@
       <c r="I4" s="102" t="s">
         <v>519</v>
       </c>
-      <c r="J4" s="111" t="s">
+      <c r="J4" s="102" t="s">
         <v>519</v>
       </c>
-      <c r="K4" s="112" t="s">
+      <c r="K4" s="103" t="s">
         <v>519</v>
       </c>
       <c r="L4" s="103" t="s">
@@ -7767,25 +7193,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:L7">
-    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="ShrinkRight">
+    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="ShrinkRight">
       <formula>NOT(ISERROR(SEARCH("ShrinkRight",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="ShrinkLeft">
+    <cfRule type="containsText" dxfId="29" priority="2" operator="containsText" text="ShrinkLeft">
       <formula>NOT(ISERROR(SEARCH("ShrinkLeft",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="ReDistRight">
+    <cfRule type="containsText" dxfId="28" priority="3" operator="containsText" text="ReDistRight">
       <formula>NOT(ISERROR(SEARCH("ReDistRight",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="ReDistLeft">
+    <cfRule type="containsText" dxfId="27" priority="4" operator="containsText" text="ReDistLeft">
       <formula>NOT(ISERROR(SEARCH("ReDistLeft",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="PushLeft">
+    <cfRule type="containsText" dxfId="26" priority="5" operator="containsText" text="PushLeft">
       <formula>NOT(ISERROR(SEARCH("PushLeft",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="PushRight">
+    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="PushRight">
       <formula>NOT(ISERROR(SEARCH("PushRight",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="conflict">
+    <cfRule type="containsText" dxfId="24" priority="7" operator="containsText" text="conflict">
       <formula>NOT(ISERROR(SEARCH("conflict",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7797,7 +7223,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06728CA9-C11D-4FE8-8912-18D6A33E8379}">
   <dimension ref="A1:L24"/>
   <sheetViews>
@@ -7970,7 +7396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F77D648-B449-4B03-97EB-4834E79DA6CD}">
   <dimension ref="A1:F123"/>
   <sheetViews>
@@ -8529,12 +7955,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF11BE1A-892C-449D-A753-1B446ED96C7C}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15"/>
@@ -8688,135 +8114,136 @@
       <c r="H6" s="107"/>
     </row>
     <row r="7" spans="1:8" ht="30">
-      <c r="A7" s="114" t="s">
-        <v>584</v>
+      <c r="A7" s="112" t="s">
+        <v>544</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>580</v>
+        <v>540</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>586</v>
+        <v>546</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>585</v>
-      </c>
-      <c r="E7" s="113" t="s">
-        <v>587</v>
+        <v>545</v>
+      </c>
+      <c r="E7" s="111" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
-      <c r="A8" s="114" t="s">
-        <v>581</v>
+      <c r="A8" s="112" t="s">
+        <v>541</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>582</v>
+        <v>542</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>582</v>
+        <v>542</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>583</v>
+        <v>543</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>582</v>
+        <v>542</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="115" t="s">
-        <v>588</v>
+      <c r="A9" s="113" t="s">
+        <v>548</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>583</v>
+        <v>543</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>582</v>
+        <v>542</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>583</v>
+        <v>543</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>583</v>
+        <v>543</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30">
-      <c r="A10" s="115" t="s">
-        <v>589</v>
+      <c r="A10" s="113" t="s">
+        <v>549</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>582</v>
+        <v>542</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>582</v>
+        <v>542</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>582</v>
+        <v>542</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>582</v>
+        <v>542</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30">
-      <c r="A11" s="115" t="s">
-        <v>590</v>
+      <c r="A11" s="113" t="s">
+        <v>550</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>582</v>
+        <v>542</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>582</v>
+        <v>542</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>583</v>
+        <v>543</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>582</v>
+        <v>542</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:H5">
-    <cfRule type="containsText" dxfId="16" priority="4" stopIfTrue="1" operator="containsText" text="C1 Shrink">
+    <cfRule type="containsText" dxfId="23" priority="4" stopIfTrue="1" operator="containsText" text="C1 Shrink">
       <formula>NOT(ISERROR(SEARCH("C1 Shrink",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="5" stopIfTrue="1" operator="containsText" text="C2 Shrink">
+    <cfRule type="containsText" dxfId="22" priority="5" stopIfTrue="1" operator="containsText" text="C2 Shrink">
       <formula>NOT(ISERROR(SEARCH("C2 Shrink",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="6" stopIfTrue="1" operator="containsText" text="C1 ReDist">
+    <cfRule type="containsText" dxfId="21" priority="6" stopIfTrue="1" operator="containsText" text="C1 ReDist">
       <formula>NOT(ISERROR(SEARCH("C1 ReDist",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="7" stopIfTrue="1" operator="containsText" text="C2 ReDist">
+    <cfRule type="containsText" dxfId="20" priority="7" stopIfTrue="1" operator="containsText" text="C2 ReDist">
       <formula>NOT(ISERROR(SEARCH("C2 ReDist",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="8" stopIfTrue="1" operator="containsText" text="C1 Push">
+    <cfRule type="containsText" dxfId="19" priority="8" stopIfTrue="1" operator="containsText" text="C1 Push">
       <formula>NOT(ISERROR(SEARCH("C1 Push",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="9" stopIfTrue="1" operator="containsText" text="C2 Push">
+    <cfRule type="containsText" dxfId="18" priority="9" stopIfTrue="1" operator="containsText" text="C2 Push">
       <formula>NOT(ISERROR(SEARCH("C2 Push",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" stopIfTrue="1" operator="containsText" text="conflict">
+    <cfRule type="containsText" dxfId="17" priority="10" stopIfTrue="1" operator="containsText" text="conflict">
       <formula>NOT(ISERROR(SEARCH("conflict",B2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="11" stopIfTrue="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:E11">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="C1 R">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="C1 R">
       <formula>NOT(ISERROR(SEARCH("C1 R",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="C1 L">
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="C1 L">
       <formula>NOT(ISERROR(SEARCH("C1 L",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC8D572-6EFF-4BEA-BBEB-12B67F83C118}">
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
@@ -9279,25 +8706,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:H8">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="unknown">
+    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="unknown">
       <formula>NOT(ISERROR(SEARCH("unknown",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="cancel">
+    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="cancel">
       <formula>NOT(ISERROR(SEARCH("cancel",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="pN = N">
+    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="pN = N">
       <formula>NOT(ISERROR(SEARCH("pN = N",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="28" operator="containsText" text="unscheduled">
+    <cfRule type="containsText" dxfId="10" priority="28" operator="containsText" text="unscheduled">
       <formula>NOT(ISERROR(SEARCH("unscheduled",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="29" operator="containsText" text="confirm">
+    <cfRule type="containsText" dxfId="9" priority="29" operator="containsText" text="confirm">
       <formula>NOT(ISERROR(SEARCH("confirm",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="30" operator="containsText" text="conflict">
+    <cfRule type="containsText" dxfId="8" priority="30" operator="containsText" text="conflict">
       <formula>NOT(ISERROR(SEARCH("conflict",B2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="31" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9309,7 +8736,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4DB4886-0351-4FBB-AD2E-ACDCB11388DD}">
   <dimension ref="A1:F24"/>
   <sheetViews>
@@ -9564,4 +8991,229 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C7A8C5-284A-4109-8C79-92161ADBACD9}">
+  <dimension ref="A1:H29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="69" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="71" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="G12" t="s">
+        <v>488</v>
+      </c>
+      <c r="H12" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="70" t="s">
+        <v>387</v>
+      </c>
+      <c r="B13" s="58" t="s">
+        <v>392</v>
+      </c>
+      <c r="C13" s="72"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="92"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="70" t="s">
+        <v>388</v>
+      </c>
+      <c r="B14" s="61" t="s">
+        <v>391</v>
+      </c>
+      <c r="C14" s="73"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="93"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="70" t="s">
+        <v>390</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>393</v>
+      </c>
+      <c r="C15" s="74"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="89"/>
+      <c r="H15" s="94"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="70" t="s">
+        <v>389</v>
+      </c>
+      <c r="B16" s="60" t="s">
+        <v>394</v>
+      </c>
+      <c r="C16" s="75"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="95"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="70" t="s">
+        <v>386</v>
+      </c>
+      <c r="B17" s="64" t="s">
+        <v>420</v>
+      </c>
+      <c r="C17" s="76"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="91"/>
+      <c r="H17" s="96"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="29"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="29"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="29"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="29"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="29"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="29"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="29"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="29"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="29"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Day panel dimensions, concurrent objects
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="615">
   <si>
     <t>Feature</t>
   </si>
@@ -2002,6 +2002,24 @@
   </si>
   <si>
     <t>Edit Patterns from TimeTask editor</t>
+  </si>
+  <si>
+    <t>Label satisfies Task</t>
+  </si>
+  <si>
+    <t>right click select</t>
+  </si>
+  <si>
+    <t>List all of the CalendarObjects under the cursor as "Select blah blah…"</t>
+  </si>
+  <si>
+    <t>List of CalendarObjects</t>
+  </si>
+  <si>
+    <t>Togglable panel that shows a list of all CalendarObjects. Bind selection to day panel.</t>
+  </si>
+  <si>
+    <t>Horizontal Note, CheckIn objects</t>
   </si>
 </sst>
 </file>
@@ -4462,8 +4480,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:C183" totalsRowShown="0">
-  <autoFilter ref="A1:C183" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:C187" totalsRowShown="0">
+  <autoFilter ref="A1:C187" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="93"/>
     <tableColumn id="6" xr3:uid="{1FFE88A6-F499-42FB-A3F4-F5BDCD9D0CF0}" name="Done"/>
@@ -4891,10 +4909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:G187"/>
+  <dimension ref="A1:G191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99:C101"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5912,616 +5930,652 @@
       </c>
     </row>
     <row r="102" spans="1:3" s="13" customFormat="1">
-      <c r="A102" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B102" s="3"/>
-      <c r="C102" s="4" t="s">
-        <v>89</v>
-      </c>
+      <c r="A102" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B102" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C102" s="12"/>
     </row>
     <row r="103" spans="1:3" s="13" customFormat="1">
       <c r="A103" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="C103" s="12"/>
+        <v>99</v>
+      </c>
+      <c r="B103" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C103" s="4"/>
     </row>
     <row r="104" spans="1:3" s="13" customFormat="1">
       <c r="A104" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B104" s="3"/>
-      <c r="C104" s="4"/>
-    </row>
-    <row r="105" spans="1:3" s="13" customFormat="1" ht="30">
+        <v>614</v>
+      </c>
+      <c r="C104" s="12"/>
+    </row>
+    <row r="105" spans="1:3" s="13" customFormat="1">
       <c r="A105" s="11" t="s">
-        <v>347</v>
+        <v>610</v>
       </c>
       <c r="B105" s="3"/>
       <c r="C105" s="12" t="s">
-        <v>348</v>
+        <v>611</v>
       </c>
     </row>
     <row r="106" spans="1:3" s="13" customFormat="1">
       <c r="A106" s="11" t="s">
-        <v>336</v>
-      </c>
-      <c r="C106" s="12"/>
-    </row>
-    <row r="107" spans="1:3" s="13" customFormat="1">
+        <v>612</v>
+      </c>
+      <c r="B106" s="3"/>
+      <c r="C106" s="12" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" s="13" customFormat="1" ht="30">
       <c r="A107" s="11" t="s">
-        <v>608</v>
-      </c>
-      <c r="C107" s="12"/>
+        <v>347</v>
+      </c>
+      <c r="B107" s="3"/>
+      <c r="C107" s="12" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="108" spans="1:3" s="13" customFormat="1">
       <c r="A108" s="11" t="s">
-        <v>334</v>
-      </c>
-      <c r="B108" s="3"/>
+        <v>336</v>
+      </c>
       <c r="C108" s="12"/>
     </row>
     <row r="109" spans="1:3" s="13" customFormat="1">
       <c r="A109" s="11" t="s">
-        <v>356</v>
-      </c>
-      <c r="B109" s="3"/>
-      <c r="C109" s="12" t="s">
-        <v>100</v>
-      </c>
+        <v>608</v>
+      </c>
+      <c r="C109" s="12"/>
     </row>
     <row r="110" spans="1:3" s="13" customFormat="1">
       <c r="A110" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="B110" s="3"/>
+      <c r="C110" s="12"/>
+    </row>
+    <row r="111" spans="1:3" s="13" customFormat="1">
+      <c r="A111" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="B111" s="3"/>
+      <c r="C111" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" s="13" customFormat="1">
+      <c r="A112" s="11" t="s">
         <v>606</v>
       </c>
-      <c r="C110" s="12"/>
-    </row>
-    <row r="111" spans="1:3" s="13" customFormat="1">
-      <c r="A111" s="61" t="s">
+      <c r="C112" s="12"/>
+    </row>
+    <row r="113" spans="1:3" s="13" customFormat="1">
+      <c r="A113" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="B111" s="9"/>
-      <c r="C111" s="10"/>
-    </row>
-    <row r="112" spans="1:3" s="13" customFormat="1" ht="30">
-      <c r="A112" s="11" t="s">
+      <c r="B113" s="9"/>
+      <c r="C113" s="10"/>
+    </row>
+    <row r="114" spans="1:3" s="13" customFormat="1" ht="30">
+      <c r="A114" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C112" s="12" t="s">
+      <c r="C114" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="113" spans="1:3" s="13" customFormat="1" ht="30">
-      <c r="A113" s="11" t="s">
+    <row r="115" spans="1:3" s="13" customFormat="1" ht="30">
+      <c r="A115" s="11" t="s">
         <v>331</v>
-      </c>
-      <c r="B113" s="3"/>
-      <c r="C113" s="12" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" s="13" customFormat="1" ht="30">
-      <c r="A114" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B114" s="3"/>
-      <c r="C114" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" s="13" customFormat="1">
-      <c r="A115" s="11" t="s">
-        <v>205</v>
       </c>
       <c r="B115" s="3"/>
       <c r="C115" s="12" t="s">
-        <v>206</v>
+        <v>330</v>
       </c>
     </row>
     <row r="116" spans="1:3" s="13" customFormat="1" ht="30">
-      <c r="A116" s="11" t="s">
-        <v>362</v>
+      <c r="A116" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="B116" s="3"/>
-      <c r="C116" s="12" t="s">
-        <v>357</v>
+      <c r="C116" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="117" spans="1:3" s="13" customFormat="1">
       <c r="A117" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B117" s="3"/>
+      <c r="C117" s="12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" s="13" customFormat="1" ht="30">
+      <c r="A118" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="B118" s="3"/>
+      <c r="C118" s="12" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" s="13" customFormat="1">
+      <c r="A119" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="C117" s="12" t="s">
+      <c r="C119" s="12" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="118" spans="1:3" s="13" customFormat="1">
-      <c r="A118" s="2" t="s">
+    <row r="120" spans="1:3" s="13" customFormat="1">
+      <c r="A120" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B118" s="3"/>
-      <c r="C118" s="4" t="s">
+      <c r="B120" s="3"/>
+      <c r="C120" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="119" spans="1:3" s="13" customFormat="1" ht="30">
-      <c r="A119" s="11" t="s">
+    <row r="121" spans="1:3" s="13" customFormat="1">
+      <c r="A121" s="11" t="s">
+        <v>609</v>
+      </c>
+      <c r="C121" s="12"/>
+    </row>
+    <row r="122" spans="1:3" s="13" customFormat="1" ht="30">
+      <c r="A122" s="11" t="s">
         <v>441</v>
       </c>
-      <c r="C119" s="12" t="s">
+      <c r="C122" s="12" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="120" spans="1:3" s="13" customFormat="1" ht="60">
-      <c r="A120" s="11" t="s">
+    <row r="123" spans="1:3" s="13" customFormat="1" ht="60">
+      <c r="A123" s="11" t="s">
         <v>506</v>
       </c>
-      <c r="C120" s="12" t="s">
+      <c r="C123" s="12" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="121" spans="1:3" s="13" customFormat="1" ht="60">
-      <c r="A121" s="11" t="s">
+    <row r="124" spans="1:3" s="13" customFormat="1" ht="60">
+      <c r="A124" s="11" t="s">
         <v>261</v>
-      </c>
-      <c r="B121" s="3"/>
-      <c r="C121" s="12" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" s="13" customFormat="1">
-      <c r="A122" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B122" s="3"/>
-      <c r="C122" s="4"/>
-    </row>
-    <row r="123" spans="1:3" s="13" customFormat="1">
-      <c r="A123" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B123" s="3"/>
-      <c r="C123" s="4"/>
-    </row>
-    <row r="124" spans="1:3" s="13" customFormat="1" ht="30">
-      <c r="A124" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="B124" s="3"/>
       <c r="C124" s="12" t="s">
-        <v>34</v>
+        <v>262</v>
       </c>
     </row>
     <row r="125" spans="1:3" s="13" customFormat="1">
       <c r="A125" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B125" s="3"/>
       <c r="C125" s="4"/>
     </row>
     <row r="126" spans="1:3" s="13" customFormat="1">
       <c r="A126" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B126" s="3"/>
       <c r="C126" s="4"/>
     </row>
     <row r="127" spans="1:3" s="13" customFormat="1" ht="30">
-      <c r="A127" s="11" t="s">
-        <v>202</v>
+      <c r="A127" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B127" s="3"/>
       <c r="C127" s="12" t="s">
-        <v>203</v>
+        <v>34</v>
       </c>
     </row>
     <row r="128" spans="1:3" s="13" customFormat="1">
       <c r="A128" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B128" s="3"/>
       <c r="C128" s="4"/>
     </row>
     <row r="129" spans="1:3" s="13" customFormat="1">
-      <c r="A129" s="11" t="s">
+      <c r="A129" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B129" s="3"/>
+      <c r="C129" s="4"/>
+    </row>
+    <row r="130" spans="1:3" s="13" customFormat="1" ht="30">
+      <c r="A130" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B130" s="3"/>
+      <c r="C130" s="12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" s="13" customFormat="1">
+      <c r="A131" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B131" s="3"/>
+      <c r="C131" s="4"/>
+    </row>
+    <row r="132" spans="1:3" s="13" customFormat="1">
+      <c r="A132" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="C129" s="12" t="s">
+      <c r="C132" s="12" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="130" spans="1:3" s="13" customFormat="1">
-      <c r="A130" s="2" t="s">
+    <row r="133" spans="1:3" s="13" customFormat="1">
+      <c r="A133" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B130" s="3"/>
-      <c r="C130" s="4"/>
-    </row>
-    <row r="131" spans="1:3" s="13" customFormat="1" ht="30">
-      <c r="A131" s="11" t="s">
+      <c r="B133" s="3"/>
+      <c r="C133" s="4"/>
+    </row>
+    <row r="134" spans="1:3" s="13" customFormat="1" ht="30">
+      <c r="A134" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B131" s="3"/>
-      <c r="C131" s="12" t="s">
+      <c r="B134" s="3"/>
+      <c r="C134" s="12" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="132" spans="1:3" s="13" customFormat="1" ht="30">
-      <c r="A132" s="11" t="s">
+    <row r="135" spans="1:3" s="13" customFormat="1" ht="30">
+      <c r="A135" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B132" s="3"/>
-      <c r="C132" s="12" t="s">
+      <c r="B135" s="3"/>
+      <c r="C135" s="12" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
-      <c r="A133" s="2" t="s">
+    <row r="136" spans="1:3" s="13" customFormat="1">
+      <c r="A136" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="134" spans="1:3">
-      <c r="A134" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C134" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3">
-      <c r="A135" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C135" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="30">
-      <c r="A136" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C136" s="12" t="s">
-        <v>95</v>
-      </c>
+      <c r="B136" s="3"/>
+      <c r="C136" s="4"/>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C137" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="30">
+      <c r="A140" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C140" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C137" s="12" t="s">
+      <c r="C141" s="12" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="45">
-      <c r="A138" s="11" t="s">
+    <row r="142" spans="1:3" ht="45">
+      <c r="A142" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="C138" s="12" t="s">
+      <c r="C142" s="12" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="45">
-      <c r="A139" s="11" t="s">
+    <row r="143" spans="1:3" ht="45">
+      <c r="A143" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C139" s="12" t="s">
+      <c r="C143" s="12" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
-      <c r="A140" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="C140" s="12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3">
-      <c r="A141" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="C141" s="12" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" ht="90">
-      <c r="A142" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="C142" s="12" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="90">
-      <c r="A143" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="C143" s="12" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="C144" s="12"/>
-    </row>
-    <row r="145" spans="1:3" ht="60">
+        <v>138</v>
+      </c>
+      <c r="C144" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
       <c r="A145" s="11" t="s">
-        <v>294</v>
+        <v>320</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="90">
       <c r="A146" s="11" t="s">
-        <v>295</v>
+        <v>342</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="90">
       <c r="A147" s="11" t="s">
-        <v>502</v>
+        <v>344</v>
+      </c>
+      <c r="C147" s="12" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="11" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3">
+        <v>201</v>
+      </c>
+      <c r="C148" s="12"/>
+    </row>
+    <row r="149" spans="1:3" ht="60">
       <c r="A149" s="11" t="s">
-        <v>97</v>
+        <v>294</v>
+      </c>
+      <c r="C149" s="12" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="11" t="s">
-        <v>98</v>
+        <v>295</v>
+      </c>
+      <c r="C150" s="12" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="151" spans="1:3">
-      <c r="A151" s="2" t="s">
-        <v>47</v>
+      <c r="A151" s="11" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="152" spans="1:3">
-      <c r="A152" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C152" s="12" t="s">
-        <v>101</v>
+      <c r="A152" s="11" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="11" t="s">
-        <v>349</v>
-      </c>
-      <c r="C153" s="12"/>
+        <v>97</v>
+      </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C156" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="C157" s="12"/>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="C154" s="12"/>
-    </row>
-    <row r="155" spans="1:3">
-      <c r="A155" s="11" t="s">
+      <c r="C158" s="12"/>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="C155" s="12"/>
-    </row>
-    <row r="156" spans="1:3">
-      <c r="A156" s="11" t="s">
+      <c r="C159" s="12"/>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C156" s="12"/>
-    </row>
-    <row r="157" spans="1:3" ht="45">
-      <c r="A157" s="11" t="s">
+      <c r="C160" s="12"/>
+    </row>
+    <row r="161" spans="1:3" ht="45">
+      <c r="A161" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B157" s="13"/>
-      <c r="C157" s="12" t="s">
+      <c r="B161" s="13"/>
+      <c r="C161" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="30">
-      <c r="A158" s="2" t="s">
+    <row r="162" spans="1:3" ht="30">
+      <c r="A162" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C158" s="4" t="s">
+      <c r="C162" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
-      <c r="A159" s="2" t="s">
+    <row r="163" spans="1:3">
+      <c r="A163" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C159" s="4" t="s">
+      <c r="C163" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
-      <c r="A160" s="61" t="s">
+    <row r="164" spans="1:3">
+      <c r="A164" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="B160" s="9"/>
-      <c r="C160" s="10" t="s">
+      <c r="B164" s="9"/>
+      <c r="C164" s="10" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3">
-      <c r="A161" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C161" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3">
-      <c r="A162" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3">
-      <c r="A163" s="11" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3">
-      <c r="A164" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="11" t="s">
-        <v>96</v>
+        <v>125</v>
+      </c>
+      <c r="C165" s="12" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="2" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
     </row>
     <row r="167" spans="1:3">
-      <c r="A167" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="45">
-      <c r="A168" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C168" s="12" t="s">
-        <v>351</v>
+      <c r="A167" s="11" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C169" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" ht="30">
-      <c r="A170" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="B170" s="13"/>
-      <c r="C170" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" ht="30">
-      <c r="A171" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B171" s="13"/>
-      <c r="C171" s="12" t="s">
-        <v>146</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="45">
       <c r="A172" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="B172" s="13"/>
+        <v>115</v>
+      </c>
       <c r="C172" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="B173" s="13"/>
+        <v>131</v>
+      </c>
       <c r="C173" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="30">
       <c r="A174" s="11" t="s">
-        <v>219</v>
+        <v>139</v>
       </c>
       <c r="B174" s="13"/>
       <c r="C174" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="30">
       <c r="A175" s="11" t="s">
-        <v>221</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="B175" s="13"/>
       <c r="C175" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="45">
       <c r="A176" s="11" t="s">
-        <v>243</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="B176" s="13"/>
       <c r="C176" s="12" t="s">
-        <v>244</v>
+        <v>352</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="11" t="s">
-        <v>376</v>
-      </c>
-      <c r="C177" s="12"/>
-    </row>
-    <row r="178" spans="1:3">
+        <v>212</v>
+      </c>
+      <c r="B177" s="13"/>
+      <c r="C177" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="45">
       <c r="A178" s="11" t="s">
-        <v>381</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="B178" s="13"/>
       <c r="C178" s="12" t="s">
-        <v>382</v>
+        <v>220</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" s="11" t="s">
-        <v>383</v>
+        <v>221</v>
       </c>
       <c r="C179" s="12" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="30">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
       <c r="A180" s="11" t="s">
-        <v>449</v>
+        <v>243</v>
       </c>
       <c r="C180" s="12" t="s">
-        <v>450</v>
+        <v>244</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="11" t="s">
-        <v>485</v>
-      </c>
-      <c r="C181" s="12" t="s">
-        <v>486</v>
-      </c>
+        <v>376</v>
+      </c>
+      <c r="C181" s="12"/>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="11" t="s">
-        <v>490</v>
-      </c>
-      <c r="B182" s="13"/>
-      <c r="C182" s="12"/>
+        <v>381</v>
+      </c>
+      <c r="C182" s="12" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="C183" s="12" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="30">
+      <c r="A184" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="C184" s="12" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="C185" s="12" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" s="11" t="s">
+        <v>490</v>
+      </c>
+      <c r="B186" s="13"/>
+      <c r="C186" s="12"/>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" s="11" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="187" spans="1:3" s="9" customFormat="1">
-      <c r="A187" s="2"/>
-      <c r="B187" s="3"/>
-      <c r="C187" s="4"/>
+    <row r="191" spans="1:3" s="9" customFormat="1">
+      <c r="A191" s="2"/>
+      <c r="B191" s="3"/>
+      <c r="C191" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
Horizontal/Vertical Note, CheckIn, NowMark
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="615">
   <si>
     <t>Feature</t>
   </si>
@@ -2839,254 +2839,6 @@
   </cellStyles>
   <dxfs count="100">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC0CB"/>
-          <bgColor rgb="FFFFC0CB"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF7F"/>
-          <bgColor rgb="FF00FF7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7FFF00"/>
-          <bgColor rgb="FF7FFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FFDC143C"/>
-          <bgColor rgb="FFDC143C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3608,6 +3360,111 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3690,6 +3547,48 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3962,6 +3861,63 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC0CB"/>
+          <bgColor rgb="FFFFC0CB"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF7F"/>
+          <bgColor rgb="FF00FF7F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7FFF00"/>
+          <bgColor rgb="FF7FFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFDC143C"/>
+          <bgColor rgb="FFDC143C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -4063,10 +4019,54 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -4483,108 +4483,108 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:C187" totalsRowShown="0">
   <autoFilter ref="A1:C187" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="93"/>
+    <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="92"/>
     <tableColumn id="6" xr3:uid="{1FFE88A6-F499-42FB-A3F4-F5BDCD9D0CF0}" name="Done"/>
-    <tableColumn id="5" xr3:uid="{65384592-5F41-4A06-A57C-FE71C87B4BDD}" name="Notes" dataDxfId="92"/>
+    <tableColumn id="5" xr3:uid="{65384592-5F41-4A06-A57C-FE71C87B4BDD}" name="Notes" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F572A93C-B296-47BB-A2B7-E8D930E92020}" name="Table4" displayName="Table4" ref="A1:C62" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90" tableBorderDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F572A93C-B296-47BB-A2B7-E8D930E92020}" name="Table4" displayName="Table4" ref="A1:C62" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85" tableBorderDxfId="84">
   <autoFilter ref="A1:C62" xr:uid="{5B5CE518-BB75-408C-8F1B-EE90C29E48F3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2EF2C0F2-7D81-49C3-B8A7-E25CCB336A17}" name="Column1" dataDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{FCC47FF7-6739-4E5E-9E09-E5EAD7161467}" name="Column2" dataDxfId="87"/>
-    <tableColumn id="3" xr3:uid="{3079BD65-A18D-4106-9386-B084236E0CE0}" name="Column3" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{2EF2C0F2-7D81-49C3-B8A7-E25CCB336A17}" name="Column1" dataDxfId="83"/>
+    <tableColumn id="2" xr3:uid="{FCC47FF7-6739-4E5E-9E09-E5EAD7161467}" name="Column2" dataDxfId="82"/>
+    <tableColumn id="3" xr3:uid="{3079BD65-A18D-4106-9386-B084236E0CE0}" name="Column3" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E4DD08F2-9CC2-46CC-93EE-E01A4DBC8EEE}" name="Table5" displayName="Table5" ref="A1:H8" totalsRowShown="0" headerRowDxfId="85" dataDxfId="83" headerRowBorderDxfId="84" tableBorderDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E4DD08F2-9CC2-46CC-93EE-E01A4DBC8EEE}" name="Table5" displayName="Table5" ref="A1:H8" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70">
   <autoFilter ref="A1:H8" xr:uid="{9EF71295-67E3-4AA7-981B-99814F9C00D6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5F56F396-ECBF-4022-A747-BB6579150BC5}" name="Previous" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{52DF5424-7715-4094-9055-254252166B84}" name="CI Start_x000a_in Z" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{4BF25F2B-3788-4EC0-877F-738CFB7416BD}" name="CI End_x000a_in Z" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{3D1264CD-7DED-47FE-9A26-02FAA9BC34AE}" name="CI Start_x000a_out Z" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{91478E3E-F2EC-42B9-9CAC-61EA2AD657CB}" name="CI End_x000a_out Z" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{BD45968E-F796-4835-9D67-3627C99D24EC}" name="Z Start" dataDxfId="76"/>
-    <tableColumn id="7" xr3:uid="{3B4EE896-0831-43E7-8AE0-49A3476BEA97}" name="Z End" dataDxfId="75"/>
-    <tableColumn id="8" xr3:uid="{D4DAA8AA-8B7A-4978-8C26-61D2C9036856}" name="P End" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{5F56F396-ECBF-4022-A747-BB6579150BC5}" name="Previous" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{52DF5424-7715-4094-9055-254252166B84}" name="CI Start_x000a_in Z" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{4BF25F2B-3788-4EC0-877F-738CFB7416BD}" name="CI End_x000a_in Z" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{3D1264CD-7DED-47FE-9A26-02FAA9BC34AE}" name="CI Start_x000a_out Z" dataDxfId="66"/>
+    <tableColumn id="5" xr3:uid="{91478E3E-F2EC-42B9-9CAC-61EA2AD657CB}" name="CI End_x000a_out Z" dataDxfId="65"/>
+    <tableColumn id="6" xr3:uid="{BD45968E-F796-4835-9D67-3627C99D24EC}" name="Z Start" dataDxfId="64"/>
+    <tableColumn id="7" xr3:uid="{3B4EE896-0831-43E7-8AE0-49A3476BEA97}" name="Z End" dataDxfId="63"/>
+    <tableColumn id="8" xr3:uid="{D4DAA8AA-8B7A-4978-8C26-61D2C9036856}" name="P End" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC6FE9AE-35E3-4705-A142-315DB9D43B3A}" name="Table3" displayName="Table3" ref="A1:A117" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC6FE9AE-35E3-4705-A142-315DB9D43B3A}" name="Table3" displayName="Table3" ref="A1:A117" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A1:A117" xr:uid="{A2F7B623-DE53-4896-BDD6-CCC38D4467C3}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0C8999A5-1CD8-483C-A3BB-7AD00E0E2478}" name="Collision Theory" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{0C8999A5-1CD8-483C-A3BB-7AD00E0E2478}" name="Collision Theory" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67135CB1-5074-4EBE-BD9A-48C30A4CB81B}" name="Table2" displayName="Table2" ref="A1:E5" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" tableBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67135CB1-5074-4EBE-BD9A-48C30A4CB81B}" name="Table2" displayName="Table2" ref="A1:E5" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51" tableBorderDxfId="50">
   <autoFilter ref="A1:E5" xr:uid="{B388395A-7532-4521-958E-47A4C8955AF2}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{70C2C4E6-CAF6-425B-8E04-929D489EC9D7}" name="Determine L, R_x000a_Step1" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{2FE5E346-C794-4C60-92C1-0865C7DF44B2}" name="C2.LT_x000a_C2.RT" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{D05D7189-86A2-4E66-978C-200C858C620C}" name="C2.LT null_x000a_C2.RT" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{9D36A042-6482-4DEE-A827-BCFC97E3E6B9}" name="C2.LT_x000a_C2.RT null" dataDxfId="64"/>
-    <tableColumn id="5" xr3:uid="{DCA50F46-3DCF-4728-AFF9-64F17E91077A}" name="C2.LT null_x000a_C2.RT null" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{70C2C4E6-CAF6-425B-8E04-929D489EC9D7}" name="Determine L, R_x000a_Step1" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{2FE5E346-C794-4C60-92C1-0865C7DF44B2}" name="C2.LT_x000a_C2.RT" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{D05D7189-86A2-4E66-978C-200C858C620C}" name="C2.LT null_x000a_C2.RT" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{9D36A042-6482-4DEE-A827-BCFC97E3E6B9}" name="C2.LT_x000a_C2.RT null" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{DCA50F46-3DCF-4728-AFF9-64F17E91077A}" name="C2.LT null_x000a_C2.RT null" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1D0690DC-ACA6-40D8-866A-1D8C44DE4AC8}" name="Table7" displayName="Table7" ref="A7:D8" totalsRowShown="0" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1D0690DC-ACA6-40D8-866A-1D8C44DE4AC8}" name="Table7" displayName="Table7" ref="A7:D8" totalsRowShown="0" tableBorderDxfId="44">
   <autoFilter ref="A7:D8" xr:uid="{ACCFA163-AAF6-4628-ADE5-97056064C206}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9757D096-D900-42A9-8E11-C4ACA310AE56}" name="Determine L, R_x000a_Step2" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{C3069A29-6915-46B5-977A-E175A6DEB3D2}" name="C1.S &lt; C2.S" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{12A8AD37-B3F9-4A8B-9EA6-A0F6EB34B35A}" name="C1.S == C2.S" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{7A2BF950-BBF5-494B-8BCE-AD358D4349E2}" name="C1.S &gt; C2.S" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{9757D096-D900-42A9-8E11-C4ACA310AE56}" name="Determine L, R_x000a_Step2" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{C3069A29-6915-46B5-977A-E175A6DEB3D2}" name="C1.S &lt; C2.S" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{12A8AD37-B3F9-4A8B-9EA6-A0F6EB34B35A}" name="C1.S == C2.S" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{7A2BF950-BBF5-494B-8BCE-AD358D4349E2}" name="C1.S &gt; C2.S" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BEABA309-E652-49AF-B0CA-0DBB8732C3D3}" name="Table6" displayName="Table6" ref="A1:N8" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BEABA309-E652-49AF-B0CA-0DBB8732C3D3}" name="Table6" displayName="Table6" ref="A1:N8" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A1:N8" xr:uid="{3AB9159B-B403-4CC8-8649-2A74831EFA39}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{72C9A77E-AFBC-404B-A7F6-E681135EDAE9}" name="Redistribute_x000a_Collision_x000a_… T L ∩ R T …" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{7B5E19F2-C874-4B16-82C8-FA89018E0F3A}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="54"/>
-    <tableColumn id="13" xr3:uid="{140BB756-BA0B-42B4-96AC-20E496CA56A3}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{E21AAA4F-92B4-436C-B55B-4DFD07C4BE29}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="52"/>
-    <tableColumn id="14" xr3:uid="{7026FFA9-3F08-448A-86A1-E71772461B72}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="51"/>
-    <tableColumn id="12" xr3:uid="{59C7730E-CD9C-445B-A9A4-AEE7F50B376A}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="50"/>
-    <tableColumn id="11" xr3:uid="{6F38818E-A5E5-47C6-AFD4-C58CF1FD3DD5}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{DFFA66D7-E0E3-4911-BECE-C58139CDD28D}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{C2DC972A-AC9A-4140-A684-443F75AEE447}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{833A1012-7AE2-431D-82C0-B7CB5960C752}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{43D8BEE4-A2A2-4CFF-9608-9E5B08D746D9}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{0599BB19-BD4F-4332-92DE-B1E045C56EEF}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{3C3A9FF5-1451-4E38-87EA-C000A51EC5B5}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{D413EC93-83CF-4773-9080-8AB9148DFA4E}" name="R.S🔒" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{72C9A77E-AFBC-404B-A7F6-E681135EDAE9}" name="Redistribute_x000a_Collision_x000a_… T L ∩ R T …" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{7B5E19F2-C874-4B16-82C8-FA89018E0F3A}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{140BB756-BA0B-42B4-96AC-20E496CA56A3}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{E21AAA4F-92B4-436C-B55B-4DFD07C4BE29}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{7026FFA9-3F08-448A-86A1-E71772461B72}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{59C7730E-CD9C-445B-A9A4-AEE7F50B376A}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{6F38818E-A5E5-47C6-AFD4-C58CF1FD3DD5}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{DFFA66D7-E0E3-4911-BECE-C58139CDD28D}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{C2DC972A-AC9A-4140-A684-443F75AEE447}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{833A1012-7AE2-431D-82C0-B7CB5960C752}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{43D8BEE4-A2A2-4CFF-9608-9E5B08D746D9}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{0599BB19-BD4F-4332-92DE-B1E045C56EEF}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{3C3A9FF5-1451-4E38-87EA-C000A51EC5B5}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{D413EC93-83CF-4773-9080-8AB9148DFA4E}" name="R.S🔒" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BB600374-B6B9-40D7-85BD-757E0CB6012B}" name="Table8" displayName="Table8" ref="A10:I14" totalsRowShown="0" headerRowDxfId="41" tableBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BB600374-B6B9-40D7-85BD-757E0CB6012B}" name="Table8" displayName="Table8" ref="A10:I14" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A10:I14" xr:uid="{CC633682-C369-475E-BC03-B121AB91AB17}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{78CD584E-A9D4-40D7-9D09-CF0EF6806B2D}" name="GetPushData" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{78CD584E-A9D4-40D7-9D09-CF0EF6806B2D}" name="GetPushData" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{A08CEA82-1CE9-4441-B0EF-0A975D8FE65A}" name="LT.CanReDist=T_x000a_LT.Limited=T_x000a_LT &lt; WC"/>
     <tableColumn id="6" xr3:uid="{F6036D13-DB0F-4AF8-A1E6-30BCCEB2A5F3}" name="LT.CanReDist=T_x000a_LT.Limited=T_x000a_LT &gt;= WC"/>
     <tableColumn id="4" xr3:uid="{B3ED7712-7A0A-4E68-A538-F34B63335364}" name="LT.CanReDist=T_x000a_LT.Limited=F_x000a_LT &lt; WC"/>
@@ -4599,14 +4599,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2B1B7CE4-90F7-42CA-B974-855205A0C605}" name="Table11" displayName="Table11" ref="A2:E12" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2B1B7CE4-90F7-42CA-B974-855205A0C605}" name="Table11" displayName="Table11" ref="A2:E12" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A2:E12" xr:uid="{78FF5B0B-0912-499F-8F6A-339F3CEEC95F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F251C872-2A1D-42A0-994A-2DFC09D7C047}" name="State" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{F251C872-2A1D-42A0-994A-2DFC09D7C047}" name="State" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{AB62CF60-B9F3-442C-A4D1-2FC89B02B851}" name="Border Color"/>
-    <tableColumn id="3" xr3:uid="{E3035B58-4720-4F96-BC43-0FE1566CB1AC}" name="Happens When" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{64A950F1-3FCD-413C-8376-9DAD13362BEC}" name="Details" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{6FB2B197-5E34-46A9-BA2C-CE95765F93BA}" name="Leads to" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{E3035B58-4720-4F96-BC43-0FE1566CB1AC}" name="Happens When" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{64A950F1-3FCD-413C-8376-9DAD13362BEC}" name="Details" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{6FB2B197-5E34-46A9-BA2C-CE95765F93BA}" name="Leads to" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4912,7 +4912,7 @@
   <dimension ref="A1:G191"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5951,6 +5951,9 @@
       <c r="A104" s="11" t="s">
         <v>614</v>
       </c>
+      <c r="B104" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="C104" s="12"/>
     </row>
     <row r="105" spans="1:3" s="13" customFormat="1">
@@ -6579,7 +6582,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7323,18 +7326,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B62">
-    <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="Triaged">
+    <cfRule type="containsText" dxfId="90" priority="1" operator="containsText" text="Triaged">
       <formula>NOT(ISERROR(SEARCH("Triaged",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="2" operator="containsText" text="Won't Fix">
+    <cfRule type="containsText" dxfId="89" priority="2" operator="containsText" text="Won't Fix">
       <formula>NOT(ISERROR(SEARCH("Won't Fix",B2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="4" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7951,25 +7954,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:H8">
-    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="unknown">
+    <cfRule type="containsText" dxfId="80" priority="1" operator="containsText" text="unknown">
       <formula>NOT(ISERROR(SEARCH("unknown",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="2" operator="containsText" text="cancel">
+    <cfRule type="containsText" dxfId="79" priority="2" operator="containsText" text="cancel">
       <formula>NOT(ISERROR(SEARCH("cancel",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="3" operator="containsText" text="pN = N">
+    <cfRule type="containsText" dxfId="78" priority="3" operator="containsText" text="pN = N">
       <formula>NOT(ISERROR(SEARCH("pN = N",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="unscheduled">
+    <cfRule type="containsText" dxfId="77" priority="28" operator="containsText" text="unscheduled">
       <formula>NOT(ISERROR(SEARCH("unscheduled",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="29" operator="containsText" text="confirm">
+    <cfRule type="containsText" dxfId="76" priority="29" operator="containsText" text="confirm">
       <formula>NOT(ISERROR(SEARCH("confirm",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="30" operator="containsText" text="conflict">
+    <cfRule type="containsText" dxfId="75" priority="30" operator="containsText" text="conflict">
       <formula>NOT(ISERROR(SEARCH("conflict",B2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="31" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8718,24 +8721,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:E5">
-    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="Step2">
+    <cfRule type="containsText" dxfId="58" priority="4" operator="containsText" text="Step2">
       <formula>NOT(ISERROR(SEARCH("Step2",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="C1 R">
+    <cfRule type="containsText" dxfId="57" priority="5" operator="containsText" text="C1 R">
       <formula>NOT(ISERROR(SEARCH("C1 R",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="C1 L">
+    <cfRule type="containsText" dxfId="56" priority="6" operator="containsText" text="C1 L">
       <formula>NOT(ISERROR(SEARCH("C1 L",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:D8">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Step2">
+    <cfRule type="containsText" dxfId="55" priority="1" operator="containsText" text="Step2">
       <formula>NOT(ISERROR(SEARCH("Step2",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="C1 R">
+    <cfRule type="containsText" dxfId="54" priority="2" operator="containsText" text="C1 R">
       <formula>NOT(ISERROR(SEARCH("C1 R",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="C1 L">
+    <cfRule type="containsText" dxfId="53" priority="3" operator="containsText" text="C1 L">
       <formula>NOT(ISERROR(SEARCH("C1 L",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9271,51 +9274,51 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:N8">
-    <cfRule type="containsText" dxfId="14" priority="1" stopIfTrue="1" operator="containsText" text="ShrinkRight WC">
+    <cfRule type="containsText" dxfId="39" priority="1" stopIfTrue="1" operator="containsText" text="ShrinkRight WC">
       <formula>NOT(ISERROR(SEARCH("ShrinkRight WC",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" stopIfTrue="1" operator="containsText" text="ShrinkLeft WC">
+    <cfRule type="containsText" dxfId="38" priority="2" stopIfTrue="1" operator="containsText" text="ShrinkLeft WC">
       <formula>NOT(ISERROR(SEARCH("ShrinkLeft WC",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="ShrinkRight">
+    <cfRule type="containsText" dxfId="37" priority="3" operator="containsText" text="ShrinkRight">
       <formula>NOT(ISERROR(SEARCH("ShrinkRight",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="ShrinkLeft">
+    <cfRule type="containsText" dxfId="36" priority="4" operator="containsText" text="ShrinkLeft">
       <formula>NOT(ISERROR(SEARCH("ShrinkLeft",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" stopIfTrue="1" operator="containsText" text="ReDistRight WC">
+    <cfRule type="containsText" dxfId="35" priority="5" stopIfTrue="1" operator="containsText" text="ReDistRight WC">
       <formula>NOT(ISERROR(SEARCH("ReDistRight WC",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" stopIfTrue="1" operator="containsText" text="ReDistLeft WC">
+    <cfRule type="containsText" dxfId="34" priority="6" stopIfTrue="1" operator="containsText" text="ReDistLeft WC">
       <formula>NOT(ISERROR(SEARCH("ReDistLeft WC",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="ReDistRight">
+    <cfRule type="containsText" dxfId="33" priority="10" operator="containsText" text="ReDistRight">
       <formula>NOT(ISERROR(SEARCH("ReDistRight",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="ReDistLeft">
+    <cfRule type="containsText" dxfId="32" priority="11" operator="containsText" text="ReDistLeft">
       <formula>NOT(ISERROR(SEARCH("ReDistLeft",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="12" stopIfTrue="1" operator="containsText" text="PushLeft WC">
+    <cfRule type="containsText" dxfId="31" priority="12" stopIfTrue="1" operator="containsText" text="PushLeft WC">
       <formula>NOT(ISERROR(SEARCH("PushLeft WC",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="PushLeft">
+    <cfRule type="containsText" dxfId="30" priority="13" operator="containsText" text="PushLeft">
       <formula>NOT(ISERROR(SEARCH("PushLeft",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="14" stopIfTrue="1" operator="containsText" text="PushRight WC">
+    <cfRule type="containsText" dxfId="29" priority="14" stopIfTrue="1" operator="containsText" text="PushRight WC">
       <formula>NOT(ISERROR(SEARCH("PushRight WC",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="15" operator="containsText" text="PushRight">
+    <cfRule type="containsText" dxfId="28" priority="15" operator="containsText" text="PushRight">
       <formula>NOT(ISERROR(SEARCH("PushRight",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="16" operator="containsText" text="conflict">
+    <cfRule type="containsText" dxfId="27" priority="16" operator="containsText" text="conflict">
       <formula>NOT(ISERROR(SEARCH("conflict",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:I14">
-    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="skip">
+    <cfRule type="containsText" dxfId="26" priority="8" operator="containsText" text="skip">
       <formula>NOT(ISERROR(SEARCH("skip",B11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="9" operator="containsText" text="WC=LT">
+    <cfRule type="containsText" dxfId="25" priority="9" operator="containsText" text="WC=LT">
       <formula>NOT(ISERROR(SEARCH("WC=LT",B11)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Month panel, MonthView working
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neubu\Source\Repos\TimekeeperWPF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neubu\source\repos\TimekeeperWPF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96948C5-F6DF-4252-A8DF-F107D269A2A7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D260151D-5E99-4991-883E-7FAE6FE2EDF6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24930" windowHeight="12330" tabRatio="775" xr2:uid="{B08B66F6-8B10-48BD-8CBC-92B4F4D60D54}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="690">
   <si>
     <t>Feature</t>
   </si>
@@ -2204,9 +2204,6 @@
     <t>Style CalendarObjects</t>
   </si>
   <si>
-    <t>left side 10% color by state, right side 90% color by tasktype, no border</t>
-  </si>
-  <si>
     <t>YearViewModel</t>
   </si>
   <si>
@@ -2225,13 +2222,31 @@
     <t>Refactor</t>
   </si>
   <si>
-    <t>DimensionMargin</t>
-  </si>
-  <si>
-    <t>Like text margin, a top bar that indicates the dimension</t>
-  </si>
-  <si>
     <t>Toggle show cell lines</t>
+  </si>
+  <si>
+    <t>LINQ to XML</t>
+  </si>
+  <si>
+    <t>Is this for local file?</t>
+  </si>
+  <si>
+    <t>July works? But June is messed up? CalendarTaskObjects placed weird</t>
+  </si>
+  <si>
+    <t>left side 10% color by state, right side 90% color by tasktype, no border. Use Grids and rectangles.</t>
+  </si>
+  <si>
+    <t>compound orientation modes</t>
+  </si>
+  <si>
+    <t>Horizontal-Horizontal: Dates are left to right, Time is left to right. Vertical-Vertical: Dates are top to bottom, Time is top to bottom</t>
+  </si>
+  <si>
+    <t>Margins</t>
+  </si>
+  <si>
+    <t>DimensionMargin: Like text margin, a top bar that indicates the dimension. Cell Margins: space between rows and columns respecting orientations.</t>
   </si>
 </sst>
 </file>
@@ -3037,7 +3052,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="108">
+  <dxfs count="109">
     <dxf>
       <fill>
         <patternFill>
@@ -3313,7 +3328,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4448,15 +4470,15 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="4" xr9:uid="{5F0E2908-E7EC-43FB-9BBB-CB014E9A6F67}">
-      <tableStyleElement type="wholeTable" dxfId="107"/>
-      <tableStyleElement type="headerRow" dxfId="106"/>
-      <tableStyleElement type="firstColumn" dxfId="105"/>
+      <tableStyleElement type="wholeTable" dxfId="108"/>
+      <tableStyleElement type="headerRow" dxfId="107"/>
+      <tableStyleElement type="firstColumn" dxfId="106"/>
       <tableStyleElement type="firstRowStripe" size="2"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="3" xr9:uid="{A53ADC7C-9332-4916-9ACB-0EFC07D28AC6}">
-      <tableStyleElement type="wholeTable" dxfId="104"/>
-      <tableStyleElement type="headerRow" dxfId="103"/>
-      <tableStyleElement type="secondRowStripe" dxfId="102"/>
+      <tableStyleElement type="wholeTable" dxfId="105"/>
+      <tableStyleElement type="headerRow" dxfId="104"/>
+      <tableStyleElement type="secondRowStripe" dxfId="103"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -4765,112 +4787,112 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D212" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
-  <autoFilter ref="A1:D212" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D215" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
+  <autoFilter ref="A1:D215" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="99"/>
-    <tableColumn id="6" xr3:uid="{1FFE88A6-F499-42FB-A3F4-F5BDCD9D0CF0}" name="Done" dataDxfId="98"/>
-    <tableColumn id="2" xr3:uid="{75DC89E8-11B6-4EA2-BBEB-7D8F4C2B75D4}" name="Type" dataDxfId="97"/>
-    <tableColumn id="5" xr3:uid="{65384592-5F41-4A06-A57C-FE71C87B4BDD}" name="Notes" dataDxfId="96"/>
+    <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="100"/>
+    <tableColumn id="6" xr3:uid="{1FFE88A6-F499-42FB-A3F4-F5BDCD9D0CF0}" name="Done" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{75DC89E8-11B6-4EA2-BBEB-7D8F4C2B75D4}" name="Type" dataDxfId="98"/>
+    <tableColumn id="5" xr3:uid="{65384592-5F41-4A06-A57C-FE71C87B4BDD}" name="Notes" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F572A93C-B296-47BB-A2B7-E8D930E92020}" name="Table4" displayName="Table4" ref="A1:C77" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94" tableBorderDxfId="93">
-  <autoFilter ref="A1:C77" xr:uid="{5B5CE518-BB75-408C-8F1B-EE90C29E48F3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F572A93C-B296-47BB-A2B7-E8D930E92020}" name="Table4" displayName="Table4" ref="A1:C78" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95" tableBorderDxfId="94">
+  <autoFilter ref="A1:C78" xr:uid="{5B5CE518-BB75-408C-8F1B-EE90C29E48F3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2EF2C0F2-7D81-49C3-B8A7-E25CCB336A17}" name="Column1" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{FCC47FF7-6739-4E5E-9E09-E5EAD7161467}" name="Column2" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{3079BD65-A18D-4106-9386-B084236E0CE0}" name="Column3" dataDxfId="90"/>
+    <tableColumn id="1" xr3:uid="{2EF2C0F2-7D81-49C3-B8A7-E25CCB336A17}" name="Column1" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{FCC47FF7-6739-4E5E-9E09-E5EAD7161467}" name="Column2" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{3079BD65-A18D-4106-9386-B084236E0CE0}" name="Column3" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E4DD08F2-9CC2-46CC-93EE-E01A4DBC8EEE}" name="Table5" displayName="Table5" ref="A1:H8" totalsRowShown="0" headerRowDxfId="89" dataDxfId="87" headerRowBorderDxfId="88" tableBorderDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E4DD08F2-9CC2-46CC-93EE-E01A4DBC8EEE}" name="Table5" displayName="Table5" ref="A1:H8" totalsRowShown="0" headerRowDxfId="90" dataDxfId="88" headerRowBorderDxfId="89" tableBorderDxfId="87">
   <autoFilter ref="A1:H8" xr:uid="{9EF71295-67E3-4AA7-981B-99814F9C00D6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5F56F396-ECBF-4022-A747-BB6579150BC5}" name="Previous" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{52DF5424-7715-4094-9055-254252166B84}" name="CI Start_x000a_in Z" dataDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{4BF25F2B-3788-4EC0-877F-738CFB7416BD}" name="CI End_x000a_in Z" dataDxfId="83"/>
-    <tableColumn id="4" xr3:uid="{3D1264CD-7DED-47FE-9A26-02FAA9BC34AE}" name="CI Start_x000a_out Z" dataDxfId="82"/>
-    <tableColumn id="5" xr3:uid="{91478E3E-F2EC-42B9-9CAC-61EA2AD657CB}" name="CI End_x000a_out Z" dataDxfId="81"/>
-    <tableColumn id="6" xr3:uid="{BD45968E-F796-4835-9D67-3627C99D24EC}" name="Z Start" dataDxfId="80"/>
-    <tableColumn id="7" xr3:uid="{3B4EE896-0831-43E7-8AE0-49A3476BEA97}" name="Z End" dataDxfId="79"/>
-    <tableColumn id="8" xr3:uid="{D4DAA8AA-8B7A-4978-8C26-61D2C9036856}" name="P End" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{5F56F396-ECBF-4022-A747-BB6579150BC5}" name="Previous" dataDxfId="86"/>
+    <tableColumn id="2" xr3:uid="{52DF5424-7715-4094-9055-254252166B84}" name="CI Start_x000a_in Z" dataDxfId="85"/>
+    <tableColumn id="3" xr3:uid="{4BF25F2B-3788-4EC0-877F-738CFB7416BD}" name="CI End_x000a_in Z" dataDxfId="84"/>
+    <tableColumn id="4" xr3:uid="{3D1264CD-7DED-47FE-9A26-02FAA9BC34AE}" name="CI Start_x000a_out Z" dataDxfId="83"/>
+    <tableColumn id="5" xr3:uid="{91478E3E-F2EC-42B9-9CAC-61EA2AD657CB}" name="CI End_x000a_out Z" dataDxfId="82"/>
+    <tableColumn id="6" xr3:uid="{BD45968E-F796-4835-9D67-3627C99D24EC}" name="Z Start" dataDxfId="81"/>
+    <tableColumn id="7" xr3:uid="{3B4EE896-0831-43E7-8AE0-49A3476BEA97}" name="Z End" dataDxfId="80"/>
+    <tableColumn id="8" xr3:uid="{D4DAA8AA-8B7A-4978-8C26-61D2C9036856}" name="P End" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC6FE9AE-35E3-4705-A142-315DB9D43B3A}" name="Table3" displayName="Table3" ref="A1:A117" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC6FE9AE-35E3-4705-A142-315DB9D43B3A}" name="Table3" displayName="Table3" ref="A1:A117" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <autoFilter ref="A1:A117" xr:uid="{A2F7B623-DE53-4896-BDD6-CCC38D4467C3}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0C8999A5-1CD8-483C-A3BB-7AD00E0E2478}" name="Collision Theory" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{0C8999A5-1CD8-483C-A3BB-7AD00E0E2478}" name="Collision Theory" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67135CB1-5074-4EBE-BD9A-48C30A4CB81B}" name="Table2" displayName="Table2" ref="A1:E5" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67135CB1-5074-4EBE-BD9A-48C30A4CB81B}" name="Table2" displayName="Table2" ref="A1:E5" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74" tableBorderDxfId="73">
   <autoFilter ref="A1:E5" xr:uid="{B388395A-7532-4521-958E-47A4C8955AF2}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{70C2C4E6-CAF6-425B-8E04-929D489EC9D7}" name="Determine L, R_x000a_Step1" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{2FE5E346-C794-4C60-92C1-0865C7DF44B2}" name="C2.LT_x000a_C2.RT" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{D05D7189-86A2-4E66-978C-200C858C620C}" name="C2.LT null_x000a_C2.RT" dataDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{9D36A042-6482-4DEE-A827-BCFC97E3E6B9}" name="C2.LT_x000a_C2.RT null" dataDxfId="68"/>
-    <tableColumn id="5" xr3:uid="{DCA50F46-3DCF-4728-AFF9-64F17E91077A}" name="C2.LT null_x000a_C2.RT null" dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{70C2C4E6-CAF6-425B-8E04-929D489EC9D7}" name="Determine L, R_x000a_Step1" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{2FE5E346-C794-4C60-92C1-0865C7DF44B2}" name="C2.LT_x000a_C2.RT" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{D05D7189-86A2-4E66-978C-200C858C620C}" name="C2.LT null_x000a_C2.RT" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{9D36A042-6482-4DEE-A827-BCFC97E3E6B9}" name="C2.LT_x000a_C2.RT null" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{DCA50F46-3DCF-4728-AFF9-64F17E91077A}" name="C2.LT null_x000a_C2.RT null" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1D0690DC-ACA6-40D8-866A-1D8C44DE4AC8}" name="Table7" displayName="Table7" ref="A7:D8" totalsRowShown="0" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1D0690DC-ACA6-40D8-866A-1D8C44DE4AC8}" name="Table7" displayName="Table7" ref="A7:D8" totalsRowShown="0" tableBorderDxfId="67">
   <autoFilter ref="A7:D8" xr:uid="{ACCFA163-AAF6-4628-ADE5-97056064C206}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9757D096-D900-42A9-8E11-C4ACA310AE56}" name="Determine L, R_x000a_Step2" dataDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{C3069A29-6915-46B5-977A-E175A6DEB3D2}" name="C1.S &lt; C2.S" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{12A8AD37-B3F9-4A8B-9EA6-A0F6EB34B35A}" name="C1.S == C2.S" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{7A2BF950-BBF5-494B-8BCE-AD358D4349E2}" name="C1.S &gt; C2.S" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{9757D096-D900-42A9-8E11-C4ACA310AE56}" name="Determine L, R_x000a_Step2" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{C3069A29-6915-46B5-977A-E175A6DEB3D2}" name="C1.S &lt; C2.S" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{12A8AD37-B3F9-4A8B-9EA6-A0F6EB34B35A}" name="C1.S == C2.S" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{7A2BF950-BBF5-494B-8BCE-AD358D4349E2}" name="C1.S &gt; C2.S" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BEABA309-E652-49AF-B0CA-0DBB8732C3D3}" name="Table6" displayName="Table6" ref="A1:N8" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BEABA309-E652-49AF-B0CA-0DBB8732C3D3}" name="Table6" displayName="Table6" ref="A1:N8" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="A1:N8" xr:uid="{3AB9159B-B403-4CC8-8649-2A74831EFA39}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{72C9A77E-AFBC-404B-A7F6-E681135EDAE9}" name="Redistribute_x000a_Collision_x000a_… T L ∩ R T …" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{7B5E19F2-C874-4B16-82C8-FA89018E0F3A}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="58"/>
-    <tableColumn id="13" xr3:uid="{140BB756-BA0B-42B4-96AC-20E496CA56A3}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{E21AAA4F-92B4-436C-B55B-4DFD07C4BE29}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="56"/>
-    <tableColumn id="14" xr3:uid="{7026FFA9-3F08-448A-86A1-E71772461B72}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="55"/>
-    <tableColumn id="12" xr3:uid="{59C7730E-CD9C-445B-A9A4-AEE7F50B376A}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="54"/>
-    <tableColumn id="11" xr3:uid="{6F38818E-A5E5-47C6-AFD4-C58CF1FD3DD5}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="53"/>
-    <tableColumn id="8" xr3:uid="{DFFA66D7-E0E3-4911-BECE-C58139CDD28D}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{C2DC972A-AC9A-4140-A684-443F75AEE447}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{833A1012-7AE2-431D-82C0-B7CB5960C752}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="50"/>
-    <tableColumn id="9" xr3:uid="{43D8BEE4-A2A2-4CFF-9608-9E5B08D746D9}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{0599BB19-BD4F-4332-92DE-B1E045C56EEF}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="48"/>
-    <tableColumn id="10" xr3:uid="{3C3A9FF5-1451-4E38-87EA-C000A51EC5B5}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{D413EC93-83CF-4773-9080-8AB9148DFA4E}" name="R.S🔒" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{72C9A77E-AFBC-404B-A7F6-E681135EDAE9}" name="Redistribute_x000a_Collision_x000a_… T L ∩ R T …" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{7B5E19F2-C874-4B16-82C8-FA89018E0F3A}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="59"/>
+    <tableColumn id="13" xr3:uid="{140BB756-BA0B-42B4-96AC-20E496CA56A3}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{E21AAA4F-92B4-436C-B55B-4DFD07C4BE29}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="57"/>
+    <tableColumn id="14" xr3:uid="{7026FFA9-3F08-448A-86A1-E71772461B72}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="56"/>
+    <tableColumn id="12" xr3:uid="{59C7730E-CD9C-445B-A9A4-AEE7F50B376A}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="55"/>
+    <tableColumn id="11" xr3:uid="{6F38818E-A5E5-47C6-AFD4-C58CF1FD3DD5}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{DFFA66D7-E0E3-4911-BECE-C58139CDD28D}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="53"/>
+    <tableColumn id="7" xr3:uid="{C2DC972A-AC9A-4140-A684-443F75AEE447}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{833A1012-7AE2-431D-82C0-B7CB5960C752}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{43D8BEE4-A2A2-4CFF-9608-9E5B08D746D9}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{0599BB19-BD4F-4332-92DE-B1E045C56EEF}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="49"/>
+    <tableColumn id="10" xr3:uid="{3C3A9FF5-1451-4E38-87EA-C000A51EC5B5}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{D413EC93-83CF-4773-9080-8AB9148DFA4E}" name="R.S🔒" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BB600374-B6B9-40D7-85BD-757E0CB6012B}" name="Table8" displayName="Table8" ref="A10:I14" totalsRowShown="0" headerRowDxfId="45" tableBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BB600374-B6B9-40D7-85BD-757E0CB6012B}" name="Table8" displayName="Table8" ref="A10:I14" totalsRowShown="0" headerRowDxfId="46" tableBorderDxfId="45">
   <autoFilter ref="A10:I14" xr:uid="{CC633682-C369-475E-BC03-B121AB91AB17}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{78CD584E-A9D4-40D7-9D09-CF0EF6806B2D}" name="GetPushData" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{78CD584E-A9D4-40D7-9D09-CF0EF6806B2D}" name="GetPushData" dataDxfId="44"/>
     <tableColumn id="2" xr3:uid="{A08CEA82-1CE9-4441-B0EF-0A975D8FE65A}" name="LT.CanReDist=T_x000a_LT.Limited=T_x000a_LT &lt; WC"/>
     <tableColumn id="6" xr3:uid="{F6036D13-DB0F-4AF8-A1E6-30BCCEB2A5F3}" name="LT.CanReDist=T_x000a_LT.Limited=T_x000a_LT &gt;= WC"/>
     <tableColumn id="4" xr3:uid="{B3ED7712-7A0A-4E68-A538-F34B63335364}" name="LT.CanReDist=T_x000a_LT.Limited=F_x000a_LT &lt; WC"/>
@@ -4885,14 +4907,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2B1B7CE4-90F7-42CA-B974-855205A0C605}" name="Table11" displayName="Table11" ref="A2:E12" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2B1B7CE4-90F7-42CA-B974-855205A0C605}" name="Table11" displayName="Table11" ref="A2:E12" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A2:E12" xr:uid="{78FF5B0B-0912-499F-8F6A-339F3CEEC95F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F251C872-2A1D-42A0-994A-2DFC09D7C047}" name="State" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{F251C872-2A1D-42A0-994A-2DFC09D7C047}" name="State" dataDxfId="41"/>
     <tableColumn id="2" xr3:uid="{AB62CF60-B9F3-442C-A4D1-2FC89B02B851}" name="Border Color"/>
-    <tableColumn id="3" xr3:uid="{E3035B58-4720-4F96-BC43-0FE1566CB1AC}" name="Happens When" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{64A950F1-3FCD-413C-8376-9DAD13362BEC}" name="Details" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{6FB2B197-5E34-46A9-BA2C-CE95765F93BA}" name="Leads to" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{E3035B58-4720-4F96-BC43-0FE1566CB1AC}" name="Happens When" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{64A950F1-3FCD-413C-8376-9DAD13362BEC}" name="Details" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{6FB2B197-5E34-46A9-BA2C-CE95765F93BA}" name="Leads to" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5195,10 +5217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:H212"/>
+  <dimension ref="A1:H214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4"/>
@@ -6405,7 +6427,10 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="7" t="s">
-        <v>681</v>
+        <v>680</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="C119" s="9" t="s">
         <v>613</v>
@@ -6413,21 +6438,21 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="7" t="s">
-        <v>682</v>
+        <v>55</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>672</v>
+        <v>23</v>
       </c>
       <c r="C120" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D120" s="8" t="s">
-        <v>683</v>
-      </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="7" t="s">
-        <v>684</v>
+        <v>25</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="C121" s="9" t="s">
         <v>613</v>
@@ -6437,53 +6462,68 @@
       <c r="A122" s="7" t="s">
         <v>140</v>
       </c>
+      <c r="B122" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="C122" s="9" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="7" t="s">
-        <v>55</v>
+        <v>665</v>
       </c>
       <c r="B123" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>613</v>
+        <v>565</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="7" t="s">
-        <v>25</v>
+        <v>674</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4">
+        <v>616</v>
+      </c>
+      <c r="D124" s="8" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="28.8">
+      <c r="A125" s="7" t="s">
+        <v>686</v>
+      </c>
       <c r="C125" s="9" t="s">
         <v>613</v>
       </c>
+      <c r="D125" s="8" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="7" t="s">
-        <v>141</v>
+        <v>681</v>
       </c>
       <c r="C126" s="9" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" ht="28.8">
       <c r="A127" s="7" t="s">
-        <v>676</v>
+        <v>688</v>
       </c>
       <c r="C127" s="9" t="s">
         <v>613</v>
       </c>
+      <c r="D127" s="8" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="7" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="C128" s="9" t="s">
         <v>613</v>
@@ -6491,7 +6531,7 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="7" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C129" s="9" t="s">
         <v>613</v>
@@ -6499,709 +6539,709 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="7" t="s">
-        <v>328</v>
+        <v>72</v>
       </c>
       <c r="C130" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D130" s="8" t="s">
-        <v>327</v>
-      </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="7" t="s">
-        <v>83</v>
+        <v>676</v>
       </c>
       <c r="C131" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D131" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="72">
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" s="7" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="C132" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="57.6">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" s="7" t="s">
-        <v>341</v>
+        <v>83</v>
       </c>
       <c r="C133" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="72">
       <c r="A134" s="7" t="s">
-        <v>199</v>
+        <v>339</v>
       </c>
       <c r="C134" s="9" t="s">
         <v>613</v>
       </c>
+      <c r="D134" s="8" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="135" spans="1:4" ht="57.6">
       <c r="A135" s="7" t="s">
-        <v>291</v>
+        <v>341</v>
       </c>
       <c r="C135" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C136" s="9" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="57.6">
+      <c r="A137" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C137" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="D137" s="8" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="C136" s="9" t="s">
+      <c r="C138" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D136" s="8" t="s">
+      <c r="D138" s="8" t="s">
         <v>293</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="A137" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C137" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D137" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
-      <c r="A138" s="110" t="s">
-        <v>629</v>
-      </c>
-      <c r="C138" s="9" t="s">
-        <v>625</v>
-      </c>
-      <c r="D138" s="8" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="7" t="s">
-        <v>6</v>
+        <v>129</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>0</v>
+        <v>615</v>
+      </c>
+      <c r="D139" s="8" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="140" spans="1:4">
-      <c r="A140" s="7" t="s">
-        <v>7</v>
+      <c r="A140" s="110" t="s">
+        <v>629</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>0</v>
+        <v>625</v>
+      </c>
+      <c r="D140" s="8" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C141" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D141" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="28.8">
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" s="7" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="C142" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D142" s="8" t="s">
-        <v>201</v>
-      </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C143" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:4">
-      <c r="A144" s="110" t="s">
-        <v>630</v>
+      <c r="D143" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="28.8">
+      <c r="A144" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>625</v>
+        <v>0</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>632</v>
+        <v>201</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C145" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="110" t="s">
+        <v>630</v>
+      </c>
+      <c r="C146" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="D146" s="8" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C145" s="9" t="s">
+      <c r="C147" s="9" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="43.2">
-      <c r="A146" s="7" t="s">
+    <row r="148" spans="1:4" ht="43.2">
+      <c r="A148" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="C146" s="9" t="s">
+      <c r="C148" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D146" s="8" t="s">
+      <c r="D148" s="8" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="28.8">
-      <c r="A147" s="7" t="s">
+    <row r="149" spans="1:4" ht="28.8">
+      <c r="A149" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="B147" s="9" t="s">
+      <c r="B149" s="9" t="s">
         <v>618</v>
       </c>
-      <c r="C147" s="9" t="s">
+      <c r="C149" s="9" t="s">
         <v>615</v>
       </c>
-      <c r="D147" s="8" t="s">
+      <c r="D149" s="8" t="s">
         <v>666</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4">
-      <c r="A148" s="7" t="s">
-        <v>621</v>
-      </c>
-      <c r="D148" s="8" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4">
-      <c r="A149" s="7" t="s">
-        <v>603</v>
-      </c>
-      <c r="C149" s="9" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C150" s="9" t="s">
-        <v>0</v>
+        <v>621</v>
+      </c>
+      <c r="D150" s="8" t="s">
+        <v>622</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="7" t="s">
-        <v>35</v>
+        <v>603</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="28.8">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
       <c r="A152" s="7" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C152" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D152" s="8" t="s">
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="28.8">
+      <c r="A154" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C154" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D154" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="28.8">
-      <c r="A153" s="7" t="s">
+    <row r="155" spans="1:4" ht="28.8">
+      <c r="A155" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="C153" s="9" t="s">
+      <c r="C155" s="9" t="s">
         <v>615</v>
       </c>
-      <c r="D153" s="8" t="s">
+      <c r="D155" s="8" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="43.2">
-      <c r="A154" s="7" t="s">
+    <row r="156" spans="1:4" ht="43.2">
+      <c r="A156" s="7" t="s">
         <v>329</v>
-      </c>
-      <c r="C154" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D154" s="8" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4">
-      <c r="A155" s="7" t="s">
-        <v>602</v>
-      </c>
-      <c r="C155" s="9" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4">
-      <c r="A156" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="C156" s="9" t="s">
         <v>615</v>
       </c>
       <c r="D156" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="28.8">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
       <c r="A157" s="7" t="s">
-        <v>146</v>
+        <v>602</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D157" s="8" t="s">
-        <v>148</v>
+        <v>613</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="D158" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="28.8">
+      <c r="A159" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C159" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="D159" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="B158" s="9" t="s">
-        <v>618</v>
-      </c>
-      <c r="C158" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D158" s="8" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4">
-      <c r="A159" s="7" t="s">
-        <v>606</v>
-      </c>
-      <c r="C159" s="9" t="s">
-        <v>613</v>
-      </c>
-      <c r="D159" s="8" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" ht="28.8">
-      <c r="A160" s="7" t="s">
-        <v>344</v>
       </c>
       <c r="B160" s="9" t="s">
         <v>618</v>
       </c>
+      <c r="C160" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="D160" s="8" t="s">
-        <v>345</v>
+        <v>639</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="7" t="s">
-        <v>333</v>
+        <v>606</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4">
+        <v>613</v>
+      </c>
+      <c r="D161" s="8" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="28.8">
       <c r="A162" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C162" s="9" t="s">
-        <v>614</v>
+        <v>344</v>
+      </c>
+      <c r="B162" s="9" t="s">
+        <v>618</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>86</v>
+        <v>345</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="7" t="s">
-        <v>5</v>
+        <v>333</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D163" s="8" t="s">
-        <v>186</v>
+        <v>614</v>
       </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C164" s="9" t="s">
+        <v>614</v>
+      </c>
+      <c r="D164" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C165" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D165" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="7" t="s">
         <v>609</v>
       </c>
-      <c r="C164" s="9" t="s">
+      <c r="C166" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D164" s="8" t="s">
+      <c r="D166" s="8" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="28.8">
-      <c r="A165" s="7" t="s">
+    <row r="167" spans="1:4" ht="28.8">
+      <c r="A167" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="C165" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D165" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" ht="43.2">
-      <c r="A166" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C166" s="9" t="s">
-        <v>613</v>
-      </c>
-      <c r="D166" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4">
-      <c r="A167" s="7" t="s">
-        <v>136</v>
       </c>
       <c r="C167" s="9" t="s">
         <v>615</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="43.2">
       <c r="A168" s="7" t="s">
-        <v>376</v>
+        <v>142</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>615</v>
+        <v>613</v>
+      </c>
+      <c r="D168" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="7" t="s">
-        <v>81</v>
+        <v>136</v>
       </c>
       <c r="C169" s="9" t="s">
         <v>615</v>
       </c>
       <c r="D169" s="8" t="s">
-        <v>82</v>
+        <v>135</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="7" t="s">
-        <v>496</v>
+        <v>376</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="A171" s="7" t="s">
-        <v>497</v>
+        <v>81</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>613</v>
+        <v>615</v>
+      </c>
+      <c r="D171" s="8" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" s="7" t="s">
-        <v>317</v>
+        <v>496</v>
       </c>
       <c r="C172" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D172" s="8" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" s="7" t="s">
-        <v>58</v>
+        <v>497</v>
       </c>
       <c r="C173" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D173" s="8" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" s="7" t="s">
-        <v>346</v>
+        <v>317</v>
       </c>
       <c r="C174" s="9" t="s">
         <v>613</v>
       </c>
+      <c r="D174" s="8" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" s="7" t="s">
-        <v>205</v>
+        <v>58</v>
       </c>
       <c r="C175" s="9" t="s">
         <v>613</v>
       </c>
+      <c r="D175" s="8" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B176" s="9" t="s">
-        <v>618</v>
-      </c>
-      <c r="D176" s="8" t="s">
-        <v>91</v>
+        <v>346</v>
+      </c>
+      <c r="C176" s="9" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="7" t="s">
-        <v>123</v>
+        <v>205</v>
       </c>
       <c r="C177" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D177" s="8" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" s="7" t="s">
-        <v>641</v>
-      </c>
-      <c r="C178" s="9" t="s">
-        <v>613</v>
+        <v>90</v>
+      </c>
+      <c r="B178" s="9" t="s">
+        <v>618</v>
       </c>
       <c r="D178" s="8" t="s">
-        <v>642</v>
+        <v>91</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" s="7" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>0</v>
+        <v>613</v>
+      </c>
+      <c r="D179" s="8" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="7" t="s">
-        <v>66</v>
+        <v>641</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>0</v>
+        <v>613</v>
+      </c>
+      <c r="D180" s="8" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" s="7" t="s">
-        <v>241</v>
+        <v>74</v>
       </c>
       <c r="C181" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D181" s="8" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" ht="43.2">
+    </row>
+    <row r="182" spans="1:4">
       <c r="A182" s="7" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="C182" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D182" s="8" t="s">
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C183" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D183" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" ht="43.2">
+      <c r="A184" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C184" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D184" s="8" t="s">
         <v>348</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" ht="28.8">
-      <c r="A183" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C183" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D183" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" ht="28.8">
-      <c r="A184" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C184" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D184" s="8" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="28.8">
       <c r="A185" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C185" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="D185" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" ht="28.8">
+      <c r="A186" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C186" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="D186" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" ht="28.8">
+      <c r="A187" s="7" t="s">
         <v>436</v>
       </c>
-      <c r="C185" s="9" t="s">
+      <c r="C187" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D185" s="8" t="s">
+      <c r="D187" s="8" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="43.2">
-      <c r="A186" s="7" t="s">
+    <row r="188" spans="1:4" ht="43.2">
+      <c r="A188" s="7" t="s">
         <v>500</v>
       </c>
-      <c r="C186" s="9" t="s">
+      <c r="C188" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D186" s="8" t="s">
+      <c r="D188" s="8" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="43.2">
-      <c r="A187" s="7" t="s">
+    <row r="189" spans="1:4" ht="43.2">
+      <c r="A189" s="7" t="s">
         <v>145</v>
-      </c>
-      <c r="C187" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D187" s="8" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4">
-      <c r="A188" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C188" s="9" t="s">
-        <v>613</v>
-      </c>
-      <c r="D188" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4">
-      <c r="A189" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="C189" s="9" t="s">
         <v>615</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" ht="43.2">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
       <c r="A190" s="7" t="s">
-        <v>217</v>
+        <v>44</v>
       </c>
       <c r="C190" s="9" t="s">
-        <v>0</v>
+        <v>613</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>218</v>
+        <v>45</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="7" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="C191" s="9" t="s">
-        <v>0</v>
+        <v>615</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="43.2">
       <c r="A192" s="7" t="s">
-        <v>377</v>
+        <v>217</v>
       </c>
       <c r="C192" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>378</v>
+        <v>218</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193" s="7" t="s">
-        <v>377</v>
+        <v>219</v>
       </c>
       <c r="C193" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D193" s="8" t="s">
-        <v>640</v>
+        <v>220</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C194" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B195" s="9" t="s">
-        <v>618</v>
+        <v>377</v>
+      </c>
+      <c r="C195" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D195" s="8" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="B196" s="9" t="s">
-        <v>618</v>
+        <v>379</v>
       </c>
       <c r="C196" s="9" t="s">
-        <v>615</v>
+        <v>0</v>
+      </c>
+      <c r="D196" s="8" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C197" s="9" t="s">
-        <v>0</v>
+        <v>76</v>
+      </c>
+      <c r="B197" s="9" t="s">
+        <v>618</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198" s="7" t="s">
-        <v>96</v>
+        <v>372</v>
+      </c>
+      <c r="B198" s="9" t="s">
+        <v>618</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>0</v>
+        <v>615</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" s="7" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C199" s="9" t="s">
         <v>0</v>
@@ -7209,23 +7249,23 @@
     </row>
     <row r="200" spans="1:4">
       <c r="A200" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>616</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:4">
       <c r="A201" s="7" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C201" s="9" t="s">
-        <v>616</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" s="7" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="C202" s="9" t="s">
         <v>616</v>
@@ -7233,26 +7273,23 @@
     </row>
     <row r="203" spans="1:4">
       <c r="A203" s="7" t="s">
-        <v>484</v>
+        <v>56</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>0</v>
+        <v>616</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" s="7" t="s">
-        <v>566</v>
+        <v>57</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D204" s="8" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
     </row>
     <row r="205" spans="1:4">
       <c r="A205" s="7" t="s">
-        <v>633</v>
+        <v>484</v>
       </c>
       <c r="C205" s="9" t="s">
         <v>0</v>
@@ -7260,15 +7297,18 @@
     </row>
     <row r="206" spans="1:4">
       <c r="A206" s="7" t="s">
-        <v>635</v>
+        <v>566</v>
       </c>
       <c r="C206" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="D206" s="8" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" s="7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C207" s="9" t="s">
         <v>0</v>
@@ -7276,51 +7316,67 @@
     </row>
     <row r="208" spans="1:4">
       <c r="A208" s="7" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>613</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" s="7" t="s">
-        <v>657</v>
+        <v>634</v>
       </c>
       <c r="C209" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D209" s="8" t="s">
-        <v>658</v>
-      </c>
     </row>
     <row r="210" spans="1:4">
       <c r="A210" s="7" t="s">
-        <v>668</v>
+        <v>636</v>
       </c>
       <c r="C210" s="9" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="211" spans="1:4">
       <c r="A211" s="7" t="s">
-        <v>674</v>
+        <v>657</v>
       </c>
       <c r="C211" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D211" s="8" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212" s="7" t="s">
+        <v>668</v>
+      </c>
+      <c r="C212" s="9" t="s">
         <v>616</v>
       </c>
-      <c r="D211" s="8" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" ht="43.2">
-      <c r="A212" s="7" t="s">
+    </row>
+    <row r="213" spans="1:4" ht="43.2">
+      <c r="A213" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="C213" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="D213" s="8" t="s">
         <v>678</v>
       </c>
-      <c r="C212" s="9" t="s">
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214" s="7" t="s">
+        <v>682</v>
+      </c>
+      <c r="C214" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D212" s="8" t="s">
-        <v>679</v>
+      <c r="D214" s="8" t="s">
+        <v>683</v>
       </c>
     </row>
   </sheetData>
@@ -7464,10 +7520,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F160C7F-FB27-4F84-8171-6D9C64590D99}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8306,7 +8362,9 @@
       <c r="A76" s="61" t="s">
         <v>663</v>
       </c>
-      <c r="B76" s="60"/>
+      <c r="B76" s="60" t="s">
+        <v>23</v>
+      </c>
       <c r="C76" s="60" t="s">
         <v>673</v>
       </c>
@@ -8319,11 +8377,22 @@
         <v>672</v>
       </c>
       <c r="C77" s="60" t="s">
-        <v>680</v>
+        <v>679</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="B78" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="C78" s="60" t="s">
+        <v>684</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B77">
+  <conditionalFormatting sqref="B2:B78">
     <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="Triaged">
       <formula>NOT(ISERROR(SEARCH("Triaged",B2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Horizontal time in week panel with single cell
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neubu\source\repos\TimekeeperWPF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neubu\Source\Repos\TimekeeperWPF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD7F494-8C3C-4974-A5A8-1B963E35DB8C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AF08AE-0F98-40F5-975D-9C58B4EBA04B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24930" windowHeight="12330" tabRatio="775" xr2:uid="{B08B66F6-8B10-48BD-8CBC-92B4F4D60D54}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="699">
   <si>
     <t>Feature</t>
   </si>
@@ -2262,6 +2262,18 @@
   </si>
   <si>
     <t>Horizontal-Horizontal: Dates are left to right, Time is left to right. Vertical-Vertical: Dates are top to bottom, Time is top to bottom. SecondaryOrientation: go through everything that checks orientation and modify for secondaryorientation</t>
+  </si>
+  <si>
+    <t>Month orientation modes</t>
+  </si>
+  <si>
+    <t>force horizontal date only, allow vertical or horizontal time. Do horizontal time with continuous mode.</t>
+  </si>
+  <si>
+    <t>Serialization to file</t>
+  </si>
+  <si>
+    <t>Serialize options for persistence between sessions. Save what view we were last using, save state of all options.</t>
   </si>
 </sst>
 </file>
@@ -3067,7 +3079,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="106">
+  <dxfs count="109">
     <dxf>
       <fill>
         <patternFill>
@@ -3327,6 +3339,30 @@
       <fill>
         <patternFill>
           <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4461,15 +4497,15 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="4" xr9:uid="{5F0E2908-E7EC-43FB-9BBB-CB014E9A6F67}">
-      <tableStyleElement type="wholeTable" dxfId="105"/>
-      <tableStyleElement type="headerRow" dxfId="104"/>
-      <tableStyleElement type="firstColumn" dxfId="103"/>
+      <tableStyleElement type="wholeTable" dxfId="108"/>
+      <tableStyleElement type="headerRow" dxfId="107"/>
+      <tableStyleElement type="firstColumn" dxfId="106"/>
       <tableStyleElement type="firstRowStripe" size="2"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="3" xr9:uid="{A53ADC7C-9332-4916-9ACB-0EFC07D28AC6}">
-      <tableStyleElement type="wholeTable" dxfId="102"/>
-      <tableStyleElement type="headerRow" dxfId="101"/>
-      <tableStyleElement type="secondRowStripe" dxfId="100"/>
+      <tableStyleElement type="wholeTable" dxfId="105"/>
+      <tableStyleElement type="headerRow" dxfId="104"/>
+      <tableStyleElement type="secondRowStripe" dxfId="103"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -4778,112 +4814,112 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D217" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
-  <autoFilter ref="A1:D217" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D220" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
+  <autoFilter ref="A1:D220" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="97"/>
-    <tableColumn id="6" xr3:uid="{1FFE88A6-F499-42FB-A3F4-F5BDCD9D0CF0}" name="Done" dataDxfId="96"/>
-    <tableColumn id="2" xr3:uid="{75DC89E8-11B6-4EA2-BBEB-7D8F4C2B75D4}" name="Type" dataDxfId="95"/>
-    <tableColumn id="5" xr3:uid="{65384592-5F41-4A06-A57C-FE71C87B4BDD}" name="Notes" dataDxfId="94"/>
+    <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="100"/>
+    <tableColumn id="6" xr3:uid="{1FFE88A6-F499-42FB-A3F4-F5BDCD9D0CF0}" name="Done" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{75DC89E8-11B6-4EA2-BBEB-7D8F4C2B75D4}" name="Type" dataDxfId="98"/>
+    <tableColumn id="5" xr3:uid="{65384592-5F41-4A06-A57C-FE71C87B4BDD}" name="Notes" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F572A93C-B296-47BB-A2B7-E8D930E92020}" name="Table4" displayName="Table4" ref="A1:C78" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92" tableBorderDxfId="91">
-  <autoFilter ref="A1:C78" xr:uid="{5B5CE518-BB75-408C-8F1B-EE90C29E48F3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F572A93C-B296-47BB-A2B7-E8D930E92020}" name="Table4" displayName="Table4" ref="A1:C79" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95" tableBorderDxfId="94">
+  <autoFilter ref="A1:C79" xr:uid="{5B5CE518-BB75-408C-8F1B-EE90C29E48F3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2EF2C0F2-7D81-49C3-B8A7-E25CCB336A17}" name="Column1" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{FCC47FF7-6739-4E5E-9E09-E5EAD7161467}" name="Column2" dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{3079BD65-A18D-4106-9386-B084236E0CE0}" name="Column3" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{2EF2C0F2-7D81-49C3-B8A7-E25CCB336A17}" name="Column1" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{FCC47FF7-6739-4E5E-9E09-E5EAD7161467}" name="Column2" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{3079BD65-A18D-4106-9386-B084236E0CE0}" name="Column3" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E4DD08F2-9CC2-46CC-93EE-E01A4DBC8EEE}" name="Table5" displayName="Table5" ref="A1:H8" totalsRowShown="0" headerRowDxfId="87" dataDxfId="85" headerRowBorderDxfId="86" tableBorderDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E4DD08F2-9CC2-46CC-93EE-E01A4DBC8EEE}" name="Table5" displayName="Table5" ref="A1:H8" totalsRowShown="0" headerRowDxfId="90" dataDxfId="88" headerRowBorderDxfId="89" tableBorderDxfId="87">
   <autoFilter ref="A1:H8" xr:uid="{9EF71295-67E3-4AA7-981B-99814F9C00D6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5F56F396-ECBF-4022-A747-BB6579150BC5}" name="Previous" dataDxfId="83"/>
-    <tableColumn id="2" xr3:uid="{52DF5424-7715-4094-9055-254252166B84}" name="CI Start_x000a_in Z" dataDxfId="82"/>
-    <tableColumn id="3" xr3:uid="{4BF25F2B-3788-4EC0-877F-738CFB7416BD}" name="CI End_x000a_in Z" dataDxfId="81"/>
-    <tableColumn id="4" xr3:uid="{3D1264CD-7DED-47FE-9A26-02FAA9BC34AE}" name="CI Start_x000a_out Z" dataDxfId="80"/>
-    <tableColumn id="5" xr3:uid="{91478E3E-F2EC-42B9-9CAC-61EA2AD657CB}" name="CI End_x000a_out Z" dataDxfId="79"/>
-    <tableColumn id="6" xr3:uid="{BD45968E-F796-4835-9D67-3627C99D24EC}" name="Z Start" dataDxfId="78"/>
-    <tableColumn id="7" xr3:uid="{3B4EE896-0831-43E7-8AE0-49A3476BEA97}" name="Z End" dataDxfId="77"/>
-    <tableColumn id="8" xr3:uid="{D4DAA8AA-8B7A-4978-8C26-61D2C9036856}" name="P End" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{5F56F396-ECBF-4022-A747-BB6579150BC5}" name="Previous" dataDxfId="86"/>
+    <tableColumn id="2" xr3:uid="{52DF5424-7715-4094-9055-254252166B84}" name="CI Start_x000a_in Z" dataDxfId="85"/>
+    <tableColumn id="3" xr3:uid="{4BF25F2B-3788-4EC0-877F-738CFB7416BD}" name="CI End_x000a_in Z" dataDxfId="84"/>
+    <tableColumn id="4" xr3:uid="{3D1264CD-7DED-47FE-9A26-02FAA9BC34AE}" name="CI Start_x000a_out Z" dataDxfId="83"/>
+    <tableColumn id="5" xr3:uid="{91478E3E-F2EC-42B9-9CAC-61EA2AD657CB}" name="CI End_x000a_out Z" dataDxfId="82"/>
+    <tableColumn id="6" xr3:uid="{BD45968E-F796-4835-9D67-3627C99D24EC}" name="Z Start" dataDxfId="81"/>
+    <tableColumn id="7" xr3:uid="{3B4EE896-0831-43E7-8AE0-49A3476BEA97}" name="Z End" dataDxfId="80"/>
+    <tableColumn id="8" xr3:uid="{D4DAA8AA-8B7A-4978-8C26-61D2C9036856}" name="P End" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC6FE9AE-35E3-4705-A142-315DB9D43B3A}" name="Table3" displayName="Table3" ref="A1:A117" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC6FE9AE-35E3-4705-A142-315DB9D43B3A}" name="Table3" displayName="Table3" ref="A1:A117" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <autoFilter ref="A1:A117" xr:uid="{A2F7B623-DE53-4896-BDD6-CCC38D4467C3}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0C8999A5-1CD8-483C-A3BB-7AD00E0E2478}" name="Collision Theory" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{0C8999A5-1CD8-483C-A3BB-7AD00E0E2478}" name="Collision Theory" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67135CB1-5074-4EBE-BD9A-48C30A4CB81B}" name="Table2" displayName="Table2" ref="A1:E5" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" tableBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67135CB1-5074-4EBE-BD9A-48C30A4CB81B}" name="Table2" displayName="Table2" ref="A1:E5" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74" tableBorderDxfId="73">
   <autoFilter ref="A1:E5" xr:uid="{B388395A-7532-4521-958E-47A4C8955AF2}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{70C2C4E6-CAF6-425B-8E04-929D489EC9D7}" name="Determine L, R_x000a_Step1" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{2FE5E346-C794-4C60-92C1-0865C7DF44B2}" name="C2.LT_x000a_C2.RT" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{D05D7189-86A2-4E66-978C-200C858C620C}" name="C2.LT null_x000a_C2.RT" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{9D36A042-6482-4DEE-A827-BCFC97E3E6B9}" name="C2.LT_x000a_C2.RT null" dataDxfId="66"/>
-    <tableColumn id="5" xr3:uid="{DCA50F46-3DCF-4728-AFF9-64F17E91077A}" name="C2.LT null_x000a_C2.RT null" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{70C2C4E6-CAF6-425B-8E04-929D489EC9D7}" name="Determine L, R_x000a_Step1" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{2FE5E346-C794-4C60-92C1-0865C7DF44B2}" name="C2.LT_x000a_C2.RT" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{D05D7189-86A2-4E66-978C-200C858C620C}" name="C2.LT null_x000a_C2.RT" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{9D36A042-6482-4DEE-A827-BCFC97E3E6B9}" name="C2.LT_x000a_C2.RT null" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{DCA50F46-3DCF-4728-AFF9-64F17E91077A}" name="C2.LT null_x000a_C2.RT null" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1D0690DC-ACA6-40D8-866A-1D8C44DE4AC8}" name="Table7" displayName="Table7" ref="A7:D8" totalsRowShown="0" tableBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1D0690DC-ACA6-40D8-866A-1D8C44DE4AC8}" name="Table7" displayName="Table7" ref="A7:D8" totalsRowShown="0" tableBorderDxfId="67">
   <autoFilter ref="A7:D8" xr:uid="{ACCFA163-AAF6-4628-ADE5-97056064C206}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9757D096-D900-42A9-8E11-C4ACA310AE56}" name="Determine L, R_x000a_Step2" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{C3069A29-6915-46B5-977A-E175A6DEB3D2}" name="C1.S &lt; C2.S" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{12A8AD37-B3F9-4A8B-9EA6-A0F6EB34B35A}" name="C1.S == C2.S" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{7A2BF950-BBF5-494B-8BCE-AD358D4349E2}" name="C1.S &gt; C2.S" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{9757D096-D900-42A9-8E11-C4ACA310AE56}" name="Determine L, R_x000a_Step2" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{C3069A29-6915-46B5-977A-E175A6DEB3D2}" name="C1.S &lt; C2.S" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{12A8AD37-B3F9-4A8B-9EA6-A0F6EB34B35A}" name="C1.S == C2.S" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{7A2BF950-BBF5-494B-8BCE-AD358D4349E2}" name="C1.S &gt; C2.S" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BEABA309-E652-49AF-B0CA-0DBB8732C3D3}" name="Table6" displayName="Table6" ref="A1:N8" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BEABA309-E652-49AF-B0CA-0DBB8732C3D3}" name="Table6" displayName="Table6" ref="A1:N8" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="A1:N8" xr:uid="{3AB9159B-B403-4CC8-8649-2A74831EFA39}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{72C9A77E-AFBC-404B-A7F6-E681135EDAE9}" name="Redistribute_x000a_Collision_x000a_… T L ∩ R T …" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{7B5E19F2-C874-4B16-82C8-FA89018E0F3A}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="56"/>
-    <tableColumn id="13" xr3:uid="{140BB756-BA0B-42B4-96AC-20E496CA56A3}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{E21AAA4F-92B4-436C-B55B-4DFD07C4BE29}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="54"/>
-    <tableColumn id="14" xr3:uid="{7026FFA9-3F08-448A-86A1-E71772461B72}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="53"/>
-    <tableColumn id="12" xr3:uid="{59C7730E-CD9C-445B-A9A4-AEE7F50B376A}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="52"/>
-    <tableColumn id="11" xr3:uid="{6F38818E-A5E5-47C6-AFD4-C58CF1FD3DD5}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="51"/>
-    <tableColumn id="8" xr3:uid="{DFFA66D7-E0E3-4911-BECE-C58139CDD28D}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{C2DC972A-AC9A-4140-A684-443F75AEE447}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{833A1012-7AE2-431D-82C0-B7CB5960C752}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="48"/>
-    <tableColumn id="9" xr3:uid="{43D8BEE4-A2A2-4CFF-9608-9E5B08D746D9}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{0599BB19-BD4F-4332-92DE-B1E045C56EEF}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="46"/>
-    <tableColumn id="10" xr3:uid="{3C3A9FF5-1451-4E38-87EA-C000A51EC5B5}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{D413EC93-83CF-4773-9080-8AB9148DFA4E}" name="R.S🔒" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{72C9A77E-AFBC-404B-A7F6-E681135EDAE9}" name="Redistribute_x000a_Collision_x000a_… T L ∩ R T …" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{7B5E19F2-C874-4B16-82C8-FA89018E0F3A}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="59"/>
+    <tableColumn id="13" xr3:uid="{140BB756-BA0B-42B4-96AC-20E496CA56A3}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{E21AAA4F-92B4-436C-B55B-4DFD07C4BE29}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="57"/>
+    <tableColumn id="14" xr3:uid="{7026FFA9-3F08-448A-86A1-E71772461B72}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="56"/>
+    <tableColumn id="12" xr3:uid="{59C7730E-CD9C-445B-A9A4-AEE7F50B376A}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="55"/>
+    <tableColumn id="11" xr3:uid="{6F38818E-A5E5-47C6-AFD4-C58CF1FD3DD5}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{DFFA66D7-E0E3-4911-BECE-C58139CDD28D}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="53"/>
+    <tableColumn id="7" xr3:uid="{C2DC972A-AC9A-4140-A684-443F75AEE447}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{833A1012-7AE2-431D-82C0-B7CB5960C752}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{43D8BEE4-A2A2-4CFF-9608-9E5B08D746D9}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{0599BB19-BD4F-4332-92DE-B1E045C56EEF}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="49"/>
+    <tableColumn id="10" xr3:uid="{3C3A9FF5-1451-4E38-87EA-C000A51EC5B5}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{D413EC93-83CF-4773-9080-8AB9148DFA4E}" name="R.S🔒" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BB600374-B6B9-40D7-85BD-757E0CB6012B}" name="Table8" displayName="Table8" ref="A10:I14" totalsRowShown="0" headerRowDxfId="43" tableBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BB600374-B6B9-40D7-85BD-757E0CB6012B}" name="Table8" displayName="Table8" ref="A10:I14" totalsRowShown="0" headerRowDxfId="46" tableBorderDxfId="45">
   <autoFilter ref="A10:I14" xr:uid="{CC633682-C369-475E-BC03-B121AB91AB17}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{78CD584E-A9D4-40D7-9D09-CF0EF6806B2D}" name="GetPushData" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{78CD584E-A9D4-40D7-9D09-CF0EF6806B2D}" name="GetPushData" dataDxfId="44"/>
     <tableColumn id="2" xr3:uid="{A08CEA82-1CE9-4441-B0EF-0A975D8FE65A}" name="LT.CanReDist=T_x000a_LT.Limited=T_x000a_LT &lt; WC"/>
     <tableColumn id="6" xr3:uid="{F6036D13-DB0F-4AF8-A1E6-30BCCEB2A5F3}" name="LT.CanReDist=T_x000a_LT.Limited=T_x000a_LT &gt;= WC"/>
     <tableColumn id="4" xr3:uid="{B3ED7712-7A0A-4E68-A538-F34B63335364}" name="LT.CanReDist=T_x000a_LT.Limited=F_x000a_LT &lt; WC"/>
@@ -4898,14 +4934,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2B1B7CE4-90F7-42CA-B974-855205A0C605}" name="Table11" displayName="Table11" ref="A2:E12" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2B1B7CE4-90F7-42CA-B974-855205A0C605}" name="Table11" displayName="Table11" ref="A2:E12" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A2:E12" xr:uid="{78FF5B0B-0912-499F-8F6A-339F3CEEC95F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F251C872-2A1D-42A0-994A-2DFC09D7C047}" name="State" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{F251C872-2A1D-42A0-994A-2DFC09D7C047}" name="State" dataDxfId="41"/>
     <tableColumn id="2" xr3:uid="{AB62CF60-B9F3-442C-A4D1-2FC89B02B851}" name="Border Color"/>
-    <tableColumn id="3" xr3:uid="{E3035B58-4720-4F96-BC43-0FE1566CB1AC}" name="Happens When" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{64A950F1-3FCD-413C-8376-9DAD13362BEC}" name="Details" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{6FB2B197-5E34-46A9-BA2C-CE95765F93BA}" name="Leads to" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{E3035B58-4720-4F96-BC43-0FE1566CB1AC}" name="Happens When" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{64A950F1-3FCD-413C-8376-9DAD13362BEC}" name="Details" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{6FB2B197-5E34-46A9-BA2C-CE95765F93BA}" name="Leads to" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5208,21 +5244,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:H216"/>
+  <dimension ref="A1:H219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+    <sheetView tabSelected="1" topLeftCell="A156" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="37.41796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.68359375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83984375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="78.15625" style="8" customWidth="1"/>
-    <col min="5" max="6" width="9.15625" style="9"/>
-    <col min="7" max="7" width="10.15625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.15625" style="9"/>
+    <col min="1" max="1" width="37.3984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="78.1328125" style="8" customWidth="1"/>
+    <col min="5" max="6" width="9.1328125" style="9"/>
+    <col min="7" max="7" width="10.1328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5247,7 +5283,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8">
+    <row r="3" spans="1:4" ht="28.5">
       <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
@@ -5258,7 +5294,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8">
+    <row r="4" spans="1:4" ht="28.5">
       <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
@@ -5309,7 +5345,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.8">
+    <row r="10" spans="1:4" ht="28.5">
       <c r="A10" s="7" t="s">
         <v>42</v>
       </c>
@@ -5320,7 +5356,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28.8">
+    <row r="11" spans="1:4" ht="28.5">
       <c r="A11" s="7" t="s">
         <v>37</v>
       </c>
@@ -5331,7 +5367,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28.8">
+    <row r="12" spans="1:4" ht="28.5">
       <c r="A12" s="7" t="s">
         <v>40</v>
       </c>
@@ -5342,7 +5378,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" ht="28.8">
+    <row r="13" spans="1:4" s="2" customFormat="1" ht="28.5">
       <c r="A13" s="7" t="s">
         <v>60</v>
       </c>
@@ -5478,7 +5514,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="57.6">
+    <row r="26" spans="1:8" ht="57">
       <c r="A26" s="7" t="s">
         <v>22</v>
       </c>
@@ -5524,7 +5560,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="28.8">
+    <row r="31" spans="1:8" ht="28.5">
       <c r="A31" s="4" t="s">
         <v>9</v>
       </c>
@@ -5621,7 +5657,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="43.2">
+    <row r="42" spans="1:4" ht="42.75">
       <c r="A42" s="7" t="s">
         <v>114</v>
       </c>
@@ -5670,7 +5706,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="43.2">
+    <row r="47" spans="1:4" ht="42.75">
       <c r="A47" s="7" t="s">
         <v>111</v>
       </c>
@@ -5711,7 +5747,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:4" s="10" customFormat="1" ht="57.6">
+    <row r="51" spans="1:4" s="10" customFormat="1" ht="57">
       <c r="A51" s="7" t="s">
         <v>117</v>
       </c>
@@ -5789,7 +5825,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="43.2">
+    <row r="59" spans="1:4" ht="42.75">
       <c r="A59" s="7" t="s">
         <v>190</v>
       </c>
@@ -5833,7 +5869,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="28.8">
+    <row r="63" spans="1:4" ht="28.5">
       <c r="A63" s="7" t="s">
         <v>229</v>
       </c>
@@ -5903,7 +5939,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="43.2">
+    <row r="71" spans="1:4" ht="42.75">
       <c r="A71" s="7" t="s">
         <v>249</v>
       </c>
@@ -5973,7 +6009,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="28.8">
+    <row r="79" spans="1:4" ht="28.5">
       <c r="A79" s="7" t="s">
         <v>313</v>
       </c>
@@ -6091,7 +6127,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="28.8">
+    <row r="90" spans="1:4" ht="28.5">
       <c r="A90" s="7" t="s">
         <v>499</v>
       </c>
@@ -6124,7 +6160,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="57.6">
+    <row r="93" spans="1:4" ht="57">
       <c r="A93" s="7" t="s">
         <v>435</v>
       </c>
@@ -6135,7 +6171,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="28.8">
+    <row r="94" spans="1:4" ht="28.5">
       <c r="A94" s="7" t="s">
         <v>519</v>
       </c>
@@ -6146,7 +6182,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="28.8">
+    <row r="95" spans="1:4" ht="28.5">
       <c r="A95" s="7" t="s">
         <v>518</v>
       </c>
@@ -6168,7 +6204,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="28.8">
+    <row r="97" spans="1:4" ht="28.5">
       <c r="A97" s="7" t="s">
         <v>565</v>
       </c>
@@ -6187,7 +6223,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="28.8">
+    <row r="99" spans="1:4" ht="28.5">
       <c r="A99" s="7" t="s">
         <v>314</v>
       </c>
@@ -6198,7 +6234,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="28.8">
+    <row r="100" spans="1:4" ht="28.5">
       <c r="A100" s="7" t="s">
         <v>117</v>
       </c>
@@ -6209,7 +6245,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="43.2">
+    <row r="101" spans="1:4" ht="42.75">
       <c r="A101" s="7" t="s">
         <v>150</v>
       </c>
@@ -6266,7 +6302,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="28.8">
+    <row r="107" spans="1:4" ht="28.5">
       <c r="A107" s="7" t="s">
         <v>49</v>
       </c>
@@ -6294,7 +6330,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="28.8">
+    <row r="109" spans="1:4" ht="28.5">
       <c r="A109" s="7" t="s">
         <v>358</v>
       </c>
@@ -6361,7 +6397,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="28.8">
+    <row r="114" spans="1:4" ht="28.5">
       <c r="A114" s="7" t="s">
         <v>77</v>
       </c>
@@ -6471,7 +6507,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" ht="28.5">
       <c r="A124" s="7" t="s">
         <v>674</v>
       </c>
@@ -6485,10 +6521,13 @@
         <v>685</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="43.2">
+    <row r="125" spans="1:4" ht="42.75">
       <c r="A125" s="7" t="s">
         <v>686</v>
       </c>
+      <c r="B125" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="C125" s="9" t="s">
         <v>613</v>
       </c>
@@ -6496,10 +6535,13 @@
         <v>694</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="28.8">
+    <row r="126" spans="1:4" ht="28.5">
       <c r="A126" s="7" t="s">
         <v>692</v>
       </c>
+      <c r="B126" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="C126" s="9" t="s">
         <v>613</v>
       </c>
@@ -6507,55 +6549,61 @@
         <v>693</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" ht="28.5">
       <c r="A127" s="7" t="s">
-        <v>681</v>
+        <v>695</v>
       </c>
       <c r="C127" s="9" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" ht="28.8">
+      <c r="D127" s="8" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" s="7" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
       <c r="C128" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D128" s="8" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4">
+    </row>
+    <row r="129" spans="1:4" ht="28.5">
       <c r="A129" s="7" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="C129" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="7" t="s">
-        <v>141</v>
+        <v>690</v>
       </c>
       <c r="C130" s="9" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="131" spans="1:4">
+      <c r="D130" s="8" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="28.5">
       <c r="A131" s="7" t="s">
-        <v>675</v>
+        <v>697</v>
       </c>
       <c r="C131" s="9" t="s">
         <v>613</v>
       </c>
+      <c r="D131" s="8" t="s">
+        <v>698</v>
+      </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="7" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="C132" s="9" t="s">
         <v>613</v>
@@ -6563,7 +6611,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="7" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C133" s="9" t="s">
         <v>613</v>
@@ -6571,463 +6619,452 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="7" t="s">
-        <v>328</v>
+        <v>72</v>
       </c>
       <c r="C134" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D134" s="8" t="s">
-        <v>327</v>
-      </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="7" t="s">
-        <v>83</v>
+        <v>676</v>
       </c>
       <c r="C135" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D135" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="72">
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" s="7" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="C136" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" ht="57.6">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137" s="7" t="s">
-        <v>341</v>
+        <v>83</v>
       </c>
       <c r="C137" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="71.25">
       <c r="A138" s="7" t="s">
-        <v>199</v>
+        <v>339</v>
       </c>
       <c r="C138" s="9" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" ht="57.6">
+      <c r="D138" s="8" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="71.25">
       <c r="A139" s="7" t="s">
-        <v>291</v>
+        <v>341</v>
       </c>
       <c r="C139" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="7" t="s">
-        <v>292</v>
+        <v>199</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D140" s="8" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="57">
       <c r="A141" s="7" t="s">
-        <v>76</v>
+        <v>291</v>
+      </c>
+      <c r="C141" s="9" t="s">
+        <v>613</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>689</v>
+        <v>343</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="7" t="s">
-        <v>129</v>
+        <v>292</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>615</v>
+        <v>0</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>130</v>
+        <v>293</v>
       </c>
     </row>
     <row r="143" spans="1:4">
-      <c r="A143" s="110" t="s">
-        <v>629</v>
-      </c>
-      <c r="C143" s="9" t="s">
-        <v>625</v>
+      <c r="A143" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>631</v>
+        <v>689</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C144" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="D144" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="110" t="s">
+        <v>629</v>
+      </c>
+      <c r="C145" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="D145" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="110"/>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="C144" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4">
-      <c r="A145" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C145" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4">
-      <c r="A146" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C146" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D146" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="28.8">
-      <c r="A147" s="7" t="s">
-        <v>200</v>
       </c>
       <c r="C147" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D147" s="8" t="s">
-        <v>201</v>
-      </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C148" s="9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:4">
-      <c r="A149" s="110" t="s">
-        <v>630</v>
+      <c r="A149" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>625</v>
+        <v>0</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="28.5">
       <c r="A150" s="7" t="s">
-        <v>8</v>
+        <v>200</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="43.2">
+        <v>0</v>
+      </c>
+      <c r="D150" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151" s="7" t="s">
-        <v>259</v>
+        <v>10</v>
       </c>
       <c r="C151" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D151" s="8" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="28.8">
-      <c r="A152" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="B152" s="9" t="s">
-        <v>618</v>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="110" t="s">
+        <v>630</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>615</v>
+        <v>625</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>666</v>
+        <v>632</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="7" t="s">
-        <v>621</v>
-      </c>
-      <c r="D153" s="8" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4">
+        <v>8</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="42.75">
       <c r="A154" s="7" t="s">
-        <v>603</v>
+        <v>259</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4">
+        <v>0</v>
+      </c>
+      <c r="D154" s="8" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="28.5">
       <c r="A155" s="7" t="s">
-        <v>13</v>
+        <v>147</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>618</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>0</v>
+        <v>615</v>
+      </c>
+      <c r="D155" s="8" t="s">
+        <v>666</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="D156" s="8" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="C157" s="9" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C156" s="9" t="s">
+      <c r="C159" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="28.8">
-      <c r="A157" s="7" t="s">
+    <row r="160" spans="1:4" ht="28.5">
+      <c r="A160" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C157" s="9" t="s">
+      <c r="C160" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D157" s="8" t="s">
+      <c r="D160" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="28.8">
-      <c r="A158" s="7" t="s">
+    <row r="161" spans="1:4" ht="28.5">
+      <c r="A161" s="7" t="s">
         <v>444</v>
-      </c>
-      <c r="C158" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D158" s="8" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" ht="43.2">
-      <c r="A159" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="C159" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D159" s="8" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4">
-      <c r="A160" s="7" t="s">
-        <v>602</v>
-      </c>
-      <c r="C160" s="9" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4">
-      <c r="A161" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="C161" s="9" t="s">
         <v>615</v>
       </c>
       <c r="D161" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" ht="28.8">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="42.75">
       <c r="A162" s="7" t="s">
-        <v>146</v>
+        <v>329</v>
       </c>
       <c r="C162" s="9" t="s">
         <v>615</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>148</v>
+        <v>330</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B163" s="9" t="s">
-        <v>618</v>
+        <v>602</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D163" s="8" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="28.5">
       <c r="A164" s="7" t="s">
-        <v>606</v>
+        <v>92</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" ht="28.8">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="28.5">
       <c r="A165" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="B165" s="9" t="s">
-        <v>618</v>
+        <v>146</v>
+      </c>
+      <c r="C165" s="9" t="s">
+        <v>615</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>345</v>
+        <v>148</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="7" t="s">
-        <v>333</v>
+        <v>87</v>
+      </c>
+      <c r="B166" s="9" t="s">
+        <v>618</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>614</v>
+        <v>0</v>
+      </c>
+      <c r="D166" s="8" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="7" t="s">
-        <v>85</v>
+        <v>606</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="28.5">
       <c r="A168" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C168" s="9" t="s">
-        <v>0</v>
+        <v>344</v>
+      </c>
+      <c r="B168" s="9" t="s">
+        <v>618</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>186</v>
+        <v>345</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="7" t="s">
-        <v>609</v>
+        <v>333</v>
       </c>
       <c r="C169" s="9" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C170" s="9" t="s">
+        <v>614</v>
+      </c>
+      <c r="D170" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C171" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D169" s="8" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" ht="28.8">
-      <c r="A170" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C170" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D170" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" ht="43.2">
-      <c r="A171" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C171" s="9" t="s">
-        <v>613</v>
-      </c>
       <c r="D171" s="8" t="s">
-        <v>36</v>
+        <v>186</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" s="7" t="s">
-        <v>136</v>
+        <v>609</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>615</v>
+        <v>0</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" ht="28.5">
       <c r="A173" s="7" t="s">
-        <v>376</v>
+        <v>134</v>
       </c>
       <c r="C173" s="9" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="174" spans="1:4">
+      <c r="D173" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="42.75">
       <c r="A174" s="7" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D174" s="8" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" s="7" t="s">
-        <v>496</v>
+        <v>136</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>613</v>
+        <v>615</v>
+      </c>
+      <c r="D175" s="8" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" s="7" t="s">
-        <v>497</v>
+        <v>376</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="7" t="s">
-        <v>317</v>
+        <v>81</v>
       </c>
       <c r="C177" s="9" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="D177" s="8" t="s">
-        <v>318</v>
+        <v>82</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" s="7" t="s">
-        <v>58</v>
+        <v>496</v>
       </c>
       <c r="C178" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D178" s="8" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" s="7" t="s">
-        <v>346</v>
+        <v>497</v>
       </c>
       <c r="C179" s="9" t="s">
         <v>613</v>
@@ -7035,304 +7072,307 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="7" t="s">
-        <v>205</v>
+        <v>317</v>
       </c>
       <c r="C180" s="9" t="s">
         <v>613</v>
       </c>
+      <c r="D180" s="8" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B181" s="9" t="s">
-        <v>618</v>
+        <v>58</v>
+      </c>
+      <c r="C181" s="9" t="s">
+        <v>613</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" s="7" t="s">
-        <v>123</v>
+        <v>346</v>
       </c>
       <c r="C182" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D182" s="8" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" s="7" t="s">
-        <v>641</v>
+        <v>205</v>
       </c>
       <c r="C183" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D183" s="8" t="s">
-        <v>642</v>
-      </c>
     </row>
     <row r="184" spans="1:4">
       <c r="A184" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C184" s="9" t="s">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="B184" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="D184" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="185" spans="1:4">
       <c r="A185" s="7" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>0</v>
+        <v>613</v>
+      </c>
+      <c r="D185" s="8" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186" s="7" t="s">
-        <v>241</v>
+        <v>641</v>
       </c>
       <c r="C186" s="9" t="s">
-        <v>0</v>
+        <v>613</v>
       </c>
       <c r="D186" s="8" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" ht="43.2">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
       <c r="A187" s="7" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="C187" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D187" s="8" t="s">
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C188" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C189" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D189" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="42.75">
+      <c r="A190" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C190" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D190" s="8" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="28.8">
-      <c r="A188" s="7" t="s">
+    <row r="191" spans="1:4" ht="28.5">
+      <c r="A191" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C188" s="9" t="s">
+      <c r="C191" s="9" t="s">
         <v>615</v>
       </c>
-      <c r="D188" s="8" t="s">
+      <c r="D191" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="28.8">
-      <c r="A189" s="7" t="s">
+    <row r="192" spans="1:4" ht="28.5">
+      <c r="A192" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="C189" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D189" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" ht="28.8">
-      <c r="A190" s="7" t="s">
-        <v>436</v>
-      </c>
-      <c r="C190" s="9" t="s">
-        <v>613</v>
-      </c>
-      <c r="D190" s="8" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" ht="43.2">
-      <c r="A191" s="7" t="s">
-        <v>500</v>
-      </c>
-      <c r="C191" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D191" s="8" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" ht="43.2">
-      <c r="A192" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="C192" s="9" t="s">
         <v>615</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="28.5">
       <c r="A193" s="7" t="s">
-        <v>44</v>
+        <v>436</v>
       </c>
       <c r="C193" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D193" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="42.75">
       <c r="A194" s="7" t="s">
-        <v>210</v>
+        <v>500</v>
       </c>
       <c r="C194" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D194" s="8" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" ht="42.75">
+      <c r="A195" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C195" s="9" t="s">
         <v>615</v>
       </c>
-      <c r="D194" s="8" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" ht="43.2">
-      <c r="A195" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="C195" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="D195" s="8" t="s">
-        <v>218</v>
+        <v>617</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" s="7" t="s">
-        <v>219</v>
+        <v>44</v>
       </c>
       <c r="C196" s="9" t="s">
-        <v>0</v>
+        <v>613</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>220</v>
+        <v>45</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" s="7" t="s">
-        <v>377</v>
+        <v>210</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>0</v>
+        <v>615</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" ht="42.75">
       <c r="A198" s="7" t="s">
-        <v>377</v>
+        <v>217</v>
       </c>
       <c r="C198" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>640</v>
+        <v>218</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" s="7" t="s">
-        <v>379</v>
+        <v>219</v>
       </c>
       <c r="C199" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>380</v>
+        <v>220</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="B200" s="9" t="s">
-        <v>618</v>
+        <v>377</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>615</v>
+        <v>0</v>
+      </c>
+      <c r="D200" s="8" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="201" spans="1:4">
       <c r="A201" s="7" t="s">
-        <v>95</v>
+        <v>377</v>
       </c>
       <c r="C201" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="D201" s="8" t="s">
+        <v>640</v>
+      </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" s="7" t="s">
-        <v>96</v>
+        <v>379</v>
       </c>
       <c r="C202" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="D202" s="8" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" s="7" t="s">
-        <v>47</v>
+        <v>372</v>
+      </c>
+      <c r="B203" s="9" t="s">
+        <v>618</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>0</v>
+        <v>615</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>616</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:4">
       <c r="A205" s="7" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>616</v>
+        <v>0</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>616</v>
+        <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" s="7" t="s">
-        <v>484</v>
+        <v>94</v>
       </c>
       <c r="C207" s="9" t="s">
-        <v>0</v>
+        <v>616</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" s="7" t="s">
-        <v>566</v>
+        <v>56</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D208" s="8" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" s="7" t="s">
-        <v>633</v>
+        <v>57</v>
       </c>
       <c r="C209" s="9" t="s">
-        <v>0</v>
+        <v>616</v>
       </c>
     </row>
     <row r="210" spans="1:4">
       <c r="A210" s="7" t="s">
-        <v>635</v>
+        <v>484</v>
       </c>
       <c r="C210" s="9" t="s">
         <v>0</v>
@@ -7340,58 +7380,85 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" s="7" t="s">
-        <v>634</v>
+        <v>566</v>
       </c>
       <c r="C211" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="D211" s="8" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="212" spans="1:4">
       <c r="A212" s="7" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C212" s="9" t="s">
-        <v>613</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213" spans="1:4">
       <c r="A213" s="7" t="s">
-        <v>657</v>
+        <v>635</v>
       </c>
       <c r="C213" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D213" s="8" t="s">
-        <v>658</v>
-      </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" s="7" t="s">
-        <v>668</v>
+        <v>634</v>
       </c>
       <c r="C214" s="9" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" ht="43.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
       <c r="A215" s="7" t="s">
-        <v>677</v>
+        <v>636</v>
       </c>
       <c r="C215" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D215" s="8" t="s">
-        <v>678</v>
-      </c>
     </row>
     <row r="216" spans="1:4">
       <c r="A216" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="C216" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D216" s="8" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217" s="7" t="s">
+        <v>668</v>
+      </c>
+      <c r="C217" s="9" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" ht="42.75">
+      <c r="A218" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="C218" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="D218" s="8" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
+      <c r="A219" s="7" t="s">
         <v>682</v>
       </c>
-      <c r="C216" s="9" t="s">
+      <c r="C219" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D216" s="8" t="s">
+      <c r="D219" s="8" t="s">
         <v>683</v>
       </c>
     </row>
@@ -7429,9 +7496,9 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="16384" width="9.15625" style="1"/>
+    <col min="1" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -7462,7 +7529,7 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -7536,17 +7603,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F160C7F-FB27-4F84-8171-6D9C64590D99}">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="27.15625" customWidth="1"/>
+    <col min="1" max="1" width="27.1328125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="88.578125" customWidth="1"/>
+    <col min="3" max="3" width="88.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -7560,7 +7627,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8">
+    <row r="2" spans="1:3" ht="28.5">
       <c r="A2" s="58" t="s">
         <v>322</v>
       </c>
@@ -7571,7 +7638,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.2">
+    <row r="3" spans="1:3" ht="42.75">
       <c r="A3" s="58" t="s">
         <v>322</v>
       </c>
@@ -7604,7 +7671,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" ht="28.5">
       <c r="A6" s="58" t="s">
         <v>322</v>
       </c>
@@ -7648,7 +7715,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="43.2">
+    <row r="10" spans="1:3" ht="42.75">
       <c r="A10" s="58" t="s">
         <v>322</v>
       </c>
@@ -7681,7 +7748,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="28.8">
+    <row r="13" spans="1:3" ht="28.5">
       <c r="A13" s="58" t="s">
         <v>322</v>
       </c>
@@ -7692,7 +7759,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="115.2">
+    <row r="14" spans="1:3" ht="114">
       <c r="A14" s="58" t="s">
         <v>322</v>
       </c>
@@ -7725,7 +7792,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="57.6">
+    <row r="17" spans="1:3" ht="57">
       <c r="A17" s="58" t="s">
         <v>322</v>
       </c>
@@ -7747,7 +7814,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="19" customFormat="1" ht="57.6">
+    <row r="19" spans="1:3" s="19" customFormat="1" ht="57">
       <c r="A19" s="58" t="s">
         <v>322</v>
       </c>
@@ -7758,7 +7825,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="19" customFormat="1" ht="28.8">
+    <row r="20" spans="1:3" s="19" customFormat="1" ht="28.5">
       <c r="A20" s="58" t="s">
         <v>322</v>
       </c>
@@ -7813,7 +7880,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="43.2">
+    <row r="25" spans="1:3" ht="42.75">
       <c r="A25" s="58" t="s">
         <v>114</v>
       </c>
@@ -7846,7 +7913,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="57.6">
+    <row r="28" spans="1:3" ht="57">
       <c r="A28" s="61" t="s">
         <v>322</v>
       </c>
@@ -7868,7 +7935,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="28.8">
+    <row r="30" spans="1:3" ht="28.5">
       <c r="A30" s="61" t="s">
         <v>114</v>
       </c>
@@ -7945,7 +8012,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="28.8">
+    <row r="37" spans="1:3" ht="28.5">
       <c r="A37" s="61" t="s">
         <v>322</v>
       </c>
@@ -7989,7 +8056,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="28.8">
+    <row r="41" spans="1:3" ht="28.5">
       <c r="A41" s="61" t="s">
         <v>322</v>
       </c>
@@ -8033,7 +8100,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="28.8">
+    <row r="45" spans="1:3" ht="28.5">
       <c r="A45" s="61" t="s">
         <v>322</v>
       </c>
@@ -8044,7 +8111,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="57.6">
+    <row r="46" spans="1:3" ht="57">
       <c r="A46" s="61" t="s">
         <v>322</v>
       </c>
@@ -8055,7 +8122,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="72">
+    <row r="47" spans="1:3" ht="71.25">
       <c r="A47" s="61" t="s">
         <v>114</v>
       </c>
@@ -8066,7 +8133,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="100.8">
+    <row r="48" spans="1:3" ht="99.75">
       <c r="A48" s="61" t="s">
         <v>114</v>
       </c>
@@ -8077,7 +8144,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="28.8">
+    <row r="49" spans="1:3" ht="28.5">
       <c r="A49" s="61" t="s">
         <v>322</v>
       </c>
@@ -8099,7 +8166,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="57.6">
+    <row r="51" spans="1:3" ht="57">
       <c r="A51" s="61" t="s">
         <v>114</v>
       </c>
@@ -8110,7 +8177,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="28.8">
+    <row r="52" spans="1:3" ht="28.5">
       <c r="A52" s="61" t="s">
         <v>322</v>
       </c>
@@ -8132,7 +8199,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="43.2">
+    <row r="54" spans="1:3" ht="42.75">
       <c r="A54" s="61" t="s">
         <v>114</v>
       </c>
@@ -8143,7 +8210,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="72">
+    <row r="55" spans="1:3" ht="85.5">
       <c r="A55" s="61" t="s">
         <v>111</v>
       </c>
@@ -8154,7 +8221,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="28.8">
+    <row r="56" spans="1:3" ht="28.5">
       <c r="A56" s="61" t="s">
         <v>111</v>
       </c>
@@ -8165,7 +8232,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="19" customFormat="1" ht="43.2">
+    <row r="57" spans="1:3" s="19" customFormat="1" ht="42.75">
       <c r="A57" s="61" t="s">
         <v>111</v>
       </c>
@@ -8176,7 +8243,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="43.2">
+    <row r="58" spans="1:3" ht="42.75">
       <c r="A58" s="61" t="s">
         <v>114</v>
       </c>
@@ -8187,7 +8254,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="19" customFormat="1" ht="28.8">
+    <row r="59" spans="1:3" s="19" customFormat="1" ht="28.5">
       <c r="A59" s="61" t="s">
         <v>322</v>
       </c>
@@ -8209,7 +8276,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="28.8">
+    <row r="61" spans="1:3" ht="28.5">
       <c r="A61" s="58" t="s">
         <v>322</v>
       </c>
@@ -8264,7 +8331,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="43.2">
+    <row r="66" spans="1:3" ht="42.75">
       <c r="A66" s="61" t="s">
         <v>322</v>
       </c>
@@ -8308,7 +8375,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="28.8">
+    <row r="70" spans="1:3" ht="28.5">
       <c r="A70" s="61" t="s">
         <v>114</v>
       </c>
@@ -8319,7 +8386,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="28.8">
+    <row r="71" spans="1:3" ht="28.5">
       <c r="A71" s="61" t="s">
         <v>663</v>
       </c>
@@ -8330,7 +8397,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="43.2">
+    <row r="72" spans="1:3" ht="42.75">
       <c r="A72" s="61" t="s">
         <v>663</v>
       </c>
@@ -8385,7 +8452,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="28.8">
+    <row r="77" spans="1:3" ht="28.5">
       <c r="A77" s="61" t="s">
         <v>322</v>
       </c>
@@ -8407,8 +8474,13 @@
         <v>684</v>
       </c>
     </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="61"/>
+      <c r="B79" s="60"/>
+      <c r="C79" s="60"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B78">
+  <conditionalFormatting sqref="B2:B79">
     <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="Triaged">
       <formula>NOT(ISERROR(SEARCH("Triaged",B2)))</formula>
     </cfRule>
@@ -8440,11 +8512,11 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="28.68359375" customWidth="1"/>
-    <col min="2" max="2" width="98.41796875" style="11" customWidth="1"/>
-    <col min="12" max="12" width="9.68359375" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="98.3984375" style="11" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -8471,7 +8543,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.8">
+    <row r="4" spans="1:12" ht="28.5">
       <c r="A4" t="s">
         <v>212</v>
       </c>
@@ -8479,7 +8551,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.8">
+    <row r="5" spans="1:12" ht="28.5">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -8495,7 +8567,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="19" customFormat="1" ht="28.8">
+    <row r="7" spans="1:12" s="19" customFormat="1" ht="28.5">
       <c r="A7" s="19" t="s">
         <v>224</v>
       </c>
@@ -8527,7 +8599,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="19" customFormat="1" ht="43.2">
+    <row r="11" spans="1:12" s="19" customFormat="1" ht="42.75">
       <c r="A11" t="s">
         <v>249</v>
       </c>
@@ -8535,7 +8607,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="72">
+    <row r="12" spans="1:12" ht="71.25">
       <c r="A12" t="s">
         <v>185</v>
       </c>
@@ -8543,7 +8615,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="19" customFormat="1" ht="43.2">
+    <row r="13" spans="1:12" s="19" customFormat="1" ht="42.75">
       <c r="A13" s="19" t="s">
         <v>315</v>
       </c>
@@ -8551,7 +8623,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="57.6">
+    <row r="14" spans="1:12" ht="57">
       <c r="A14" t="s">
         <v>206</v>
       </c>
@@ -8588,17 +8660,17 @@
       <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.26171875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="22.265625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.59765625" style="21" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="22" style="21" customWidth="1"/>
-    <col min="4" max="4" width="24.83984375" style="21" customWidth="1"/>
-    <col min="5" max="5" width="24.15625" style="21" customWidth="1"/>
-    <col min="6" max="8" width="15.15625" style="21" customWidth="1"/>
-    <col min="11" max="16384" width="22.26171875" style="21"/>
+    <col min="4" max="4" width="24.86328125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="24.1328125" style="21" customWidth="1"/>
+    <col min="6" max="8" width="15.1328125" style="21" customWidth="1"/>
+    <col min="11" max="16384" width="22.265625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29.1" thickBot="1">
+    <row r="1" spans="1:10" ht="28.9" thickBot="1">
       <c r="A1" s="41" t="s">
         <v>248</v>
       </c>
@@ -8624,7 +8696,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="72">
+    <row r="2" spans="1:10" ht="71.25">
       <c r="A2" s="37" t="s">
         <v>398</v>
       </c>
@@ -8652,7 +8724,7 @@
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
     </row>
-    <row r="3" spans="1:10" ht="57.6">
+    <row r="3" spans="1:10" ht="57">
       <c r="A3" s="38" t="s">
         <v>399</v>
       </c>
@@ -8680,7 +8752,7 @@
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
     </row>
-    <row r="4" spans="1:10" ht="72">
+    <row r="4" spans="1:10" ht="71.25">
       <c r="A4" s="38" t="s">
         <v>400</v>
       </c>
@@ -8708,7 +8780,7 @@
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
     </row>
-    <row r="5" spans="1:10" ht="57.6">
+    <row r="5" spans="1:10" ht="57">
       <c r="A5" s="38" t="s">
         <v>401</v>
       </c>
@@ -8736,7 +8808,7 @@
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
     </row>
-    <row r="6" spans="1:10" ht="57.6">
+    <row r="6" spans="1:10" ht="57">
       <c r="A6" s="38" t="s">
         <v>246</v>
       </c>
@@ -8764,7 +8836,7 @@
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
     </row>
-    <row r="7" spans="1:10" ht="57.6">
+    <row r="7" spans="1:10" ht="57">
       <c r="A7" s="38" t="s">
         <v>247</v>
       </c>
@@ -8792,7 +8864,7 @@
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
     </row>
-    <row r="8" spans="1:10" ht="57.6">
+    <row r="8" spans="1:10" ht="57">
       <c r="A8" s="45" t="s">
         <v>244</v>
       </c>
@@ -9075,12 +9147,12 @@
       <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="127.26171875" style="23" customWidth="1"/>
-    <col min="2" max="2" width="9.15625" style="16" customWidth="1"/>
-    <col min="3" max="6" width="9.15625" style="16"/>
-    <col min="7" max="16384" width="9.15625" style="23"/>
+    <col min="1" max="1" width="127.265625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="16" customWidth="1"/>
+    <col min="3" max="6" width="9.1328125" style="16"/>
+    <col min="7" max="16384" width="9.1328125" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="8" customFormat="1">
@@ -9173,27 +9245,27 @@
         <v>296</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8">
+    <row r="16" spans="1:6" ht="28.5">
       <c r="A16" s="8" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="28.8">
+    <row r="17" spans="1:1" ht="28.5">
       <c r="A17" s="23" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="28.8">
+    <row r="18" spans="1:1" ht="28.5">
       <c r="A18" s="23" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="28.8">
+    <row r="19" spans="1:1" ht="28.5">
       <c r="A19" s="23" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="28.8">
+    <row r="20" spans="1:1" ht="28.5">
       <c r="A20" s="23" t="s">
         <v>287</v>
       </c>
@@ -9218,7 +9290,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="28.8">
+    <row r="26" spans="1:1" ht="28.5">
       <c r="A26" s="23" t="s">
         <v>310</v>
       </c>
@@ -9228,12 +9300,12 @@
         <v>311</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="100.8">
+    <row r="28" spans="1:1" ht="99.75">
       <c r="A28" s="50" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="28.8">
+    <row r="29" spans="1:1" ht="28.5">
       <c r="A29" s="8" t="s">
         <v>395</v>
       </c>
@@ -9268,7 +9340,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="144">
+    <row r="37" spans="1:1" ht="142.5">
       <c r="A37" s="50" t="s">
         <v>312</v>
       </c>
@@ -9283,12 +9355,12 @@
         <v>288</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="43.2">
+    <row r="41" spans="1:1" ht="42.75">
       <c r="A41" s="23" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="43.2">
+    <row r="42" spans="1:1" ht="42.75">
       <c r="A42" s="23" t="s">
         <v>295</v>
       </c>
@@ -9298,7 +9370,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="43.2">
+    <row r="44" spans="1:1" ht="42.75">
       <c r="A44" s="23" t="s">
         <v>294</v>
       </c>
@@ -9313,7 +9385,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="5" customFormat="1" ht="28.8">
+    <row r="50" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A50" s="5" t="s">
         <v>276</v>
       </c>
@@ -9323,7 +9395,7 @@
       <c r="E50" s="51"/>
       <c r="F50" s="51"/>
     </row>
-    <row r="51" spans="1:6" s="5" customFormat="1" ht="43.2">
+    <row r="51" spans="1:6" s="5" customFormat="1" ht="42.75">
       <c r="A51" s="5" t="s">
         <v>274</v>
       </c>
@@ -9333,7 +9405,7 @@
       <c r="E51" s="51"/>
       <c r="F51" s="51"/>
     </row>
-    <row r="52" spans="1:6" s="5" customFormat="1" ht="28.8">
+    <row r="52" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A52" s="5" t="s">
         <v>270</v>
       </c>
@@ -9380,7 +9452,7 @@
       <c r="E56" s="51"/>
       <c r="F56" s="51"/>
     </row>
-    <row r="57" spans="1:6" s="5" customFormat="1" ht="28.8">
+    <row r="57" spans="1:6" s="5" customFormat="1" ht="28.5">
       <c r="A57" s="5" t="s">
         <v>277</v>
       </c>
@@ -9400,7 +9472,7 @@
       <c r="E58" s="51"/>
       <c r="F58" s="51"/>
     </row>
-    <row r="59" spans="1:6" s="5" customFormat="1" ht="57.6">
+    <row r="59" spans="1:6" s="5" customFormat="1" ht="57">
       <c r="A59" s="5" t="s">
         <v>278</v>
       </c>
@@ -9425,7 +9497,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="57.6">
+    <row r="65" spans="1:1" ht="57">
       <c r="A65" s="50" t="s">
         <v>422</v>
       </c>
@@ -9440,7 +9512,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="57.6">
+    <row r="69" spans="1:1" ht="57">
       <c r="A69" s="23" t="s">
         <v>457</v>
       </c>
@@ -9455,7 +9527,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="28.8">
+    <row r="72" spans="1:1" ht="28.5">
       <c r="A72" s="8" t="s">
         <v>461</v>
       </c>
@@ -9539,7 +9611,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="28.8">
+    <row r="90" spans="1:1" ht="28.5">
       <c r="A90" s="8" t="s">
         <v>557</v>
       </c>
@@ -9681,17 +9753,17 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.578125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="16.59765625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.83984375" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.41796875" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.578125" style="19"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.86328125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.3984375" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.59765625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8">
+    <row r="1" spans="1:5" ht="28.5">
       <c r="A1" s="104" t="s">
         <v>503</v>
       </c>
@@ -9708,7 +9780,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8">
+    <row r="2" spans="1:5" ht="28.5">
       <c r="A2" s="104" t="s">
         <v>487</v>
       </c>
@@ -9725,7 +9797,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8">
+    <row r="3" spans="1:5" ht="28.5">
       <c r="A3" s="105" t="s">
         <v>493</v>
       </c>
@@ -9742,7 +9814,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8">
+    <row r="4" spans="1:5" ht="28.5">
       <c r="A4" s="105" t="s">
         <v>494</v>
       </c>
@@ -9759,7 +9831,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8">
+    <row r="5" spans="1:5" ht="28.5">
       <c r="A5" s="105" t="s">
         <v>495</v>
       </c>
@@ -9776,7 +9848,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.8">
+    <row r="7" spans="1:5" ht="28.5">
       <c r="A7" s="104" t="s">
         <v>505</v>
       </c>
@@ -9790,7 +9862,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8">
+    <row r="8" spans="1:5" ht="28.5">
       <c r="A8" s="106"/>
       <c r="B8" s="21" t="s">
         <v>488</v>
@@ -9846,16 +9918,16 @@
       <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.578125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="17.59765625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="15.83984375" style="19" customWidth="1"/>
-    <col min="8" max="11" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="15.86328125" style="19" customWidth="1"/>
+    <col min="8" max="11" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="57.6">
+    <row r="1" spans="1:14" ht="57">
       <c r="A1" s="49" t="s">
         <v>589</v>
       </c>
@@ -9899,7 +9971,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="28.8">
+    <row r="2" spans="1:14" ht="28.5">
       <c r="A2" s="101" t="s">
         <v>590</v>
       </c>
@@ -9943,7 +10015,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="19" customFormat="1" ht="28.8">
+    <row r="3" spans="1:14" s="19" customFormat="1" ht="28.5">
       <c r="A3" s="101" t="s">
         <v>591</v>
       </c>
@@ -9987,7 +10059,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="19" customFormat="1" ht="43.2">
+    <row r="4" spans="1:14" s="19" customFormat="1" ht="42.75">
       <c r="A4" s="101" t="s">
         <v>592</v>
       </c>
@@ -10031,7 +10103,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="43.2">
+    <row r="5" spans="1:14" ht="42.75">
       <c r="A5" s="101" t="s">
         <v>593</v>
       </c>
@@ -10075,7 +10147,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="28.8">
+    <row r="6" spans="1:14" ht="28.5">
       <c r="A6" s="101" t="s">
         <v>594</v>
       </c>
@@ -10119,7 +10191,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="28.8">
+    <row r="7" spans="1:14" ht="28.5">
       <c r="A7" s="101" t="s">
         <v>595</v>
       </c>
@@ -10163,7 +10235,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="14.7" thickBot="1">
+    <row r="8" spans="1:14" ht="14.65" thickBot="1">
       <c r="A8" s="102" t="s">
         <v>596</v>
       </c>
@@ -10210,7 +10282,7 @@
     <row r="9" spans="1:14">
       <c r="B9" s="35"/>
     </row>
-    <row r="10" spans="1:14" ht="43.2">
+    <row r="10" spans="1:14" ht="42.75">
       <c r="A10" s="106" t="s">
         <v>544</v>
       </c>
@@ -10239,7 +10311,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="28.8">
+    <row r="11" spans="1:14" ht="28.5">
       <c r="A11" s="104" t="s">
         <v>532</v>
       </c>
@@ -10268,7 +10340,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="28.8">
+    <row r="12" spans="1:14" ht="28.5">
       <c r="A12" s="104" t="s">
         <v>534</v>
       </c>
@@ -10297,7 +10369,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="28.8">
+    <row r="13" spans="1:14" ht="28.5">
       <c r="A13" s="104" t="s">
         <v>533</v>
       </c>
@@ -10326,7 +10398,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="43.2">
+    <row r="14" spans="1:14" ht="42.75">
       <c r="A14" s="104" t="s">
         <v>535</v>
       </c>
@@ -10422,15 +10494,15 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.26171875" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.15625" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.265625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.59765625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.1328125" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63" style="16" customWidth="1"/>
     <col min="5" max="5" width="48" style="16" customWidth="1"/>
-    <col min="6" max="6" width="9.68359375" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.15625" style="16"/>
+    <col min="6" max="6" width="9.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -10679,10 +10751,10 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83984375" customWidth="1"/>
+    <col min="1" max="1" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">

</xml_diff>

<commit_message>
moving plans to git
</commit_message>
<xml_diff>
--- a/Plans.xlsx
+++ b/Plans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neubu\Source\Repos\TimekeeperWPF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AF08AE-0F98-40F5-975D-9C58B4EBA04B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C9A36D-9446-41A3-9CC7-4D806B4BCE57}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24930" windowHeight="12330" tabRatio="775" xr2:uid="{B08B66F6-8B10-48BD-8CBC-92B4F4D60D54}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="699">
   <si>
     <t>Feature</t>
   </si>
@@ -2207,9 +2207,6 @@
     <t>YearViewModel</t>
   </si>
   <si>
-    <t>Refactor Panels</t>
-  </si>
-  <si>
     <t>Refactoring</t>
   </si>
   <si>
@@ -2274,6 +2271,9 @@
   </si>
   <si>
     <t>Serialize options for persistence between sessions. Save what view we were last using, save state of all options.</t>
+  </si>
+  <si>
+    <t>Git</t>
   </si>
 </sst>
 </file>
@@ -3079,7 +3079,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="109">
+  <dxfs count="107">
     <dxf>
       <fill>
         <patternFill>
@@ -3343,26 +3343,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4497,15 +4480,15 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="4" xr9:uid="{5F0E2908-E7EC-43FB-9BBB-CB014E9A6F67}">
-      <tableStyleElement type="wholeTable" dxfId="108"/>
-      <tableStyleElement type="headerRow" dxfId="107"/>
-      <tableStyleElement type="firstColumn" dxfId="106"/>
+      <tableStyleElement type="wholeTable" dxfId="106"/>
+      <tableStyleElement type="headerRow" dxfId="105"/>
+      <tableStyleElement type="firstColumn" dxfId="104"/>
       <tableStyleElement type="firstRowStripe" size="2"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="3" xr9:uid="{A53ADC7C-9332-4916-9ACB-0EFC07D28AC6}">
-      <tableStyleElement type="wholeTable" dxfId="105"/>
-      <tableStyleElement type="headerRow" dxfId="104"/>
-      <tableStyleElement type="secondRowStripe" dxfId="103"/>
+      <tableStyleElement type="wholeTable" dxfId="103"/>
+      <tableStyleElement type="headerRow" dxfId="102"/>
+      <tableStyleElement type="secondRowStripe" dxfId="101"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -4814,112 +4797,112 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D220" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
-  <autoFilter ref="A1:D220" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65952822-3284-40E9-9481-C13F5965A79B}" name="Table1" displayName="Table1" ref="A1:D218" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
+  <autoFilter ref="A1:D218" xr:uid="{BF00F6B2-463B-4ADE-983E-2EF4E635F59B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="100"/>
-    <tableColumn id="6" xr3:uid="{1FFE88A6-F499-42FB-A3F4-F5BDCD9D0CF0}" name="Done" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{75DC89E8-11B6-4EA2-BBEB-7D8F4C2B75D4}" name="Type" dataDxfId="98"/>
-    <tableColumn id="5" xr3:uid="{65384592-5F41-4A06-A57C-FE71C87B4BDD}" name="Notes" dataDxfId="97"/>
+    <tableColumn id="1" xr3:uid="{D3AD27DB-285B-4F25-830A-2F06B20F1459}" name="Feature" dataDxfId="98"/>
+    <tableColumn id="6" xr3:uid="{1FFE88A6-F499-42FB-A3F4-F5BDCD9D0CF0}" name="Done" dataDxfId="97"/>
+    <tableColumn id="2" xr3:uid="{75DC89E8-11B6-4EA2-BBEB-7D8F4C2B75D4}" name="Type" dataDxfId="96"/>
+    <tableColumn id="5" xr3:uid="{65384592-5F41-4A06-A57C-FE71C87B4BDD}" name="Notes" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F572A93C-B296-47BB-A2B7-E8D930E92020}" name="Table4" displayName="Table4" ref="A1:C79" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95" tableBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F572A93C-B296-47BB-A2B7-E8D930E92020}" name="Table4" displayName="Table4" ref="A1:C79" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93" tableBorderDxfId="92">
   <autoFilter ref="A1:C79" xr:uid="{5B5CE518-BB75-408C-8F1B-EE90C29E48F3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2EF2C0F2-7D81-49C3-B8A7-E25CCB336A17}" name="Column1" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{FCC47FF7-6739-4E5E-9E09-E5EAD7161467}" name="Column2" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{3079BD65-A18D-4106-9386-B084236E0CE0}" name="Column3" dataDxfId="91"/>
+    <tableColumn id="1" xr3:uid="{2EF2C0F2-7D81-49C3-B8A7-E25CCB336A17}" name="Column1" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{FCC47FF7-6739-4E5E-9E09-E5EAD7161467}" name="Column2" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{3079BD65-A18D-4106-9386-B084236E0CE0}" name="Column3" dataDxfId="89"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E4DD08F2-9CC2-46CC-93EE-E01A4DBC8EEE}" name="Table5" displayName="Table5" ref="A1:H8" totalsRowShown="0" headerRowDxfId="90" dataDxfId="88" headerRowBorderDxfId="89" tableBorderDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E4DD08F2-9CC2-46CC-93EE-E01A4DBC8EEE}" name="Table5" displayName="Table5" ref="A1:H8" totalsRowShown="0" headerRowDxfId="88" dataDxfId="86" headerRowBorderDxfId="87" tableBorderDxfId="85">
   <autoFilter ref="A1:H8" xr:uid="{9EF71295-67E3-4AA7-981B-99814F9C00D6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5F56F396-ECBF-4022-A747-BB6579150BC5}" name="Previous" dataDxfId="86"/>
-    <tableColumn id="2" xr3:uid="{52DF5424-7715-4094-9055-254252166B84}" name="CI Start_x000a_in Z" dataDxfId="85"/>
-    <tableColumn id="3" xr3:uid="{4BF25F2B-3788-4EC0-877F-738CFB7416BD}" name="CI End_x000a_in Z" dataDxfId="84"/>
-    <tableColumn id="4" xr3:uid="{3D1264CD-7DED-47FE-9A26-02FAA9BC34AE}" name="CI Start_x000a_out Z" dataDxfId="83"/>
-    <tableColumn id="5" xr3:uid="{91478E3E-F2EC-42B9-9CAC-61EA2AD657CB}" name="CI End_x000a_out Z" dataDxfId="82"/>
-    <tableColumn id="6" xr3:uid="{BD45968E-F796-4835-9D67-3627C99D24EC}" name="Z Start" dataDxfId="81"/>
-    <tableColumn id="7" xr3:uid="{3B4EE896-0831-43E7-8AE0-49A3476BEA97}" name="Z End" dataDxfId="80"/>
-    <tableColumn id="8" xr3:uid="{D4DAA8AA-8B7A-4978-8C26-61D2C9036856}" name="P End" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{5F56F396-ECBF-4022-A747-BB6579150BC5}" name="Previous" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{52DF5424-7715-4094-9055-254252166B84}" name="CI Start_x000a_in Z" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{4BF25F2B-3788-4EC0-877F-738CFB7416BD}" name="CI End_x000a_in Z" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{3D1264CD-7DED-47FE-9A26-02FAA9BC34AE}" name="CI Start_x000a_out Z" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{91478E3E-F2EC-42B9-9CAC-61EA2AD657CB}" name="CI End_x000a_out Z" dataDxfId="80"/>
+    <tableColumn id="6" xr3:uid="{BD45968E-F796-4835-9D67-3627C99D24EC}" name="Z Start" dataDxfId="79"/>
+    <tableColumn id="7" xr3:uid="{3B4EE896-0831-43E7-8AE0-49A3476BEA97}" name="Z End" dataDxfId="78"/>
+    <tableColumn id="8" xr3:uid="{D4DAA8AA-8B7A-4978-8C26-61D2C9036856}" name="P End" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC6FE9AE-35E3-4705-A142-315DB9D43B3A}" name="Table3" displayName="Table3" ref="A1:A117" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC6FE9AE-35E3-4705-A142-315DB9D43B3A}" name="Table3" displayName="Table3" ref="A1:A117" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
   <autoFilter ref="A1:A117" xr:uid="{A2F7B623-DE53-4896-BDD6-CCC38D4467C3}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{0C8999A5-1CD8-483C-A3BB-7AD00E0E2478}" name="Collision Theory" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{0C8999A5-1CD8-483C-A3BB-7AD00E0E2478}" name="Collision Theory" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67135CB1-5074-4EBE-BD9A-48C30A4CB81B}" name="Table2" displayName="Table2" ref="A1:E5" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74" tableBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67135CB1-5074-4EBE-BD9A-48C30A4CB81B}" name="Table2" displayName="Table2" ref="A1:E5" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72" tableBorderDxfId="71">
   <autoFilter ref="A1:E5" xr:uid="{B388395A-7532-4521-958E-47A4C8955AF2}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{70C2C4E6-CAF6-425B-8E04-929D489EC9D7}" name="Determine L, R_x000a_Step1" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{2FE5E346-C794-4C60-92C1-0865C7DF44B2}" name="C2.LT_x000a_C2.RT" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{D05D7189-86A2-4E66-978C-200C858C620C}" name="C2.LT null_x000a_C2.RT" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{9D36A042-6482-4DEE-A827-BCFC97E3E6B9}" name="C2.LT_x000a_C2.RT null" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{DCA50F46-3DCF-4728-AFF9-64F17E91077A}" name="C2.LT null_x000a_C2.RT null" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{70C2C4E6-CAF6-425B-8E04-929D489EC9D7}" name="Determine L, R_x000a_Step1" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{2FE5E346-C794-4C60-92C1-0865C7DF44B2}" name="C2.LT_x000a_C2.RT" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{D05D7189-86A2-4E66-978C-200C858C620C}" name="C2.LT null_x000a_C2.RT" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{9D36A042-6482-4DEE-A827-BCFC97E3E6B9}" name="C2.LT_x000a_C2.RT null" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{DCA50F46-3DCF-4728-AFF9-64F17E91077A}" name="C2.LT null_x000a_C2.RT null" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1D0690DC-ACA6-40D8-866A-1D8C44DE4AC8}" name="Table7" displayName="Table7" ref="A7:D8" totalsRowShown="0" tableBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1D0690DC-ACA6-40D8-866A-1D8C44DE4AC8}" name="Table7" displayName="Table7" ref="A7:D8" totalsRowShown="0" tableBorderDxfId="65">
   <autoFilter ref="A7:D8" xr:uid="{ACCFA163-AAF6-4628-ADE5-97056064C206}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9757D096-D900-42A9-8E11-C4ACA310AE56}" name="Determine L, R_x000a_Step2" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{C3069A29-6915-46B5-977A-E175A6DEB3D2}" name="C1.S &lt; C2.S" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{12A8AD37-B3F9-4A8B-9EA6-A0F6EB34B35A}" name="C1.S == C2.S" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{7A2BF950-BBF5-494B-8BCE-AD358D4349E2}" name="C1.S &gt; C2.S" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{9757D096-D900-42A9-8E11-C4ACA310AE56}" name="Determine L, R_x000a_Step2" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{C3069A29-6915-46B5-977A-E175A6DEB3D2}" name="C1.S &lt; C2.S" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{12A8AD37-B3F9-4A8B-9EA6-A0F6EB34B35A}" name="C1.S == C2.S" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{7A2BF950-BBF5-494B-8BCE-AD358D4349E2}" name="C1.S &gt; C2.S" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BEABA309-E652-49AF-B0CA-0DBB8732C3D3}" name="Table6" displayName="Table6" ref="A1:N8" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BEABA309-E652-49AF-B0CA-0DBB8732C3D3}" name="Table6" displayName="Table6" ref="A1:N8" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="A1:N8" xr:uid="{3AB9159B-B403-4CC8-8649-2A74831EFA39}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{72C9A77E-AFBC-404B-A7F6-E681135EDAE9}" name="Redistribute_x000a_Collision_x000a_… T L ∩ R T …" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{7B5E19F2-C874-4B16-82C8-FA89018E0F3A}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="59"/>
-    <tableColumn id="13" xr3:uid="{140BB756-BA0B-42B4-96AC-20E496CA56A3}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{E21AAA4F-92B4-436C-B55B-4DFD07C4BE29}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="57"/>
-    <tableColumn id="14" xr3:uid="{7026FFA9-3F08-448A-86A1-E71772461B72}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="56"/>
-    <tableColumn id="12" xr3:uid="{59C7730E-CD9C-445B-A9A4-AEE7F50B376A}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="55"/>
-    <tableColumn id="11" xr3:uid="{6F38818E-A5E5-47C6-AFD4-C58CF1FD3DD5}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="54"/>
-    <tableColumn id="8" xr3:uid="{DFFA66D7-E0E3-4911-BECE-C58139CDD28D}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="53"/>
-    <tableColumn id="7" xr3:uid="{C2DC972A-AC9A-4140-A684-443F75AEE447}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{833A1012-7AE2-431D-82C0-B7CB5960C752}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="51"/>
-    <tableColumn id="9" xr3:uid="{43D8BEE4-A2A2-4CFF-9608-9E5B08D746D9}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{0599BB19-BD4F-4332-92DE-B1E045C56EEF}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="49"/>
-    <tableColumn id="10" xr3:uid="{3C3A9FF5-1451-4E38-87EA-C000A51EC5B5}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{D413EC93-83CF-4773-9080-8AB9148DFA4E}" name="R.S🔒" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{72C9A77E-AFBC-404B-A7F6-E681135EDAE9}" name="Redistribute_x000a_Collision_x000a_… T L ∩ R T …" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{7B5E19F2-C874-4B16-82C8-FA89018E0F3A}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="57"/>
+    <tableColumn id="13" xr3:uid="{140BB756-BA0B-42B4-96AC-20E496CA56A3}" name="RHasRoom=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{E21AAA4F-92B4-436C-B55B-4DFD07C4BE29}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="55"/>
+    <tableColumn id="14" xr3:uid="{7026FFA9-3F08-448A-86A1-E71772461B72}" name="RHasRoom=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="54"/>
+    <tableColumn id="12" xr3:uid="{59C7730E-CD9C-445B-A9A4-AEE7F50B376A}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="53"/>
+    <tableColumn id="11" xr3:uid="{6F38818E-A5E5-47C6-AFD4-C58CF1FD3DD5}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{DFFA66D7-E0E3-4911-BECE-C58139CDD28D}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{C2DC972A-AC9A-4140-A684-443F75AEE447}" name="RHasRoom=F_x000a_RCanReDist=T_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{833A1012-7AE2-431D-82C0-B7CB5960C752}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R != WCR" dataDxfId="49"/>
+    <tableColumn id="9" xr3:uid="{43D8BEE4-A2A2-4CFF-9608-9E5B08D746D9}" name="RHasRoom=F_x000a_WCL &gt;= WCR_x000a_R == WCR" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{0599BB19-BD4F-4332-92DE-B1E045C56EEF}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R != WCR" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{3C3A9FF5-1451-4E38-87EA-C000A51EC5B5}" name="RHasRoom=F_x000a_WCL &lt; WCR_x000a_R == WCR" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{D413EC93-83CF-4773-9080-8AB9148DFA4E}" name="R.S🔒" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BB600374-B6B9-40D7-85BD-757E0CB6012B}" name="Table8" displayName="Table8" ref="A10:I14" totalsRowShown="0" headerRowDxfId="46" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BB600374-B6B9-40D7-85BD-757E0CB6012B}" name="Table8" displayName="Table8" ref="A10:I14" totalsRowShown="0" headerRowDxfId="44" tableBorderDxfId="43">
   <autoFilter ref="A10:I14" xr:uid="{CC633682-C369-475E-BC03-B121AB91AB17}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{78CD584E-A9D4-40D7-9D09-CF0EF6806B2D}" name="GetPushData" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{78CD584E-A9D4-40D7-9D09-CF0EF6806B2D}" name="GetPushData" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{A08CEA82-1CE9-4441-B0EF-0A975D8FE65A}" name="LT.CanReDist=T_x000a_LT.Limited=T_x000a_LT &lt; WC"/>
     <tableColumn id="6" xr3:uid="{F6036D13-DB0F-4AF8-A1E6-30BCCEB2A5F3}" name="LT.CanReDist=T_x000a_LT.Limited=T_x000a_LT &gt;= WC"/>
     <tableColumn id="4" xr3:uid="{B3ED7712-7A0A-4E68-A538-F34B63335364}" name="LT.CanReDist=T_x000a_LT.Limited=F_x000a_LT &lt; WC"/>
@@ -4934,14 +4917,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2B1B7CE4-90F7-42CA-B974-855205A0C605}" name="Table11" displayName="Table11" ref="A2:E12" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2B1B7CE4-90F7-42CA-B974-855205A0C605}" name="Table11" displayName="Table11" ref="A2:E12" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A2:E12" xr:uid="{78FF5B0B-0912-499F-8F6A-339F3CEEC95F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F251C872-2A1D-42A0-994A-2DFC09D7C047}" name="State" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{F251C872-2A1D-42A0-994A-2DFC09D7C047}" name="State" dataDxfId="39"/>
     <tableColumn id="2" xr3:uid="{AB62CF60-B9F3-442C-A4D1-2FC89B02B851}" name="Border Color"/>
-    <tableColumn id="3" xr3:uid="{E3035B58-4720-4F96-BC43-0FE1566CB1AC}" name="Happens When" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{64A950F1-3FCD-413C-8376-9DAD13362BEC}" name="Details" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{6FB2B197-5E34-46A9-BA2C-CE95765F93BA}" name="Leads to" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{E3035B58-4720-4F96-BC43-0FE1566CB1AC}" name="Happens When" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{64A950F1-3FCD-413C-8376-9DAD13362BEC}" name="Details" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{6FB2B197-5E34-46A9-BA2C-CE95765F93BA}" name="Leads to" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5244,10 +5227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F1E44D-0EC6-4B80-951F-3617AE94E3C2}">
-  <dimension ref="A1:H219"/>
+  <dimension ref="A1:H217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D132" sqref="D132"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -6454,7 +6437,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="7" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B119" s="9" t="s">
         <v>23</v>
@@ -6518,12 +6501,12 @@
         <v>616</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="42.75">
       <c r="A125" s="7" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B125" s="9" t="s">
         <v>23</v>
@@ -6532,12 +6515,12 @@
         <v>613</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="28.5">
       <c r="A126" s="7" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B126" s="9" t="s">
         <v>23</v>
@@ -6546,23 +6529,29 @@
         <v>613</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="28.5">
       <c r="A127" s="7" t="s">
-        <v>695</v>
+        <v>694</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="C127" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="7" t="s">
-        <v>681</v>
+        <v>680</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="C128" s="9" t="s">
         <v>613</v>
@@ -6570,41 +6559,53 @@
     </row>
     <row r="129" spans="1:4" ht="28.5">
       <c r="A129" s="7" t="s">
-        <v>687</v>
+        <v>686</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="C129" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="7" t="s">
-        <v>690</v>
+        <v>689</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="C130" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="28.5">
       <c r="A131" s="7" t="s">
-        <v>697</v>
+        <v>696</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="C131" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="7" t="s">
         <v>141</v>
       </c>
+      <c r="B132" s="9" t="s">
+        <v>698</v>
+      </c>
       <c r="C132" s="9" t="s">
         <v>613</v>
       </c>
@@ -6613,6 +6614,9 @@
       <c r="A133" s="7" t="s">
         <v>675</v>
       </c>
+      <c r="B133" s="9" t="s">
+        <v>698</v>
+      </c>
       <c r="C133" s="9" t="s">
         <v>613</v>
       </c>
@@ -6621,710 +6625,745 @@
       <c r="A134" s="7" t="s">
         <v>72</v>
       </c>
+      <c r="B134" s="9" t="s">
+        <v>698</v>
+      </c>
       <c r="C134" s="9" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="7" t="s">
-        <v>676</v>
+        <v>328</v>
+      </c>
+      <c r="B135" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="C135" s="9" t="s">
         <v>613</v>
       </c>
+      <c r="D135" s="8" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="7" t="s">
-        <v>328</v>
+        <v>83</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="C136" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="71.25">
       <c r="A137" s="7" t="s">
-        <v>83</v>
+        <v>339</v>
+      </c>
+      <c r="B137" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="C137" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>84</v>
+        <v>340</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="71.25">
       <c r="A138" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="C138" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" ht="71.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139" s="7" t="s">
-        <v>341</v>
+        <v>199</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="C139" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D139" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4">
+    </row>
+    <row r="140" spans="1:4" ht="57">
       <c r="A140" s="7" t="s">
-        <v>199</v>
+        <v>291</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="C140" s="9" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" ht="57">
+      <c r="D140" s="8" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
+      </c>
+      <c r="B141" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>613</v>
+        <v>0</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>343</v>
+        <v>293</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="C142" s="9" t="s">
-        <v>0</v>
+        <v>76</v>
+      </c>
+      <c r="B142" s="9" t="s">
+        <v>698</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>293</v>
+        <v>688</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="7" t="s">
-        <v>76</v>
+        <v>129</v>
+      </c>
+      <c r="B143" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="C143" s="9" t="s">
+        <v>615</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>689</v>
+        <v>130</v>
       </c>
     </row>
     <row r="144" spans="1:4">
-      <c r="A144" s="7" t="s">
-        <v>129</v>
+      <c r="A144" s="110" t="s">
+        <v>629</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>615</v>
+        <v>625</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>130</v>
+        <v>631</v>
       </c>
     </row>
     <row r="145" spans="1:4">
-      <c r="A145" s="110" t="s">
-        <v>629</v>
+      <c r="A145" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>625</v>
-      </c>
-      <c r="D145" s="8" t="s">
-        <v>631</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:4">
-      <c r="A146" s="110"/>
+      <c r="A146" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C146" s="9" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C147" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:4">
+      <c r="D147" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="28.5">
       <c r="A148" s="7" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="C148" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="D148" s="8" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C149" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D149" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="28.5">
-      <c r="A150" s="7" t="s">
-        <v>200</v>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="110" t="s">
+        <v>630</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>0</v>
+        <v>625</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>201</v>
+        <v>632</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C151" s="9" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="42.75">
+      <c r="A152" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C152" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:4">
-      <c r="A152" s="110" t="s">
-        <v>630</v>
-      </c>
-      <c r="C152" s="9" t="s">
-        <v>625</v>
-      </c>
       <c r="D152" s="8" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="28.5">
       <c r="A153" s="7" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>618</v>
       </c>
       <c r="C153" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="D153" s="8" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="D154" s="8" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="C155" s="9" t="s">
         <v>613</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="42.75">
-      <c r="A154" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="C154" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D154" s="8" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="28.5">
-      <c r="A155" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="B155" s="9" t="s">
-        <v>618</v>
-      </c>
-      <c r="C155" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D155" s="8" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="7" t="s">
-        <v>621</v>
-      </c>
-      <c r="D156" s="8" t="s">
-        <v>622</v>
+        <v>13</v>
+      </c>
+      <c r="C156" s="9" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="7" t="s">
-        <v>603</v>
+        <v>35</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="28.5">
       <c r="A158" s="7" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C158" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:4">
+      <c r="D158" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="28.5">
       <c r="A159" s="7" t="s">
-        <v>35</v>
+        <v>444</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" ht="28.5">
+        <v>615</v>
+      </c>
+      <c r="D159" s="8" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="42.75">
       <c r="A160" s="7" t="s">
-        <v>33</v>
+        <v>329</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>0</v>
+        <v>615</v>
       </c>
       <c r="D160" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" ht="28.5">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
       <c r="A161" s="7" t="s">
-        <v>444</v>
+        <v>602</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D161" s="8" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" ht="42.75">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="28.5">
       <c r="A162" s="7" t="s">
-        <v>329</v>
+        <v>92</v>
       </c>
       <c r="C162" s="9" t="s">
         <v>615</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="28.5">
       <c r="A163" s="7" t="s">
-        <v>602</v>
+        <v>146</v>
       </c>
       <c r="C163" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="D163" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B164" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="C164" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D164" s="8" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="C165" s="9" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" ht="28.5">
-      <c r="A164" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C164" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D164" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" ht="28.5">
-      <c r="A165" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C165" s="9" t="s">
-        <v>615</v>
-      </c>
       <c r="D165" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="28.5">
       <c r="A166" s="7" t="s">
-        <v>87</v>
+        <v>344</v>
       </c>
       <c r="B166" s="9" t="s">
         <v>618</v>
       </c>
-      <c r="C166" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="D166" s="8" t="s">
-        <v>639</v>
+        <v>345</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="7" t="s">
-        <v>606</v>
+        <v>333</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>613</v>
-      </c>
-      <c r="D167" s="8" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" ht="28.5">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
       <c r="A168" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="B168" s="9" t="s">
-        <v>618</v>
+        <v>85</v>
+      </c>
+      <c r="C168" s="9" t="s">
+        <v>614</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>345</v>
+        <v>86</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="7" t="s">
-        <v>333</v>
+        <v>5</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>614</v>
+        <v>0</v>
+      </c>
+      <c r="D169" s="8" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="7" t="s">
-        <v>85</v>
+        <v>609</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>614</v>
+        <v>0</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="28.5">
       <c r="A171" s="7" t="s">
-        <v>5</v>
+        <v>134</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>0</v>
+        <v>615</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="42.75">
       <c r="A172" s="7" t="s">
-        <v>609</v>
+        <v>142</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>0</v>
+        <v>613</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" ht="28.5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
       <c r="A173" s="7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C173" s="9" t="s">
         <v>615</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" ht="42.75">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
       <c r="A174" s="7" t="s">
-        <v>142</v>
+        <v>376</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>613</v>
-      </c>
-      <c r="D174" s="8" t="s">
-        <v>36</v>
+        <v>615</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" s="7" t="s">
-        <v>136</v>
+        <v>81</v>
       </c>
       <c r="C175" s="9" t="s">
         <v>615</v>
       </c>
       <c r="D175" s="8" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" s="7" t="s">
-        <v>376</v>
+        <v>496</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="7" t="s">
-        <v>81</v>
+        <v>497</v>
       </c>
       <c r="C177" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D177" s="8" t="s">
-        <v>82</v>
+        <v>613</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" s="7" t="s">
-        <v>496</v>
+        <v>317</v>
       </c>
       <c r="C178" s="9" t="s">
         <v>613</v>
       </c>
+      <c r="D178" s="8" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" s="7" t="s">
-        <v>497</v>
+        <v>58</v>
       </c>
       <c r="C179" s="9" t="s">
         <v>613</v>
       </c>
+      <c r="D179" s="8" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="7" t="s">
-        <v>317</v>
+        <v>346</v>
       </c>
       <c r="C180" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D180" s="8" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" s="7" t="s">
-        <v>58</v>
+        <v>205</v>
       </c>
       <c r="C181" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D181" s="8" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="C182" s="9" t="s">
-        <v>613</v>
+        <v>90</v>
+      </c>
+      <c r="B182" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="D182" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" s="7" t="s">
-        <v>205</v>
+        <v>123</v>
       </c>
       <c r="C183" s="9" t="s">
         <v>613</v>
       </c>
+      <c r="D183" s="8" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="184" spans="1:4">
       <c r="A184" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B184" s="9" t="s">
-        <v>618</v>
+        <v>641</v>
+      </c>
+      <c r="C184" s="9" t="s">
+        <v>613</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>91</v>
+        <v>642</v>
       </c>
     </row>
     <row r="185" spans="1:4">
       <c r="A185" s="7" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>613</v>
-      </c>
-      <c r="D185" s="8" t="s">
-        <v>124</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186" s="7" t="s">
-        <v>641</v>
+        <v>66</v>
       </c>
       <c r="C186" s="9" t="s">
-        <v>613</v>
-      </c>
-      <c r="D186" s="8" t="s">
-        <v>642</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187" spans="1:4">
       <c r="A187" s="7" t="s">
-        <v>74</v>
+        <v>241</v>
       </c>
       <c r="C187" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:4">
+      <c r="D187" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="42.75">
       <c r="A188" s="7" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="C188" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="1:4">
+      <c r="D188" s="8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" ht="28.5">
       <c r="A189" s="7" t="s">
-        <v>241</v>
+        <v>137</v>
       </c>
       <c r="C189" s="9" t="s">
-        <v>0</v>
+        <v>615</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" ht="42.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="28.5">
       <c r="A190" s="7" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="C190" s="9" t="s">
-        <v>0</v>
+        <v>615</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>348</v>
+        <v>144</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="28.5">
       <c r="A191" s="7" t="s">
-        <v>137</v>
+        <v>436</v>
       </c>
       <c r="C191" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="D191" s="8" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="42.75">
+      <c r="A192" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="C192" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D192" s="8" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="42.75">
+      <c r="A193" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C193" s="9" t="s">
         <v>615</v>
       </c>
-      <c r="D191" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" ht="28.5">
-      <c r="A192" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C192" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="D192" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" ht="28.5">
-      <c r="A193" s="7" t="s">
-        <v>436</v>
-      </c>
-      <c r="C193" s="9" t="s">
+      <c r="D193" s="8" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C194" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D193" s="8" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" ht="42.75">
-      <c r="A194" s="7" t="s">
-        <v>500</v>
-      </c>
-      <c r="C194" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="D194" s="8" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" ht="42.75">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
       <c r="A195" s="7" t="s">
-        <v>145</v>
+        <v>210</v>
       </c>
       <c r="C195" s="9" t="s">
         <v>615</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" ht="42.75">
       <c r="A196" s="7" t="s">
-        <v>44</v>
+        <v>217</v>
       </c>
       <c r="C196" s="9" t="s">
-        <v>613</v>
+        <v>0</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>45</v>
+        <v>218</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" s="7" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>615</v>
+        <v>0</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" ht="42.75">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
       <c r="A198" s="7" t="s">
-        <v>217</v>
+        <v>377</v>
       </c>
       <c r="C198" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>218</v>
+        <v>378</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" s="7" t="s">
-        <v>219</v>
+        <v>377</v>
       </c>
       <c r="C199" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>220</v>
+        <v>640</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200" s="7" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C200" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="201" spans="1:4">
       <c r="A201" s="7" t="s">
-        <v>377</v>
+        <v>372</v>
+      </c>
+      <c r="B201" s="9" t="s">
+        <v>618</v>
       </c>
       <c r="C201" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D201" s="8" t="s">
-        <v>640</v>
+        <v>615</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" s="7" t="s">
-        <v>379</v>
+        <v>95</v>
       </c>
       <c r="C202" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D202" s="8" t="s">
-        <v>380</v>
-      </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="B203" s="9" t="s">
-        <v>618</v>
+        <v>96</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>615</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" s="7" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="C204" s="9" t="s">
         <v>0</v>
@@ -7332,23 +7371,23 @@
     </row>
     <row r="205" spans="1:4">
       <c r="A205" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>0</v>
+        <v>616</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" s="7" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>0</v>
+        <v>616</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" s="7" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="C207" s="9" t="s">
         <v>616</v>
@@ -7356,23 +7395,26 @@
     </row>
     <row r="208" spans="1:4">
       <c r="A208" s="7" t="s">
-        <v>56</v>
+        <v>484</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>616</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" s="7" t="s">
-        <v>57</v>
+        <v>566</v>
       </c>
       <c r="C209" s="9" t="s">
-        <v>616</v>
+        <v>0</v>
+      </c>
+      <c r="D209" s="8" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="210" spans="1:4">
       <c r="A210" s="7" t="s">
-        <v>484</v>
+        <v>633</v>
       </c>
       <c r="C210" s="9" t="s">
         <v>0</v>
@@ -7380,18 +7422,15 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" s="7" t="s">
-        <v>566</v>
+        <v>635</v>
       </c>
       <c r="C211" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D211" s="8" t="s">
-        <v>611</v>
-      </c>
     </row>
     <row r="212" spans="1:4">
       <c r="A212" s="7" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C212" s="9" t="s">
         <v>0</v>
@@ -7399,78 +7438,65 @@
     </row>
     <row r="213" spans="1:4">
       <c r="A213" s="7" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C213" s="9" t="s">
-        <v>0</v>
+        <v>613</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" s="7" t="s">
-        <v>634</v>
+        <v>657</v>
       </c>
       <c r="C214" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="D214" s="8" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="215" spans="1:4">
       <c r="A215" s="7" t="s">
-        <v>636</v>
+        <v>668</v>
       </c>
       <c r="C215" s="9" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" ht="42.75">
+      <c r="A216" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="C216" s="9" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="216" spans="1:4">
-      <c r="A216" s="7" t="s">
-        <v>657</v>
-      </c>
-      <c r="C216" s="9" t="s">
-        <v>0</v>
-      </c>
       <c r="D216" s="8" t="s">
-        <v>658</v>
+        <v>677</v>
       </c>
     </row>
     <row r="217" spans="1:4">
       <c r="A217" s="7" t="s">
-        <v>668</v>
+        <v>681</v>
       </c>
       <c r="C217" s="9" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" ht="42.75">
-      <c r="A218" s="7" t="s">
-        <v>677</v>
-      </c>
-      <c r="C218" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="D218" s="8" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4">
-      <c r="A219" s="7" t="s">
+      <c r="D217" s="8" t="s">
         <v>682</v>
-      </c>
-      <c r="C219" s="9" t="s">
-        <v>613</v>
-      </c>
-      <c r="D219" s="8" t="s">
-        <v>683</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="34" priority="1" operator="containsText" text="Triaged">
+    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="Git">
+      <formula>NOT(ISERROR(SEARCH("Git",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="Triaged">
       <formula>NOT(ISERROR(SEARCH("Triaged",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="2" operator="containsText" text="Cancelled">
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="Cancelled">
       <formula>NOT(ISERROR(SEARCH("Cancelled",B1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7493,7 +7519,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -7507,12 +7533,12 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="9" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="9" t="s">
         <v>80</v>
       </c>
     </row>
@@ -7526,7 +7552,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7605,8 +7631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F160C7F-FB27-4F84-8171-6D9C64590D99}">
   <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -8460,7 +8486,7 @@
         <v>672</v>
       </c>
       <c r="C77" s="60" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -8471,7 +8497,7 @@
         <v>23</v>
       </c>
       <c r="C78" s="60" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -8508,8 +8534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06728CA9-C11D-4FE8-8912-18D6A33E8379}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9143,8 +9169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F77D648-B449-4B03-97EB-4834E79DA6CD}">
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -9749,7 +9775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF11BE1A-892C-449D-A753-1B446ED96C7C}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -9911,7 +9937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D1CD3F-B09A-47BC-BCAB-315B61D092F4}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -10490,7 +10516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4DB4886-0351-4FBB-AD2E-ACDCB11388DD}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -10748,7 +10774,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>